<commit_message>
Add enriched review report for 2025-04-22T06:54:41Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,593 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Product Title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Seller</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Review Count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>NOTHS URL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Feefo URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1029103</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Personalised Running Shoe Tag</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-running-shoe-tag</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029103&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1065021</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1067493</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Natural Flowers Spring Door Wreath</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1114901</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Semi Precious Birthstone Sterling Silver Bracelet</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/semi-precious-birthstone-sterling-silver-bracelet</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1114901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1152259</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Personalised Stainless Steel Pizza Cutter</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1154598</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Delicate Tree Print Scarf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1229576</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kids Personalised Dinosaur Varsity Jacket</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lovetreedesign/product/kids-personalised-dinosaur-varsity-jacket</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1268751</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tiffany Blue Luxury Scented Birthday Card</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1272876</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sterling Silver Light Curb Chain Necklace</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-curb-chain-necklace</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1278588</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bunny In A Box</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1321115</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Personalised Craft Beer Christmas Hamper</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/qwertybeerbox/product/personalised-craft-beer-christmas-hamper</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1321115&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1359483</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Personalised Open Flat Washbag</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1401131</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Personalised Friends With Wine Pebble Picture</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>429696</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Men's Personalised Engraved Plaited Leather Bracelet</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/men-s-engraved-clasp-bracelet</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=429696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>469358</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Family Birthstone Link Bracelet</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>821096</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Personalised Mini Round Travel Jewellery Case</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mini-round-travel-jewellery-case</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Personalised Birth Flower Scarf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>886944</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Personalised Leather And Silver St Christopher Bracelet</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>950557</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Personalised Sleepover Weekend Bag</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>980169</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Vintage Standing Heart Garden Bird Feeder</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-standing-double-bird-house-with-stake</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=980169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add enriched review report for 2025-04-22T07:19:05Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -476,7 +476,11 @@
           <t>Personalised Running Shoe Tag</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ellie Ellie</t>
+        </is>
+      </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
@@ -528,7 +532,11 @@
           <t>Natural Flowers Spring Door Wreath</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dibor</t>
+        </is>
+      </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
@@ -554,7 +562,11 @@
           <t>Semi Precious Birthstone Sterling Silver Bracelet</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gaamaa</t>
+        </is>
+      </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
@@ -580,7 +592,11 @@
           <t>Personalised Stainless Steel Pizza Cutter</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Oakdene Designs</t>
+        </is>
+      </c>
       <c r="D6" t="n">
         <v>2</v>
       </c>
@@ -606,7 +622,11 @@
           <t>Delicate Tree Print Scarf</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>My Posh Shop</t>
+        </is>
+      </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
@@ -762,7 +782,11 @@
           <t>Personalised Open Flat Washbag</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>The Alphabet Gift Shop</t>
+        </is>
+      </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
@@ -814,7 +838,11 @@
           <t>Men's Personalised Engraved Plaited Leather Bracelet</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hurleyburley man</t>
+        </is>
+      </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
@@ -840,7 +868,11 @@
           <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Joy by Corrine Smith</t>
+        </is>
+      </c>
       <c r="D16" t="n">
         <v>3</v>
       </c>
@@ -866,7 +898,11 @@
           <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>The Rustic Dish®</t>
+        </is>
+      </c>
       <c r="D17" t="n">
         <v>2</v>
       </c>
@@ -892,7 +928,11 @@
           <t>Personalised Mini Round Travel Jewellery Case</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Lisa Angel</t>
+        </is>
+      </c>
       <c r="D18" t="n">
         <v>2</v>
       </c>
@@ -918,7 +958,11 @@
           <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>The Forest &amp; Co</t>
+        </is>
+      </c>
       <c r="D19" t="n">
         <v>2</v>
       </c>
@@ -944,7 +988,11 @@
           <t>Personalised Leather And Silver St Christopher Bracelet</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hurleyburley man</t>
+        </is>
+      </c>
       <c r="D20" t="n">
         <v>2</v>
       </c>
@@ -996,7 +1044,11 @@
           <t>Vintage Standing Heart Garden Bird Feeder</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Dibor</t>
+        </is>
+      </c>
       <c r="D22" t="n">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Add enriched review report for 2025-04-22T07:34:00Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Seller Slug</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Review Count</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>NOTHS URL</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Feefo URL</t>
         </is>
@@ -481,15 +486,20 @@
           <t>Ellie Ellie</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ellieellie</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-running-shoe-tag</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029103&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -507,15 +517,20 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>thechucklingcheesecompany</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -537,15 +552,20 @@
           <t>Dibor</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>dibor</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -567,15 +587,20 @@
           <t>Gaamaa</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gaamaa</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/gaamaa/product/semi-precious-birthstone-sterling-silver-bracelet</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1114901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -597,15 +622,20 @@
           <t>Oakdene Designs</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>oakdenedesigns</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -627,15 +657,20 @@
           <t>My Posh Shop</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>myposhshop</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -653,15 +688,20 @@
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>lovetreedesign</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/lovetreedesign/product/kids-personalised-dinosaur-varsity-jacket</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -679,15 +719,20 @@
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>madewithlovecardboutique</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -705,15 +750,20 @@
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>songsofinkandsteel</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-curb-chain-necklace</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -731,15 +781,20 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>thegourmetchocolatepizzaco</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -757,15 +812,20 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>qwertybeerbox</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/qwertybeerbox/product/personalised-craft-beer-christmas-hamper</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1321115&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -787,15 +847,20 @@
           <t>The Alphabet Gift Shop</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>thealphabetgiftshop</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -813,15 +878,20 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ladedaliving</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -843,15 +913,20 @@
           <t>Hurleyburley man</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>hurleyburleyman</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/hurleyburleyman/product/men-s-engraved-clasp-bracelet</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=429696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -873,15 +948,20 @@
           <t>Joy by Corrine Smith</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>joybycorrinesmith</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>3</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -903,15 +983,20 @@
           <t>The Rustic Dish®</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>therusticdish</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -933,15 +1018,20 @@
           <t>Lisa Angel</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mini-round-travel-jewellery-case</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -963,15 +1053,20 @@
           <t>The Forest &amp; Co</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>2</v>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>theforestandco</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -993,15 +1088,20 @@
           <t>Hurleyburley man</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>hurleyburleyman</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -1019,15 +1119,20 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>alphabetinteriors</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
@@ -1049,15 +1154,20 @@
           <t>Dibor</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>dibor</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/dibor/product/personalised-standing-double-bird-house-with-stake</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=980169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Add enriched review report for 2025-04-22T07:42:12Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -516,7 +516,11 @@
           <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>The Chuckling Cheese Company</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>thechucklingcheesecompany</t>
@@ -687,7 +691,11 @@
           <t>Kids Personalised Dinosaur Varsity Jacket</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Lovetree Design</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>lovetreedesign</t>
@@ -718,7 +726,11 @@
           <t>Tiffany Blue Luxury Scented Birthday Card</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Luxe Cards</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>madewithlovecardboutique</t>
@@ -749,7 +761,11 @@
           <t>Sterling Silver Light Curb Chain Necklace</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Songs of Ink and Steel</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>songsofinkandsteel</t>
@@ -780,7 +796,11 @@
           <t>Bunny In A Box</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The Gourmet Chocolate Pizza Co.</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>thegourmetchocolatepizzaco</t>
@@ -811,7 +831,11 @@
           <t>Personalised Craft Beer Christmas Hamper</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>QWERTY Beer Box</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>qwertybeerbox</t>
@@ -877,7 +901,11 @@
           <t>Personalised Friends With Wine Pebble Picture</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>La de da! Living</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>ladedaliving</t>
@@ -1118,7 +1146,11 @@
           <t>Personalised Sleepover Weekend Bag</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Solesmith</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>alphabetinteriors</t>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-04-24T09:52:10Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,22 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1029103</t>
+          <t>1026153</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Running Shoe Tag</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Ellie Ellie</t>
-        </is>
-      </c>
+          <t>Art Deco Emerald Baguette Earrings</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>silkpursesowsear</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -496,34 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-running-shoe-tag</t>
+          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/art-deco-emerald-baguette-earrings</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029103&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1026153&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1065021</t>
+          <t>1054703</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The Chuckling Cheese Company</t>
-        </is>
-      </c>
+          <t>Personalised Iron Heart Garden Flower Bird Dish</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>thechucklingcheesecompany</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -531,34 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-iron-heart-garden-flower-bird-dish</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1054703&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1065021</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Natural Flowers Spring Door Wreath</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dibor</t>
-        </is>
-      </c>
+          <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>thechucklingcheesecompany</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -566,12 +554,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -586,11 +574,7 @@
           <t>Semi Precious Birthstone Sterling Silver Bracelet</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Gaamaa</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>gaamaa</t>
@@ -613,22 +597,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1152259</t>
+          <t>1263737</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Stainless Steel Pizza Cutter</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Oakdene Designs</t>
-        </is>
-      </c>
+          <t>Personalised Mug 'Used To Work With Absolute Legends'</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>arrowgiftco</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -636,34 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-mug-used-to-work-with-absolute-legends</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1263737&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1154598</t>
+          <t>1268751</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Delicate Tree Print Scarf</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>My Posh Shop</t>
-        </is>
-      </c>
+          <t>Tiffany Blue Luxury Scented Birthday Card</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>madewithlovecardboutique</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -671,174 +647,154 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1229576</t>
+          <t>1278588</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kids Personalised Dinosaur Varsity Jacket</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Lovetree Design</t>
-        </is>
-      </c>
+          <t>Bunny In A Box</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>lovetreedesign</t>
+          <t>thegourmetchocolatepizzaco</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lovetreedesign/product/kids-personalised-dinosaur-varsity-jacket</t>
+          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1268751</t>
+          <t>1285611</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tiffany Blue Luxury Scented Birthday Card</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Luxe Cards</t>
-        </is>
-      </c>
+          <t>Personalised My First Easter Bunny Toy With Name</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>madewithlovecardboutique</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/personalised-my-first-easter-bunny-toy-with-name</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1272876</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sterling Silver Light Curb Chain Necklace</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Songs of Ink and Steel</t>
-        </is>
-      </c>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-curb-chain-necklace</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1278588</t>
+          <t>1401131</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bunny In A Box</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>The Gourmet Chocolate Pizza Co.</t>
-        </is>
-      </c>
+          <t>Personalised Friends With Wine Pebble Picture</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>thegourmetchocolatepizzaco</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1321115</t>
+          <t>1488236</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalised Craft Beer Christmas Hamper</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>QWERTY Beer Box</t>
-        </is>
-      </c>
+          <t>Personalized Jewelry Box</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>qwertybeerbox</t>
+          <t>lineamasks</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -846,34 +802,30 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/qwertybeerbox/product/personalised-craft-beer-christmas-hamper</t>
+          <t>https://www.notonthehighstreet.com/lineamasks/product/personalized-jewelry-box</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1321115&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1359483</t>
+          <t>1491712</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Personalised Open Flat Washbag</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>The Alphabet Gift Shop</t>
-        </is>
-      </c>
+          <t>Statement Maker Socks Box - Letterbox Gift, Three Pairs</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>thealphabetgiftshop</t>
+          <t>standoutsocks</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -881,34 +833,30 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
+          <t>https://www.notonthehighstreet.com/standoutsocks/product/statement-maker-socks-box-letterbox-gift-three-pairs</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1401131</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Friends With Wine Pebble Picture</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>La de da! Living</t>
-        </is>
-      </c>
+          <t>Personalised Metal Street Sign</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -916,82 +864,74 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>429696</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Men's Personalised Engraved Plaited Leather Bracelet</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Hurleyburley man</t>
-        </is>
-      </c>
+          <t>Family Birthstone Link Bracelet</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>hurleyburleyman</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/men-s-engraved-clasp-bracelet</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=429696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>481237</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Joy by Corrine Smith</t>
-        </is>
-      </c>
+          <t>Personalised Leather Triple Wrap Symbolic Bracelet</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-leathertriple-wrap-infinity-bracelet</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=481237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -1006,11 +946,7 @@
           <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>The Rustic Dish®</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
           <t>therusticdish</t>
@@ -1033,22 +969,18 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>821096</t>
+          <t>771041</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Mini Round Travel Jewellery Case</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Lisa Angel</t>
-        </is>
-      </c>
+          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1056,34 +988,30 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mini-round-travel-jewellery-case</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>The Forest &amp; Co</t>
-        </is>
-      </c>
+          <t>Dandelion Foil Birthday Gift Scarf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1091,34 +1019,30 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>886944</t>
+          <t>950557</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Personalised Leather And Silver St Christopher Bracelet</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Hurleyburley man</t>
-        </is>
-      </c>
+          <t>Personalised Sleepover Weekend Bag</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>hurleyburleyman</t>
+          <t>alphabetinteriors</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1126,34 +1050,30 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
+          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>950557</t>
+          <t>991741</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Sleepover Weekend Bag</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Solesmith</t>
-        </is>
-      </c>
+          <t>Personalised Swarovski Birthstone And Disc Necklace</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>alphabetinteriors</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1161,47 +1081,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-disc-necklace</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>980169</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Vintage Standing Heart Garden Bird Feeder</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Dibor</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>dibor</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-standing-double-bird-house-with-stake</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=980169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-04-28T03:31:53Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1026153</t>
+          <t>1019839</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Art Deco Emerald Baguette Earrings</t>
+          <t>Easter Chocolate Mosaic Gift With Personalised Message</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>silkpursesowsear</t>
+          <t>cocoapod</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/art-deco-emerald-baguette-earrings</t>
+          <t>https://www.notonthehighstreet.com/cocoapod/product/easter-chocolate-mosaic-gift-with-personalised-message</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1026153&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019839&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1054703</t>
+          <t>1067222</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Iron Heart Garden Flower Bird Dish</t>
+          <t>Personalised Special Year Ginger Whisky With Music</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>mixpixie</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-iron-heart-garden-flower-bird-dish</t>
+          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-ginger-whisky</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1054703&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067222&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1065021</t>
+          <t>1087692</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>You're Not Old, You're Vintage! Cheese And Beer Hamper</t>
+          <t>'Happy Birthday!' Rainbow Candles Card</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>thechucklingcheesecompany</t>
+          <t>gabriellesollyillustration</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thechucklingcheesecompany/product/you-re-not-old-you-re-vintage-cheese-beer-hamper</t>
+          <t>https://www.notonthehighstreet.com/gabriellesollyillustration/product/it-s-your-birthday-rainbow-candles-card</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1087692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1114901</t>
+          <t>1162095</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Semi Precious Birthstone Sterling Silver Bracelet</t>
+          <t>Personalised 1955 70th Birthday Threepence Keyring</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,12 +585,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/semi-precious-birthstone-sterling-silver-bracelet</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/personalised-1952-70th-birthday-threepence-keyring</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1114901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162095&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -628,49 +628,49 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1268751</t>
+          <t>1278588</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tiffany Blue Luxury Scented Birthday Card</t>
+          <t>Bunny In A Box</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>madewithlovecardboutique</t>
+          <t>thegourmetchocolatepizzaco</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madewithlovecardboutique/product/tiffany-blue-luxury-scented-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1278588</t>
+          <t>1285611</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bunny In A Box</t>
+          <t>Personalised My First Easter Bunny Toy With Name</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>thegourmetchocolatepizzaco</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,92 +678,92 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/personalised-my-first-easter-bunny-toy-with-name</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1285611</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised My First Easter Bunny Toy With Name</t>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/personalised-my-first-easter-bunny-toy-with-name</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1383730</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Personalised Relax And Unwind Spa Pamper Hamper</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>mixpixie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-relax-unwind-spa-pamper-hamper</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1383730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1401131</t>
+          <t>1435766</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Friends With Wine Pebble Picture</t>
+          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,30 +771,30 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1488236</t>
+          <t>1470941</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalized Jewelry Box</t>
+          <t>Porcelain Bird Earrings French Vintage Charm</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>lineamasks</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -802,30 +802,30 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lineamasks/product/personalized-jewelry-box</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1491712</t>
+          <t>1488236</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Statement Maker Socks Box - Letterbox Gift, Three Pairs</t>
+          <t>Personalized Jewelry Box</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>standoutsocks</t>
+          <t>lineamasks</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -833,30 +833,30 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/standoutsocks/product/statement-maker-socks-box-letterbox-gift-three-pairs</t>
+          <t>https://www.notonthehighstreet.com/lineamasks/product/personalized-jewelry-box</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>298443</t>
+          <t>1489841</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Metal Street Sign</t>
+          <t>Simnel Cake</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>theoriginalcakecompany</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -864,61 +864,61 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
+          <t>https://www.notonthehighstreet.com/theoriginalcakecompany/product/simnel-cake</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1491712</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>Statement Maker Socks Box - Letterbox Gift, Three Pairs</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>standoutsocks</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/standoutsocks/product/statement-maker-socks-box-letterbox-gift-three-pairs</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>481237</t>
+          <t>159976</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Personalised Leather Triple Wrap Symbolic Bracelet</t>
+          <t>Personalised Pet Pebble With A Pawprint</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>letterfestengraving</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -926,30 +926,30 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-leathertriple-wrap-infinity-bracelet</t>
+          <t>https://www.notonthehighstreet.com/letterfestengraving/product/personalised-pet-pebble-with-a-pawprint</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=481237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+          <t>Personalised Metal Street Sign</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -957,61 +957,61 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>771041</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>bankslyonbotanical</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>748820</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dandelion Foil Birthday Gift Scarf</t>
+          <t>Personalised Metallic Sound Wave Song Print</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>mixpixie</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1019,30 +1019,30 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-metallic-foil-sound-wave-song-print</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>950557</t>
+          <t>771041</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Personalised Sleepover Weekend Bag</t>
+          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>alphabetinteriors</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,30 +1050,30 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/personalised-sleepover-society-bag</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>991741</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Swarovski Birthstone And Disc Necklace</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>twentyseven</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1081,12 +1081,167 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-disc-necklace</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>808656</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Happy Easter Daffodil Forever Flowers Box</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>noordinarygiftcompany</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/forever-daffodils-keepsake</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=808656&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Personalised Birth Flower Scarf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>theforestandco</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>887531</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Personalised Couples Name Heart Cushion Wedding Gift</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>thatsnicethat</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-couples-name-cushion</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=887531&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>915034</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Day / First Anniversary Card</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>sascreative</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>932102</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Personalised Meaningful Message Leather Bookmark</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-meaningful-message-leather-bookmark</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=932102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-05-05T03:33:53Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1019839</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Easter Chocolate Mosaic Gift With Personalised Message</t>
+          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cocoapod</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cocoapod/product/easter-chocolate-mosaic-gift-with-personalised-message</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019839&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1067222</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Special Year Ginger Whisky With Music</t>
+          <t>Dog And Owner Personalised Walking Socks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>mixpixie</t>
+          <t>alphabetinteriors</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-ginger-whisky</t>
+          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067222&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1087692</t>
+          <t>1268629</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>'Happy Birthday!' Rainbow Candles Card</t>
+          <t>Humorous Slate Weather Reader - Novelty Home Decor - Hanging Decoration - Gift For Home</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>gabriellesollyillustration</t>
+          <t>cgbgiftware</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gabriellesollyillustration/product/it-s-your-birthday-rainbow-candles-card</t>
+          <t>https://www.notonthehighstreet.com/cgbgiftware/product/humorous-slate-weather-reader</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1087692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268629&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1162095</t>
+          <t>1305530</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised 1955 70th Birthday Threepence Keyring</t>
+          <t>F1 Formula One Gift Drinks Coaster Set Of Five</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>iconiccoasters</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/personalised-1952-70th-birthday-threepence-keyring</t>
+          <t>https://www.notonthehighstreet.com/iconiccoasters/product/f1-formula-one-gift-drinks-coaster-set</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162095&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305530&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1263737</t>
+          <t>1308378</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Mug 'Used To Work With Absolute Legends'</t>
+          <t>Women's White Cotton Nightdress Sleeveless Pink Lizzie</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>arrowgiftco</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-mug-used-to-work-with-absolute-legends</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-sleeveless-pink-lizzie</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1263737&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1308378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1278588</t>
+          <t>1317092</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bunny In A Box</t>
+          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>thegourmetchocolatepizzaco</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,43 +647,43 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/bunny-in-a-box</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1285611</t>
+          <t>1347156</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised My First Easter Bunny Toy With Name</t>
+          <t>70th Birthday 1955 Sixpence Coin Compact Mirror</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/personalised-my-first-easter-bunny-toy-with-name</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/70th-birthday-1953-sixpence-coin-compact-mirror</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -721,18 +721,18 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1383730</t>
+          <t>1364790</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Relax And Unwind Spa Pamper Hamper</t>
+          <t>Personalised Bookrest In Solid Oak</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>mixpixie</t>
+          <t>mijmoj</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,508 +740,335 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-relax-unwind-spa-pamper-hamper</t>
+          <t>https://www.notonthehighstreet.com/mijmoj/product/personalised-bookrest-in-solid-oak</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1383730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364790&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1435766</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
-        </is>
-      </c>
+          <t>1373657</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>silverrainsilver</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>2</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1373657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1470941</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Porcelain Bird Earrings French Vintage Charm</t>
-        </is>
-      </c>
+          <t>1381151</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>uniques</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>2</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
-        </is>
-      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1488236</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Personalized Jewelry Box</t>
-        </is>
-      </c>
+          <t>1385338</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>lineamasks</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>2</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lineamasks/product/personalized-jewelry-box</t>
-        </is>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1489841</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Simnel Cake</t>
-        </is>
-      </c>
+          <t>1420726</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>theoriginalcakecompany</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theoriginalcakecompany/product/simnel-cake</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1491712</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Statement Maker Socks Box - Letterbox Gift, Three Pairs</t>
-        </is>
-      </c>
+          <t>1431678</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>standoutsocks</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>2</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/standoutsocks/product/statement-maker-socks-box-letterbox-gift-three-pairs</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>159976</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Personalised Pet Pebble With A Pawprint</t>
-        </is>
-      </c>
+          <t>1476302</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>letterfestengraving</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>2</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/letterfestengraving/product/personalised-pet-pebble-with-a-pawprint</t>
-        </is>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476302&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>298443</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Personalised Metal Street Sign</t>
-        </is>
-      </c>
+          <t>1489678</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>oakdenedesigns</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>2</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>469358</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Family Birthstone Link Bracelet</t>
-        </is>
-      </c>
+          <t>1489841</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>joybycorrinesmith</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>3</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
-        </is>
-      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>748820</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Personalised Metallic Sound Wave Song Print</t>
-        </is>
-      </c>
+          <t>377170</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>mixpixie</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>2</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-metallic-foil-sound-wave-song-print</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=377170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>771041</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
-        </is>
-      </c>
+          <t>462337</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>bankslyonbotanical</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>2</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
-        </is>
-      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
-        </is>
-      </c>
+          <t>469358</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>gaamaa</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>808656</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Happy Easter Daffodil Forever Flowers Box</t>
-        </is>
-      </c>
+          <t>748820</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>noordinarygiftcompany</t>
-        </is>
-      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>2</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/forever-daffodils-keepsake</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=808656&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Personalised Birth Flower Scarf</t>
-        </is>
-      </c>
+          <t>837767</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>theforestandco</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>2</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
-        </is>
-      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837767&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>887531</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Personalised Couples Name Heart Cushion Wedding Gift</t>
-        </is>
-      </c>
+          <t>868202</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>thatsnicethat</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>2</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-couples-name-cushion</t>
-        </is>
-      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=887531&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>915034</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Day / First Anniversary Card</t>
-        </is>
-      </c>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>sascreative</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>2</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
-        </is>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>932102</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Personalised Meaningful Message Leather Bookmark</t>
-        </is>
-      </c>
+          <t>905169</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>lisaangeljewellery</t>
-        </is>
-      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>2</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-meaningful-message-leather-bookmark</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=932102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>928794</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=928794&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-05-12T03:34:44Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1159266</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+          <t>Mens Personalised Classic Silver Steel Spinner Ring</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1218428</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dog And Owner Personalised Walking Socks</t>
+          <t>Personalised 18th Birthday Card Wooden Number Gift</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>alphabetinteriors</t>
+          <t>craftheaven</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,61 +523,61 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
+          <t>https://www.notonthehighstreet.com/craftheaven/product/personalised-18th-birthday-card-wooden-number-gift</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218428&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1268629</t>
+          <t>1245496</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Humorous Slate Weather Reader - Novelty Home Decor - Hanging Decoration - Gift For Home</t>
+          <t>Solid Perfume Making Kit</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>cgbgiftware</t>
+          <t>ourhands</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cgbgiftware/product/humorous-slate-weather-reader</t>
+          <t>https://www.notonthehighstreet.com/ourhands/product/solid-perfume-making-kit</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1268629&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245496&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1305530</t>
+          <t>1308378</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F1 Formula One Gift Drinks Coaster Set Of Five</t>
+          <t>Women's White Cotton Nightdress Sleeveless Pink Lizzie</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>iconiccoasters</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/iconiccoasters/product/f1-formula-one-gift-drinks-coaster-set</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-sleeveless-pink-lizzie</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305530&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1308378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1308378</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Women's White Cotton Nightdress Sleeveless Pink Lizzie</t>
+          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,92 +616,92 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-sleeveless-pink-lizzie</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1308378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1317092</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1347156</t>
+          <t>1372940</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>70th Birthday 1955 Sixpence Coin Compact Mirror</t>
+          <t>2015 Personalised 10th Tin Wedding Anniversary Poster</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/70th-birthday-1953-sixpence-coin-compact-mirror</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-10th-tin-wedding-anniversary-poster</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372940&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1385338</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Mystery Box</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>lucysaysido</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,50 +709,38 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/lucysaysido/product/mystery-box</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1364790</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Personalised Bookrest In Solid Oak</t>
-        </is>
-      </c>
+          <t>1399796</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>mijmoj</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/mijmoj/product/personalised-bookrest-in-solid-oak</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364790&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1399796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1373657</t>
+          <t>1404697</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -764,14 +752,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1373657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404697&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1453979</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -783,14 +771,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1453979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1385338</t>
+          <t>159976</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -802,14 +790,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1420726</t>
+          <t>458484</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -821,52 +809,52 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=458484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1476302</t>
+          <t>530476</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476302&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=530476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>608022</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -878,33 +866,33 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=608022&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1489841</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>377170</t>
+          <t>816668</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -916,14 +904,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=377170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=816668&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -935,33 +923,33 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>878687</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=878687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>748820</t>
+          <t>879692</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -973,14 +961,14 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>837767</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -992,83 +980,7 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837767&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>868202</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>905169</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="n">
-        <v>4</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>928794</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=928794&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-05-19T03:39:12Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1159266</t>
+          <t>1006901</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mens Personalised Classic Silver Steel Spinner Ring</t>
+          <t>Abstract Flower Print Scarf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/valentines-abstract-flowers-scarf</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1006901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1218428</t>
+          <t>1049381</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised 18th Birthday Card Wooden Number Gift</t>
+          <t>Personalised Special Year Gin With Music</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>craftheaven</t>
+          <t>mixpixie</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,61 +523,61 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/craftheaven/product/personalised-18th-birthday-card-wooden-number-gift</t>
+          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-flavoured-gin-with-music</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218428&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1049381&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1245496</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Solid Perfume Making Kit</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ourhands</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ourhands/product/solid-perfume-making-kit</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245496&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1308378</t>
+          <t>1064249</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Women's White Cotton Nightdress Sleeveless Pink Lizzie</t>
+          <t>1965 60th Birthday Sixpence Cuff Bracelet</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-sleeveless-pink-lizzie</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/1961-60th-birthday-sixpence-cuff-chain-bracelet</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1308378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1064249&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1159266</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
+          <t>Mens Personalised Classic Silver Steel Spinner Ring</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1277120</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Oval Shape Etched Birth Flower Necklace In Gift Box</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,61 +647,61 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/oval-shape-etched-birth-flower-necklace-in-gift-box</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277120&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1372940</t>
+          <t>1313658</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2015 Personalised 10th Tin Wedding Anniversary Poster</t>
+          <t>Personalised Golf Clubs Towel Accessories For Trolley</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-10th-tin-wedding-anniversary-poster</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-golf-clubs-towel-accessories-for-trolley</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372940&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313658&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1385338</t>
+          <t>1329145</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mystery Box</t>
+          <t>Happy Birthday Self Care Pamper Hamper</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>lucysaysido</t>
+          <t>makingthingshappen</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,38 +709,50 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lucysaysido/product/mystery-box</t>
+          <t>https://www.notonthehighstreet.com/makingthingshappen/product/happy-birthday-self-care-pamper-hamper</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329145&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1399796</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>1372225</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Simple 18th Birthday Scratch Voucher</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>twiststationery</t>
+        </is>
+      </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/twiststationery/product/simple-18th-birthday-scratch-voucher</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1399796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372225&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1404697</t>
+          <t>1374306</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -752,33 +764,33 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404697&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1374306&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1453979</t>
+          <t>1385338</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1453979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>159976</t>
+          <t>311517</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -790,71 +802,71 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=311517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>458484</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=458484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>643101</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>530476</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=530476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>608022</t>
+          <t>819734</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -866,14 +878,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=608022&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=819734&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>915034</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -885,100 +897,24 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>816668</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=816668&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>2</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>878687</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=878687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>879692</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-05-26T01:23:27Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1006901</t>
+          <t>1008277</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Abstract Flower Print Scarf</t>
+          <t>Personalised 80th Birthday Book 'Memory Lane'</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>lucysworld</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,61 +492,61 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/valentines-abstract-flowers-scarf</t>
+          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-80th-birthday-book-memory-lane</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1006901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1008277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1049381</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Special Year Gin With Music</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>mixpixie</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-flavoured-gin-with-music</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1049381&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1130272</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Personalised Family Seaside Beach Pebble Picture</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-family-seaside-beach-pebble-picture</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1064249</t>
+          <t>1179458</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1965 60th Birthday Sixpence Cuff Bracelet</t>
+          <t>Long Wildflower Amazing Friend Trinket Dish</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/1961-60th-birthday-sixpence-cuff-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1064249&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1159266</t>
+          <t>1218093</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mens Personalised Classic Silver Steel Spinner Ring</t>
+          <t>Birth Month Flower Earring Studs</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,12 +616,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birth-month-flower-earring-studs</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218093&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -659,18 +659,18 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1313658</t>
+          <t>1323961</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Golf Clubs Towel Accessories For Trolley</t>
+          <t>Muslin Swaddle Blanket Hello World Newborn Baby Shower Gift</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>geople</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,81 +678,69 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-golf-clubs-towel-accessories-for-trolley</t>
+          <t>https://www.notonthehighstreet.com/geople/product/muslin-swaddle-blanket-sunshine-newborn-baby-gift</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313658&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1323961&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1329145</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Happy Birthday Self Care Pamper Hamper</t>
+          <t>Sheep Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>makingthingshappen</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/makingthingshappen/product/happy-birthday-self-care-pamper-hamper</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329145&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1372225</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Simple 18th Birthday Scratch Voucher</t>
-        </is>
-      </c>
+          <t>1348765</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>twiststationery</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/twiststationery/product/simple-18th-birthday-scratch-voucher</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372225&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1348765&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1374306</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -764,33 +752,33 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1374306&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1385338</t>
+          <t>1359483</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>311517</t>
+          <t>1385338</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -802,14 +790,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=311517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1400456</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -821,14 +809,14 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>643101</t>
+          <t>1462617</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -840,14 +828,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1462617&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>1476087</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -859,14 +847,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>819734</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -878,14 +866,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=819734&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>915034</t>
+          <t>412675</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -897,14 +885,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -916,7 +904,178 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>610619</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>631040</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>748820</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>786481</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>864619</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=864619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>905169</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-06-02T01:29:24Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,80 +473,80 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1008277</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised 80th Birthday Book 'Memory Lane'</t>
+          <t>Map Engagement Card</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lucysworld</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-80th-birthday-book-memory-lane</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1008277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1032126</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Cats On Rollerskates Gift Wrap Set Of Two Sheets</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>joclarkdesign</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/joclarkdesign/product/cats-on-rollerskates-gift-wrap-set-of-two-sheets</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1032126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1130272</t>
+          <t>1039459</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Personalised Family Seaside Beach Pebble Picture</t>
+          <t>Personalised Wedding Day Celebration Card</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,61 +554,61 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-family-seaside-beach-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-celebration-card</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039459&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1179458</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Long Wildflower Amazing Friend Trinket Dish</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1218093</t>
+          <t>1074200</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Birth Month Flower Earring Studs</t>
+          <t>Herringbone Handloomed Soft Throw, Personalised Gift</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>livingroots</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birth-month-flower-earring-studs</t>
+          <t>https://www.notonthehighstreet.com/livingroots/product/herringbone-handwoven-cotton-throw</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218093&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1074200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1277120</t>
+          <t>1077247</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Oval Shape Etched Birth Flower Necklace In Gift Box</t>
+          <t>Personalised Wooden Sofa Tray</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>hotdot</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/oval-shape-etched-birth-flower-necklace-in-gift-box</t>
+          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-wooden-sofa-tray</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277120&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1077247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1323961</t>
+          <t>1088991</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Muslin Swaddle Blanket Hello World Newborn Baby Shower Gift</t>
+          <t>70th Birthday Personalised Plant Pot</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>geople</t>
+          <t>letterfest</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,69 +678,81 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/geople/product/muslin-swaddle-blanket-sunshine-newborn-baby-gift</t>
+          <t>https://www.notonthehighstreet.com/letterfest/product/70th-birthday-personalised-plant-pot</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1323961&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088991&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1094201</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+          <t>Traditional British Ale Gift Hamper, 6x 500ml Bottles</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>qwertybeerbox</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+          <t>https://www.notonthehighstreet.com/qwertybeerbox/product/traditional-british-ale-gift-hamper-6x-500ml-bottles</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1094201&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1348765</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>1150628</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Personalised Road Sign</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>madeforyougifts</t>
+        </is>
+      </c>
       <c r="E10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1348765&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1161984</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -752,14 +764,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1161984&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1359483</t>
+          <t>1166481</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -771,14 +783,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1166481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1385338</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -790,14 +802,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1400456</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -809,14 +821,14 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1462617</t>
+          <t>1235804</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -828,33 +840,33 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1462617&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1235804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1476087</t>
+          <t>1246450</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>1260303</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -866,14 +878,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260303&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>1289073</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -885,33 +897,33 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1289073&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1303055</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1303055&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1326378</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -923,90 +935,90 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>631040</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>748820</t>
+          <t>1341083</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>1350786</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350786&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>864619</t>
+          <t>1354241</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1018,33 +1030,33 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=864619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354241&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>1367950</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1056,14 +1068,14 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367950&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>1375803</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1075,7 +1087,786 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1397661</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397661&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1411672</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411672&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1413268</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1430607</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430607&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1431678</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>1436809</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1437739</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1437739&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1465032</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>1465039</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465039&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1466037</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>1489678</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>1495769</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1495769&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>350209</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>355476</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>377170</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=377170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>416277</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=416277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>432303</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=432303&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>462337</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>469358</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="n">
+        <v>7</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>51222</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=51222&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>522124</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=522124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>539718</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=539718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>621809</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
+        <v>3</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>702561</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=702561&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>717184</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=717184&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
+        <v>3</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>771041</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>783412</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=783412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>786481</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>4</v>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>802144</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=802144&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>823762</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=823762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>826425</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=826425&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>868202</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>915034</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>915286</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>921235</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=921235&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>929871</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=929871&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>939953</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>984487</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>2</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-06-09T01:29:13Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,80 +473,80 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1049381</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Map Engagement Card</t>
+          <t>Personalised Special Year Gin With Music</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>mixpixie</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
+          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-flavoured-gin-with-music</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1049381&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1032126</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cats On Rollerskates Gift Wrap Set Of Two Sheets</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>joclarkdesign</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joclarkdesign/product/cats-on-rollerskates-gift-wrap-set-of-two-sheets</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1032126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1039459</t>
+          <t>1088994</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Personalised Wedding Day Celebration Card</t>
+          <t>80th Birthday Personalised Plant Pot</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>letterfest</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,61 +554,61 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-celebration-card</t>
+          <t>https://www.notonthehighstreet.com/letterfest/product/80th-birthday-personalised-plant-pot</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039459&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1183789</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Personalised Keyring For Mummy Or Daddy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>taylorcutco</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/taylorcutco/product/this-daddy-dad-belongs-to-kechain</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1183789&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1074200</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Herringbone Handloomed Soft Throw, Personalised Gift</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>livingroots</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/livingroots/product/herringbone-handwoven-cotton-throw</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1074200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1077247</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Wooden Sofa Tray</t>
+          <t>Christening Keepsake Gift Book Personalised For Baby</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hotdot</t>
+          <t>mymagicname</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-wooden-sofa-tray</t>
+          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1077247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1088991</t>
+          <t>1232895</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>70th Birthday Personalised Plant Pot</t>
+          <t>Mens Personalised Sterling Silver Baltic Amber Cross Necklace</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>letterfest</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,30 +678,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/70th-birthday-personalised-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-cross-pendant-necklace</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088991&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232895&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1094201</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Traditional British Ale Gift Hamper, 6x 500ml Bottles</t>
+          <t>Personalised Birth Year Football Club Print</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>qwertybeerbox</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,50 +709,38 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/qwertybeerbox/product/traditional-british-ale-gift-hamper-6x-500ml-bottles</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-birth-year-football-club-print</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1094201&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1150628</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Personalised Road Sign</t>
-        </is>
-      </c>
+          <t>1290730</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>madeforyougifts</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1161984</t>
+          <t>1313736</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -764,14 +752,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1161984&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1166481</t>
+          <t>1338344</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -783,14 +771,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1166481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1338344&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1364104</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -802,14 +790,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1378864</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -821,14 +809,14 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1235804</t>
+          <t>1379125</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -840,33 +828,33 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1235804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1379125&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1246450</t>
+          <t>1381151</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1260303</t>
+          <t>1389129</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -878,14 +866,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260303&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1289073</t>
+          <t>1402097</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -897,14 +885,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1289073&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402097&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1303055</t>
+          <t>1410750</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -916,14 +904,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1303055&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410750&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1326378</t>
+          <t>1412795</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -935,109 +923,109 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326378&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412795&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1413268</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1341083</t>
+          <t>1416298</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1427990</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1427990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1350786</t>
+          <t>1431678</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350786&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1354241</t>
+          <t>1436809</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354241&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1441793</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1049,14 +1037,14 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1441793&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1367950</t>
+          <t>1465037</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1068,14 +1056,14 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367950&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1375803</t>
+          <t>1465039</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1087,14 +1075,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465039&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1397661</t>
+          <t>1470930</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1106,14 +1094,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397661&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1411672</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1125,14 +1113,14 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411672&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1413268</t>
+          <t>1489692</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1144,14 +1132,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1430607</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1163,14 +1151,14 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430607&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>1491892</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1182,14 +1170,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491892&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1436809</t>
+          <t>1505096</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1201,14 +1189,14 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1437739</t>
+          <t>1505155</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1220,14 +1208,14 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1437739&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1465032</t>
+          <t>270975</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1239,14 +1227,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=270975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1465039</t>
+          <t>348268</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1258,14 +1246,14 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465039&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=348268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1466037</t>
+          <t>380275</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1277,14 +1265,14 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>405702</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1296,14 +1284,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=405702&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1495769</t>
+          <t>433820</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1315,52 +1303,52 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1495769&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>458484</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=458484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>355476</t>
+          <t>462337</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>377170</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1372,14 +1360,14 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=377170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>416277</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1391,33 +1379,33 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=416277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>432303</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=432303&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>631040</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1429,33 +1417,33 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>632100</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=632100&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>51222</t>
+          <t>684208</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1467,71 +1455,71 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=51222&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>522124</t>
+          <t>689351</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=522124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>539718</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=539718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>826992</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=826992&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>702561</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1543,71 +1531,71 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=702561&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>717184</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=717184&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>927611</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=927611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>771041</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>783412</t>
+          <t>984487</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1619,253 +1607,6 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=783412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="n">
-        <v>4</v>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>802144</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="n">
-        <v>2</v>
-      </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=802144&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>823762</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="n">
-        <v>2</v>
-      </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=823762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>826425</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="n">
-        <v>2</v>
-      </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=826425&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>868202</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="n">
-        <v>2</v>
-      </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="n">
-        <v>3</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>915034</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="n">
-        <v>2</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>915286</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="n">
-        <v>2</v>
-      </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>921235</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="n">
-        <v>2</v>
-      </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=921235&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>929871</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="n">
-        <v>2</v>
-      </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=929871&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="n">
-        <v>3</v>
-      </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>939953</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>984487</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr">
-        <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-06-16T01:29:27Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1049381</t>
+          <t>1037522</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Special Year Gin With Music</t>
+          <t>Graduation Map Card</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>mixpixie</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,61 +492,61 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mixpixie/product/personalised-special-year-flavoured-gin-with-music</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1049381&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1066650</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Men's Natural Jasper Stone Bracelets</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>collectionsbyhayley</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/collectionsbyhayley/product/men-s-natural-jasper-stone-bracelets</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066650&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1088994</t>
+          <t>1076391</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>80th Birthday Personalised Plant Pot</t>
+          <t>Adjustable Personalised Ring</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>letterfest</t>
+          <t>raspberryripplejewellery</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/80th-birthday-personalised-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1183789</t>
+          <t>1079916</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Keyring For Mummy Or Daddy</t>
+          <t>Personalised Debossed Faux Leather Travel Organiser</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>taylorcutco</t>
+          <t>duncanstewarttextiles</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/taylorcutco/product/this-daddy-dad-belongs-to-kechain</t>
+          <t>https://www.notonthehighstreet.com/duncanstewarttextiles/product/personalised-debossed-faux-leather-travel-organiser</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1183789&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1079916&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1088994</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>80th Birthday Personalised Plant Pot</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>letterfest</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/letterfest/product/80th-birthday-personalised-plant-pot</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1090474</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Christening Keepsake Gift Book Personalised For Baby</t>
+          <t>Collectable Personalised Country Flags</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>mymagicname</t>
+          <t>storyteller</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
+          <t>https://www.notonthehighstreet.com/storyteller/product/storyteller-flags</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1090474&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1232895</t>
+          <t>1129372</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mens Personalised Sterling Silver Baltic Amber Cross Necklace</t>
+          <t>Personalised Couples Bee Socks</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>sparksanddaughters</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,30 +678,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-cross-pendant-necklace</t>
+          <t>https://www.notonthehighstreet.com/sparksanddaughters/product/personalised-couples-bee-socks</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232895&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1129372&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Birth Year Football Club Print</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,19 +709,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-birth-year-football-club-print</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1154280</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -733,33 +733,33 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1313736</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1338344</t>
+          <t>1179458</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -771,14 +771,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1338344&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1364104</t>
+          <t>1182639</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -790,14 +790,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1378864</t>
+          <t>1184813</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -809,52 +809,52 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184813&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1379125</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1379125&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1205920</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205920&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1389129</t>
+          <t>1210513</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -866,14 +866,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1402097</t>
+          <t>1296084</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -885,14 +885,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402097&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1410750</t>
+          <t>1318464</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -904,14 +904,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410750&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1318464&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1412795</t>
+          <t>1320832</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -923,33 +923,33 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412795&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1413268</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1416298</t>
+          <t>1334260</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -961,14 +961,14 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1334260&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1427990</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -980,52 +980,52 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1427990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1436809</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1441793</t>
+          <t>1357482</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1037,14 +1037,14 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1441793&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357482&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1465037</t>
+          <t>1360293</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1056,33 +1056,33 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1360293&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1465039</t>
+          <t>1365721</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465039&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1470930</t>
+          <t>1378864</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1094,14 +1094,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1113,52 +1113,52 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1489692</t>
+          <t>1389021</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1393324</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1393324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1491892</t>
+          <t>1394198</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1170,14 +1170,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491892&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1505096</t>
+          <t>1395023</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1189,14 +1189,14 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395023&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1505155</t>
+          <t>1404947</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1208,14 +1208,14 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404947&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>270975</t>
+          <t>1416597</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1227,14 +1227,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=270975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416597&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>348268</t>
+          <t>1419090</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1246,33 +1246,33 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=348268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419090&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>380275</t>
+          <t>1421445</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421445&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>405702</t>
+          <t>1440197</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1284,14 +1284,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=405702&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1440197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>433820</t>
+          <t>1443424</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1303,14 +1303,14 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443424&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>458484</t>
+          <t>1443796</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1322,33 +1322,33 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=458484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>1479670</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1479670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1482237</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1360,71 +1360,71 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1490578</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1490578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>631040</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>632100</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1436,71 +1436,71 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=632100&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>684208</t>
+          <t>1509756</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509756&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>689351</t>
+          <t>462337</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>46761</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=46761&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>826992</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1512,14 +1512,14 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=826992&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1531,71 +1531,71 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>577930</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=577930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>927611</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=927611&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>616318</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=616318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>984487</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1607,7 +1607,311 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>663976</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>708509</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>3</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=708509&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>708521</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=708521&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>752970</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=752970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>772232</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>787804</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=787804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>823513</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=823513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>857942</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>8</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>878687</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=878687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>883946</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=883946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>910678</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=910678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>923769</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>2</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=923769&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>939869</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939869&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>986868</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=986868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>2</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-06-23T01:34:07Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,49 +473,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1037522</t>
+          <t>1029102</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Graduation Map Card</t>
+          <t>Personalised Hiking Walking Boot Boot Tag</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-hiking-walking-boot-boot-tag</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1066650</t>
+          <t>1033142</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Men's Natural Jasper Stone Bracelets</t>
+          <t>18ct Gold Plated Or Sterling Silver Heart Link Bracelet</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>collectionsbyhayley</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/collectionsbyhayley/product/men-s-natural-jasper-stone-bracelets</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-or-sterling-silver-heart-link-bracelet</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066650&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033142&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1076391</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adjustable Personalised Ring</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>raspberryripplejewellery</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1079916</t>
+          <t>1109881</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Debossed Faux Leather Travel Organiser</t>
+          <t>Personalised Wooden Snack Crate Father's Day Gift</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>duncanstewarttextiles</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/duncanstewarttextiles/product/personalised-debossed-faux-leather-travel-organiser</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-wooden-snack-crate-gift-for-dad</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1079916&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1109881&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1088994</t>
+          <t>1127852</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>80th Birthday Personalised Plant Pot</t>
+          <t>Wooden Train Personalised Framed Print</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>letterfest</t>
+          <t>noordinarygiftcompany</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/80th-birthday-personalised-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/wooden-train-personalised-framed-print</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1088994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1127852&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1090474</t>
+          <t>1149454</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Collectable Personalised Country Flags</t>
+          <t>Personalised Classic Sterling Silver Spinner Ring</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>storyteller</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/storyteller/product/storyteller-flags</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-sterling-silver-slim-spinner-ring</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1090474&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1149454&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1129372</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Couples Bee Socks</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>sparksanddaughters</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,30 +678,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sparksanddaughters/product/personalised-couples-bee-socks</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1129372&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1152259</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Stainless Steel Pizza Cutter</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,95 +709,107 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1154280</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>1162105</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1179458</t>
+          <t>1181236</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1181236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1182639</t>
+          <t>1183789</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1183789&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1184813</t>
+          <t>1185133</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -809,14 +821,14 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184813&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1185133&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1190682</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -828,33 +840,33 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190682&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1205920</t>
+          <t>1229237</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205920&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1210513</t>
+          <t>1233585</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -866,14 +878,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1233585&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1296084</t>
+          <t>1239471</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -885,14 +897,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1239471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1318464</t>
+          <t>1244126</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -904,14 +916,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1318464&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1320832</t>
+          <t>1263673</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -923,33 +935,33 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1263673&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1273930</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1273930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1334260</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -961,14 +973,14 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1334260&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1344943</t>
+          <t>1292964</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -980,52 +992,52 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1292964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1296018</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1299630</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1299630&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1357482</t>
+          <t>1300286</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1037,14 +1049,14 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357482&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1300286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1360293</t>
+          <t>1313953</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1056,33 +1068,33 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1360293&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1365721</t>
+          <t>1326272</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1378864</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1094,14 +1106,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1387361</t>
+          <t>1334530</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1113,52 +1125,52 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1334530&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1389021</t>
+          <t>1347117</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1393324</t>
+          <t>1360088</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1393324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1360088&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1394198</t>
+          <t>1367998</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1170,14 +1182,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1395023</t>
+          <t>1374931</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1189,52 +1201,52 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395023&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1374931&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1404947</t>
+          <t>1375251</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404947&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375251&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1416597</t>
+          <t>1375256</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416597&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375256&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1419090</t>
+          <t>1375264</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1246,33 +1258,33 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419090&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375264&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1421445</t>
+          <t>1381151</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421445&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1440197</t>
+          <t>1391962</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1284,14 +1296,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1440197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1391962&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1443424</t>
+          <t>1392684</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1303,14 +1315,14 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443424&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392684&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1443796</t>
+          <t>1394555</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1322,14 +1334,14 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1479670</t>
+          <t>1396441</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1341,14 +1353,14 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1479670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396441&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1482237</t>
+          <t>1422513</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1360,33 +1372,33 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>1423284</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1490578</t>
+          <t>1431678</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1398,14 +1410,14 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1490578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1436809</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1417,14 +1429,14 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>1443868</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1436,52 +1448,52 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1509756</t>
+          <t>1446494</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509756&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446494&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>1490578</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1490578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>46761</t>
+          <t>1491332</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1493,14 +1505,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=46761&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491332&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1492774</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1512,33 +1524,33 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1492774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1497868</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>577930</t>
+          <t>1499827</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1550,14 +1562,14 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=577930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1501044</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1569,52 +1581,52 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>616318</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=616318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1505309</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505309&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>663976</t>
+          <t>1505688</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1626,33 +1638,33 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505688&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>708509</t>
+          <t>162227</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=708509&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=162227&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>708521</t>
+          <t>255094</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1664,33 +1676,33 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=708521&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255094&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>752970</t>
+          <t>270975</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=752970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=270975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>772232</t>
+          <t>290733</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1702,14 +1714,14 @@
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=290733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>787804</t>
+          <t>300310</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1721,14 +1733,14 @@
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=787804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=300310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>823513</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1740,14 +1752,14 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=823513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>352545</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1759,33 +1771,33 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=352545&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>355476</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>878687</t>
+          <t>405702</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1797,14 +1809,14 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=878687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=405702&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>883946</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1816,14 +1828,14 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=883946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>910678</t>
+          <t>525334</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1835,14 +1847,14 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=910678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=525334&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>923769</t>
+          <t>533246</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -1854,14 +1866,14 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=923769&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>939869</t>
+          <t>534903</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1873,33 +1885,33 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939869&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=534903&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>986868</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=986868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>575840</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1911,6 +1923,500 @@
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=575840&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>577930</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>2</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=577930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>578815</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=578815&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>601537</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>2</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=601537&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>623616</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>2</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=623616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>643101</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>2</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>663976</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>5</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>684208</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>2</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>692849</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>5</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=692849&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>722492</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>2</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>722986</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>2</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722986&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>748820</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>4</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>786481</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>2</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>804990</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>827357</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=827357&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>860631</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860631&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>860698</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>3</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>870084</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>3</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=870084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>8</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>881907</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>2</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>882800</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>2</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>898576</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>943955</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=943955&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>966803</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>2</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=966803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>968713</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>991741</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-06-30T01:30:54Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,49 +473,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1029102</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Hiking Walking Boot Boot Tag</t>
+          <t>Map Engagement Card</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-hiking-walking-boot-boot-tag</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1033142</t>
+          <t>1033155</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18ct Gold Plated Or Sterling Silver Heart Link Bracelet</t>
+          <t>Personalised Age And Name Floral Birthday Card</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,92 +523,92 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-or-sterling-silver-heart-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-birthday-card</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033142&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Star Sign Constellation Earrings Studs</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1109881</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Wooden Snack Crate Father's Day Gift</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-wooden-snack-crate-gift-for-dad</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1109881&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1127852</t>
+          <t>1069900</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wooden Train Personalised Framed Print</t>
+          <t>Personalised Hand Drawn Wedding Venue Illustration</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>noordinarygiftcompany</t>
+          <t>placesandspacesartco</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,61 +616,61 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/wooden-train-personalised-framed-print</t>
+          <t>https://www.notonthehighstreet.com/placesandspacesartco/product/personalised-wedding-venue-illustration</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1127852&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1069900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1149454</t>
+          <t>114245</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Classic Sterling Silver Spinner Ring</t>
+          <t>Large Brim Fold Up Straw Hat</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>plumandivory</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-sterling-silver-slim-spinner-ring</t>
+          <t>https://www.notonthehighstreet.com/plumandivory/product/large-brim-fold-up-straw-hat</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1149454&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=114245&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1152259</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Stainless Steel Pizza Cutter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,61 +678,61 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1152259</t>
+          <t>1154280</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Stainless Steel Pizza Cutter</t>
+          <t>Personalised Oak Road Sign Style Plaque</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-oak-road-sign-style-plaque</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1158522</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+          <t>Personalised First Home Gift, Housewarming Map Print</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>hooddesignsco</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,19 +740,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-our-first-home-map-print</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1172375</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -764,52 +764,52 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172375&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1181236</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1181236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1183789</t>
+          <t>1182639</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1183789&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1185133</t>
+          <t>1184575</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -821,33 +821,33 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1185133&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184575&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1190682</t>
+          <t>1211012</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190682&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1229237</t>
+          <t>1221252</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -859,7 +859,7 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1221252&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1239471</t>
+          <t>1260374</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -897,14 +897,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1239471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1244126</t>
+          <t>1278985</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -916,14 +916,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1263673</t>
+          <t>1296018</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -935,33 +935,33 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1263673&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1273930</t>
+          <t>1305014</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1273930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305014&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1319990</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -973,33 +973,33 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1319990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1292964</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1292964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1296018</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1011,33 +1011,33 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1299630</t>
+          <t>1345526</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1299630&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1300286</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1049,14 +1049,14 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1300286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1313953</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1068,14 +1068,14 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1326272</t>
+          <t>1367998</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1087,14 +1087,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1368460</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1106,14 +1106,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1334530</t>
+          <t>1400456</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1125,14 +1125,14 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1334530&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1347117</t>
+          <t>1401104</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1144,14 +1144,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1360088</t>
+          <t>1413323</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1163,14 +1163,14 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1360088&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413323&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1367998</t>
+          <t>1413444</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1182,14 +1182,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1374931</t>
+          <t>1416979</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1201,52 +1201,52 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1374931&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1375251</t>
+          <t>1435766</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375251&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1375256</t>
+          <t>1442063</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375256&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1442063&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1375264</t>
+          <t>1450889</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1258,14 +1258,14 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375264&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1456430</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1277,14 +1277,14 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456430&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1391962</t>
+          <t>1470930</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1296,14 +1296,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1391962&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1392684</t>
+          <t>1475693</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1315,14 +1315,14 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392684&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1394555</t>
+          <t>1477694</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1334,52 +1334,52 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1477694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1396441</t>
+          <t>1505617</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396441&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505617&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1422513</t>
+          <t>159976</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1423284</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1391,33 +1391,33 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>401706</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=401706&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1436809</t>
+          <t>462337</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1429,33 +1429,33 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1443868</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1446494</t>
+          <t>486000</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1467,33 +1467,33 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446494&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1490578</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1490578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1491332</t>
+          <t>64050</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1505,14 +1505,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491332&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=64050&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1492774</t>
+          <t>663976</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1524,33 +1524,33 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1492774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1497868</t>
+          <t>692849</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=692849&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1499827</t>
+          <t>769676</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1562,52 +1562,52 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=769676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1501044</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>797982</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=797982&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1505309</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1619,33 +1619,33 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505309&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1505688</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505688&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>162227</t>
+          <t>939953</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1657,767 +1657,7 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=162227&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>255094</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="n">
-        <v>2</v>
-      </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255094&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>270975</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="n">
-        <v>2</v>
-      </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=270975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>290733</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="n">
-        <v>2</v>
-      </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=290733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>300310</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="n">
-        <v>2</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=300310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>350209</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="n">
-        <v>2</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>352545</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="n">
-        <v>2</v>
-      </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=352545&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>355476</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="n">
-        <v>5</v>
-      </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>405702</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="n">
-        <v>2</v>
-      </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=405702&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>469358</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="n">
-        <v>2</v>
-      </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>525334</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=525334&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>533246</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>534903</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="n">
-        <v>2</v>
-      </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=534903&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>545355</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="n">
-        <v>3</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>575840</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="n">
-        <v>2</v>
-      </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=575840&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>577930</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="n">
-        <v>2</v>
-      </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=577930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>578815</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="n">
-        <v>2</v>
-      </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=578815&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>601537</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="n">
-        <v>2</v>
-      </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=601537&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>623616</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="n">
-        <v>2</v>
-      </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=623616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>643101</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="n">
-        <v>2</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>663976</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="n">
-        <v>5</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>684208</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="n">
-        <v>2</v>
-      </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>692849</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="n">
-        <v>5</v>
-      </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=692849&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>722492</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="n">
-        <v>2</v>
-      </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>722986</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="n">
-        <v>2</v>
-      </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722986&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>748820</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="n">
-        <v>4</v>
-      </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=748820&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="n">
-        <v>2</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>804990</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="n">
-        <v>2</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>827357</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="n">
-        <v>2</v>
-      </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=827357&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>860631</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="n">
-        <v>2</v>
-      </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860631&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>860698</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="n">
-        <v>3</v>
-      </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>870084</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="n">
-        <v>3</v>
-      </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=870084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
-        <v>8</v>
-      </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>881907</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>882800</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="n">
-        <v>2</v>
-      </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>898576</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>943955</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=943955&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>966803</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="n">
-        <v>2</v>
-      </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=966803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>968713</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="n">
-        <v>2</v>
-      </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>991741</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="n">
-        <v>2</v>
-      </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>999592</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-07-07T01:31:54Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,49 +473,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Map Engagement Card</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1033155</t>
+          <t>1066713</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Floral Birthday Card</t>
+          <t>Rose Gold Plated Cat Kitten Bracelet For Animal Lovers</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>thecolourfulaura</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,92 +523,92 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/thecolourfulaura/product/rose-gold-cat-kitten-bracelet-for-animal-lovers</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1067493</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Star Sign Constellation Earrings Studs</t>
+          <t>Natural Flowers Summer Door Wreath</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1076391</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Adjustable Personalised Ring</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>raspberryripplejewellery</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1069900</t>
+          <t>1116770</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Hand Drawn Wedding Venue Illustration</t>
+          <t>Personalised Christmas Wooden Robin Pair Sign</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>placesandspacesartco</t>
+          <t>pinkpineapple</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/placesandspacesartco/product/personalised-wedding-venue-illustration</t>
+          <t>https://www.notonthehighstreet.com/pinkpineapple/product/christmas-wooden-robin-pair-sign</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1069900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116770&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>114245</t>
+          <t>1121511</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Large Brim Fold Up Straw Hat</t>
+          <t>Personalised Large Forest Green Welly Boots Planter</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>plumandivory</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/plumandivory/product/large-brim-fold-up-straw-hat</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/large-forest-green-welly-boots-planter</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=114245&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1121511&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1152259</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Stainless Steel Pizza Cutter</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,61 +678,61 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1154280</t>
+          <t>1182639</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Oak Road Sign Style Plaque</t>
+          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>bubblebusinessuk</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-oak-road-sign-style-plaque</t>
+          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1158522</t>
+          <t>1184431</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised First Home Gift, Housewarming Map Print</t>
+          <t>1985 Personalised 40th Birthday Fact Poster</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>hooddesignsco</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,38 +740,38 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-our-first-home-map-print</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/1982-personalised-40th-birthday-fact-poster</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184431&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1172375</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172375&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1229228</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -783,71 +783,71 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1182639</t>
+          <t>1240116</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1240116&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1184575</t>
+          <t>1245496</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184575&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245496&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1211012</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1221252</t>
+          <t>1264565</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -859,14 +859,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1221252&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264565&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1233585</t>
+          <t>1276721</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -878,14 +878,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1233585&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1260374</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -897,71 +897,71 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1278985</t>
+          <t>1310862</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310862&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1296018</t>
+          <t>1313736</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1305014</t>
+          <t>1330774</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305014&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1319990</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -973,33 +973,33 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1319990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1345526</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1344943</t>
+          <t>1348765</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1011,14 +1011,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1348765&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1345526</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1030,52 +1030,52 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1354859</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1367998</t>
+          <t>1359921</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1087,14 +1087,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359921&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1368460</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1106,71 +1106,71 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1400456</t>
+          <t>1367998</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1401104</t>
+          <t>1418827</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1413323</t>
+          <t>1430284</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413323&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1413444</t>
+          <t>1434628</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1182,14 +1182,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1416979</t>
+          <t>1463304</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1201,14 +1201,14 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463304&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1435766</t>
+          <t>1488228</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1220,14 +1220,14 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1442063</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1239,52 +1239,52 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1442063&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1450889</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1456430</t>
+          <t>1498299</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456430&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498299&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1470930</t>
+          <t>1499827</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1296,71 +1296,71 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1475693</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1477694</t>
+          <t>1508229</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1477694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1505617</t>
+          <t>1511275</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1505617&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1511275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>159976</t>
+          <t>348289</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1372,14 +1372,14 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=159976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=348289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>373171</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1391,14 +1391,14 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=373171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>401706</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1410,14 +1410,14 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=401706&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>482198</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1429,33 +1429,33 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>486000</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>486000</t>
+          <t>505412</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1467,33 +1467,33 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=505412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>512405</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>64050</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1505,14 +1505,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=64050&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>663976</t>
+          <t>585833</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1524,33 +1524,33 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=585833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>692849</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=692849&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>769676</t>
+          <t>631040</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1562,14 +1562,14 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=769676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>646298</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1581,14 +1581,14 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=646298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>797982</t>
+          <t>652954</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1600,52 +1600,52 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=797982&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=652954&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>663976</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>679680</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=679680&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>939953</t>
+          <t>722492</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1657,7 +1657,254 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>769805</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=769805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>772232</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>808975</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>3</v>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=808975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>821096</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>846759</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>3</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=846759&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>872066</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>879692</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>882796</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>905169</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>931408</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=931408&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>3</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>957544</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=957544&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>4</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-07-14T01:36:58Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,49 +473,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>10051</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>1st To 50th Wedding Anniversary Book</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>2littleboys</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/2littleboys/product/51_the_anniversary_book</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=10051&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1066713</t>
+          <t>1014560</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rose Gold Plated Cat Kitten Bracelet For Animal Lovers</t>
+          <t>Personalised Book Style Novel Notebook</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>thecolourfulaura</t>
+          <t>marthabrook</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thecolourfulaura/product/rose-gold-cat-kitten-bracelet-for-animal-lovers</t>
+          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-book-style-novel-notebook</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1014560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1037522</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Natural Flowers Summer Door Wreath</t>
+          <t>Graduation Map Card</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1076391</t>
+          <t>1038914</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adjustable Personalised Ring</t>
+          <t>Personalised Portable Picnic Table Wine Holder</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>raspberryripplejewellery</t>
+          <t>mijmoj</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
+          <t>https://www.notonthehighstreet.com/mijmoj/product/personalised-picnic-table</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1038914&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1116770</t>
+          <t>1047247</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Christmas Wooden Robin Pair Sign</t>
+          <t>Personalised Teacher Thank You Notebook Gift</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>pinkpineapple</t>
+          <t>oliviamorgan</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,181 +616,181 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pinkpineapple/product/christmas-wooden-robin-pair-sign</t>
+          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-teacher-thank-you-notebook-gift</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116770&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1121511</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Large Forest Green Welly Boots Planter</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/large-forest-green-welly-boots-planter</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1121511&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1067493</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Natural Flowers Summer Door Wreath</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1182639</t>
+          <t>1116770</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
+          <t>Personalised Christmas Wooden Robin Pair Sign</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>bubblebusinessuk</t>
+          <t>pinkpineapple</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
+          <t>https://www.notonthehighstreet.com/pinkpineapple/product/christmas-wooden-robin-pair-sign</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116770&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1184431</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1985 Personalised 40th Birthday Fact Poster</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/1982-personalised-40th-birthday-fact-poster</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1184431&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1229228</t>
+          <t>1179458</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1240116</t>
+          <t>1181236</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -802,52 +802,52 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1240116&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1181236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1245496</t>
+          <t>1182639</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245496&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1187498</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187498&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1264565</t>
+          <t>1187757</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -859,14 +859,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264565&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187757&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1276721</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -878,14 +878,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -897,52 +897,52 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1310862</t>
+          <t>1234030</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310862&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1313736</t>
+          <t>1244132</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244132&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1330774</t>
+          <t>1246966</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -954,14 +954,14 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1264251</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -973,14 +973,14 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264251&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1345526</t>
+          <t>1267594</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -992,14 +992,14 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1267594&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1348765</t>
+          <t>1272876</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1011,14 +1011,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1348765&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1278602</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1030,52 +1030,52 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1354859</t>
+          <t>1290822</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1359921</t>
+          <t>1299630</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1087,109 +1087,109 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359921&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1299630&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1307555</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1367998</t>
+          <t>1310158</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310158&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1418827</t>
+          <t>1312519</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1312519&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1430284</t>
+          <t>1317092</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1434628</t>
+          <t>1320832</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1463304</t>
+          <t>1328533</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1201,14 +1201,14 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463304&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1328533&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1488228</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1220,14 +1220,14 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>1345526</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1239,14 +1239,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1258,128 +1258,128 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1498299</t>
+          <t>1350143</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498299&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1499827</t>
+          <t>1350786</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350786&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1508229</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1511275</t>
+          <t>1354859</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1511275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>348289</t>
+          <t>1365394</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=348289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>373171</t>
+          <t>1368285</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1391,33 +1391,33 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=373171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>136955</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=136955&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>482198</t>
+          <t>1385645</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1429,14 +1429,14 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385645&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>486000</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1448,14 +1448,14 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>505412</t>
+          <t>1389021</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1467,14 +1467,14 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=505412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>512405</t>
+          <t>1402198</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1486,14 +1486,14 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1406416</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1505,14 +1505,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1406416&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>585833</t>
+          <t>1406717</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1524,52 +1524,52 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=585833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1406717&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1412709</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412709&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>631040</t>
+          <t>1417133</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1417133&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>646298</t>
+          <t>1422330</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1581,14 +1581,14 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=646298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422330&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>652954</t>
+          <t>1438876</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1600,14 +1600,14 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=652954&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>663976</t>
+          <t>1448523</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1619,14 +1619,14 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=663976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1448523&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>679680</t>
+          <t>1462298</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1638,14 +1638,14 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=679680&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1462298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>722492</t>
+          <t>1466040</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1657,33 +1657,33 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>769805</t>
+          <t>1470930</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=769805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>772232</t>
+          <t>1478443</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1695,52 +1695,52 @@
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>808975</t>
+          <t>1478663</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=808975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>821096</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>846759</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1752,14 +1752,14 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=846759&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>872066</t>
+          <t>1496544</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1771,14 +1771,14 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496544&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>879692</t>
+          <t>1497862</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1790,33 +1790,33 @@
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497862&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>882796</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1828,14 +1828,14 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>931408</t>
+          <t>307261</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1847,62 +1847,822 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=931408&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=307261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>380275</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>957544</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=957544&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>446429</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>469358</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>6</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>486442</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>2</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486442&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>492043</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=492043&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>493192</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>2</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=493192&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>510573</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>2</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=510573&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>533246</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>545355</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>7</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>581579</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>2</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=581579&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>621809</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>5</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>684433</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>2</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684433&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>689351</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>2</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>706455</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>2</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=706455&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>722492</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>3</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>761621</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=761621&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>771041</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>785952</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>2</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=785952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>804990</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>866983</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>868202</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>2</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>872066</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>2</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>875307</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=875307&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>5</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>879581</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>2</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879581&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>880642</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>881907</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>905169</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>909642</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="n">
+        <v>2</v>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=909642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="n">
+        <v>2</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>940836</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=940836&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>941353</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="n">
+        <v>2</v>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=941353&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>944163</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="n">
+        <v>2</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944163&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>950557</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="n">
+        <v>2</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>950712</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="n">
+        <v>2</v>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>950732</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="n">
+        <v>3</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>976980</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="n">
+        <v>2</v>
+      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>982044</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>2</v>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>990259</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>2</v>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=990259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>991741</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="n">
+        <v>2</v>
+      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="n">
+        <v>3</v>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-07-21T01:57:22Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10051</t>
+          <t>1029102</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1st To 50th Wedding Anniversary Book</t>
+          <t>Personalised Hiking Walking Boot Boot Tag</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2littleboys</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/2littleboys/product/51_the_anniversary_book</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-hiking-walking-boot-boot-tag</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=10051&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1014560</t>
+          <t>1030998</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Book Style Novel Notebook</t>
+          <t>Name Among Stars Personalised Luxury Notebook Journal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>marthabrook</t>
+          <t>betsybenn</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-book-style-novel-notebook</t>
+          <t>https://www.notonthehighstreet.com/betsybenn/product/name-among-stars-personalised-luxury-notebook-journal</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1014560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1030998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1037522</t>
+          <t>1031001</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Graduation Map Card</t>
+          <t>Adventure Personalised Travel Journal Notebook</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>betsybenn</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
+          <t>https://www.notonthehighstreet.com/betsybenn/product/adventure-personalised-travel-journal-notebook</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1031001&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1038914</t>
+          <t>1033155</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Portable Picnic Table Wine Holder</t>
+          <t>Personalised Age And Name Floral Birthday Card</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>mijmoj</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mijmoj/product/personalised-picnic-table</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-birthday-card</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1038914&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1047247</t>
+          <t>1035850</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Teacher Thank You Notebook Gift</t>
+          <t>Personalised Graduation Hinged Wooden Bottle Gift Box</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>oliviamorgan</t>
+          <t>dreamstoreality</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,2053 +616,3625 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-teacher-thank-you-notebook-gift</t>
+          <t>https://www.notonthehighstreet.com/dreamstoreality/product/personalised-graduation-hinged-wooden-bottle-gift-box</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035850&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1036840</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>13th Lace Wedding Anniversary Personalised Card</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>thehummingbirdcardcompany</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/thehummingbirdcardcompany/product/13th-lace-wedding-anniversary-card</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1036840&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1037522</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Natural Flowers Summer Door Wreath</t>
+          <t>Graduation Map Card</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1116770</t>
+          <t>1047473</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Christmas Wooden Robin Pair Sign</t>
+          <t>Personalised Brilliant Teacher Notebook Journal</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>pinkpineapple</t>
+          <t>betsybenn</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pinkpineapple/product/christmas-wooden-robin-pair-sign</t>
+          <t>https://www.notonthehighstreet.com/betsybenn/product/personalised-brilliant-teacher-notebook-journal</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116770&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047473&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1047587</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Van Gogh Print Silk Scarf</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/van-gogh-almond-blossom-silk-scarf</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047587&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1162105</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+          <t>1051200</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Personalised Birth Flower Locket Necklace</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
       <c r="E11" t="n">
-        <v>3</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-birth-flower-locket-necklace</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1051200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1179458</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>1053070</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Birth Flower Scarf And Card In A Gift Box</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>theforestandco</t>
+        </is>
+      </c>
       <c r="E12" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/birth-flower-scarf-and-card-in-a-gift-box</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053070&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1181236</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>1060664</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Personalised Garden Sign</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>daisymaison</t>
+        </is>
+      </c>
       <c r="E13" t="n">
         <v>2</v>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-garden-sign</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1181236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1060664&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1182639</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>1061842</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Personalised Family Street Sign</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>daisymaison</t>
+        </is>
+      </c>
       <c r="E14" t="n">
         <v>2</v>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-family-street-sign</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1187498</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>1062346</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187498&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1187757</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
+          <t>1065178</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Planner And Organiser</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>marthabrook</t>
+        </is>
+      </c>
       <c r="E16" t="n">
         <v>2</v>
       </c>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-wedding-planner-and-organiser</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187757&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1198294</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
+          <t>1067493</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Natural Flowers Summer Door Wreath</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>dibor</t>
+        </is>
+      </c>
       <c r="E17" t="n">
         <v>2</v>
       </c>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1209526</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+          <t>1091599</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Personalised Graduation Silver Plated Certificate Holder</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>bellapersonalisedgiftsltd</t>
+        </is>
+      </c>
       <c r="E18" t="n">
         <v>2</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/bellapersonalisedgiftsltd/product/personalised-silver-plated-certificate-holder-gift</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1091599&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1234030</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
+          <t>1095606</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Edinburgh Graduation Skyline Personalised Card</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>mooandsnip</t>
+        </is>
+      </c>
       <c r="E19" t="n">
         <v>2</v>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mooandsnip/product/edinburgh-graduation-skyline-personalised-card</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1095606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1244132</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
+          <t>109904</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Tabletop Garden Oil Torch Steel Ltzaf152</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>thelondongardentradingco</t>
+        </is>
+      </c>
       <c r="E20" t="n">
         <v>2</v>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thelondongardentradingco/product/glass-and-steel-oil-burning-torch-red</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244132&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=109904&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1246966</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
+          <t>1150628</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Personalised Road Sign</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>madeforyougifts</t>
+        </is>
+      </c>
       <c r="E21" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1264251</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
+          <t>1154280</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Personalised Oak Road Sign Style Plaque</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>madeforyougifts</t>
+        </is>
+      </c>
       <c r="E22" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-oak-road-sign-style-plaque</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264251&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1267594</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
+          <t>1162105</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E23" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1267594&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1272876</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
+          <t>1179458</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Long Wildflower Amazing Friend Trinket Dish</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
       <c r="E24" t="n">
-        <v>2</v>
-      </c>
-      <c r="F24" t="inlineStr"/>
+        <v>6</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1278602</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
+          <t>1180998</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Personalised Women's Technology Travel Case Gift</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>thatsnicethat</t>
+        </is>
+      </c>
       <c r="E25" t="n">
-        <v>2</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1290730</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
+          <t>1182280</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Personalised Floral 30th Birthday Card</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>oliviamorgan</t>
+        </is>
+      </c>
       <c r="E26" t="n">
         <v>2</v>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-floral-30th-birthday-card</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1290822</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
+          <t>1182639</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>bubblebusinessuk</t>
+        </is>
+      </c>
       <c r="E27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1299630</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
+          <t>1198294</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Personalised Age And Name Happy Birthday Card</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>sascreative</t>
+        </is>
+      </c>
       <c r="E28" t="n">
         <v>2</v>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1299630&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1307555</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
+          <t>1200812</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Indoor Plant Pot</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>letterfest</t>
+        </is>
+      </c>
       <c r="E29" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-wedding-indoor-plant-pot</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1200812&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1310158</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
+          <t>1211012</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Sterling Silver Bold Coil Drop Earrings</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>marthajackson</t>
+        </is>
+      </c>
       <c r="E30" t="n">
-        <v>2</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310158&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1312519</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
+          <t>1212257</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Personalised Birthday Card Day You Were Born Music</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>elevencorners</t>
+        </is>
+      </c>
       <c r="E31" t="n">
         <v>2</v>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/elevencorners/product/personalised-birthday-card-day-you-were-born-music</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1312519&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1212257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1317092</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr"/>
+          <t>1234030</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Personalised Sterling Silver Baltic Amber Bumble Bee Necklace</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>songsofinkandsteel</t>
+        </is>
+      </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
-      <c r="F32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
+        </is>
+      </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1320832</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
+          <t>1244126</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>60th Birthday Sterling Silver Bracelet</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>sophiejonesjewellery</t>
+        </is>
+      </c>
       <c r="E33" t="n">
-        <v>5</v>
-      </c>
-      <c r="F33" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/60th-birthday-sterling-silver-bracelet</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1328533</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr"/>
+          <t>1245502</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Sterling Silver And Gold Daisy April Birth Flower Earrings</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>songsofinkandsteel</t>
+        </is>
+      </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
-      <c r="F34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
+        </is>
+      </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1328533&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>133151</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr"/>
+          <t>1246450</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Weekly Positivity Floral Desktop Flip Chart</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
       <c r="E35" t="n">
         <v>2</v>
       </c>
-      <c r="F35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1345526</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr"/>
+          <t>1246966</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Mustard Ginkgo Print Scarf</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>myposhshop</t>
+        </is>
+      </c>
       <c r="E36" t="n">
-        <v>3</v>
-      </c>
-      <c r="F36" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/ginkgo-print-scarf</t>
+        </is>
+      </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1345877</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr"/>
+          <t>1269933</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Sunshine Jewellery Stand With Terrazzo Base</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
       <c r="E37" t="n">
-        <v>3</v>
-      </c>
-      <c r="F37" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/sunshine-jewellery-stand-with-terrazzo-base</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1269933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1350143</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr"/>
+          <t>1276721</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Metallic Personalised Record Player Song Lyrics Print</t>
+        </is>
+      </c>
       <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>spincollective</t>
+        </is>
+      </c>
       <c r="E38" t="n">
         <v>2</v>
       </c>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/spincollective/product/metallic-personalised-record-player-song-lyrics-print</t>
+        </is>
+      </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1350786</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr"/>
+          <t>1290822</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Anniversary Gift Candle Holder Set</t>
+        </is>
+      </c>
       <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>mirrorin</t>
+        </is>
+      </c>
       <c r="E39" t="n">
-        <v>5</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-anniversary-candle-holder-set</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350786&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1351207</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr"/>
+          <t>1301141</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Set Of Two Wire Robin Decorative Ornament</t>
+        </is>
+      </c>
       <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>paperhigh</t>
+        </is>
+      </c>
       <c r="E40" t="n">
         <v>2</v>
       </c>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/paperhigh/product/set-of-two-wire-robin-decorative-ornament</t>
+        </is>
+      </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1301141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1353406</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
+          <t>1302008</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Your Own Words Block Text Personalised Notebook</t>
+        </is>
+      </c>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>betsybenn</t>
+        </is>
+      </c>
       <c r="E41" t="n">
-        <v>5</v>
-      </c>
-      <c r="F41" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/betsybenn/product/your-own-words-block-text-personalised-notebook</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1302008&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1354859</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
+          <t>1304639</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Personalised Teacher Pebble Picture</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>ladedaliving</t>
+        </is>
+      </c>
       <c r="E42" t="n">
-        <v>3</v>
-      </c>
-      <c r="F42" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-teacher-pebble-picture</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1304639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1365394</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr"/>
+          <t>1307555</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Personalised Graduation Pebble Picture</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>ladedaliving</t>
+        </is>
+      </c>
       <c r="E43" t="n">
-        <v>4</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-graduation-pebble-picture</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1368285</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr"/>
+          <t>1314094</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Sterling Silver Sewing Button Stud Earrings</t>
+        </is>
+      </c>
       <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>songsofinkandsteel</t>
+        </is>
+      </c>
       <c r="E44" t="n">
         <v>2</v>
       </c>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/round-sewing-button-earrings-in-sterling-silver</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1314094&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>136955</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr"/>
+          <t>1317092</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>charlieboots</t>
+        </is>
+      </c>
       <c r="E45" t="n">
         <v>2</v>
       </c>
-      <c r="F45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=136955&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1385645</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
+          <t>1326272</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Orange Sunflower Motif Scarf</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E46" t="n">
         <v>2</v>
       </c>
-      <c r="F46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/orange-sunflower-motif-scarf-in-a-box</t>
+        </is>
+      </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385645&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1387361</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr"/>
+          <t>1330966</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Handmade Personalised Leather Curved Corner Bookmark</t>
+        </is>
+      </c>
       <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>parkerandco</t>
+        </is>
+      </c>
       <c r="E47" t="n">
         <v>2</v>
       </c>
-      <c r="F47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/parkerandco/product/handmade-personalised-leather-curved-corner-bookmark</t>
+        </is>
+      </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1389021</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr"/>
+          <t>133151</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>jomanda</t>
+        </is>
+      </c>
       <c r="E48" t="n">
-        <v>2</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1402198</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
+          <t>1345526</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Friendship Knot Bangle With Birthstone Hearts</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>joybycorrinesmith</t>
+        </is>
+      </c>
       <c r="E49" t="n">
-        <v>2</v>
-      </c>
-      <c r="F49" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle-with-birthstone-hearts</t>
+        </is>
+      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1406416</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr"/>
+          <t>1345877</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>hurleyburley</t>
+        </is>
+      </c>
       <c r="E50" t="n">
-        <v>2</v>
-      </c>
-      <c r="F50" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
+        </is>
+      </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1406416&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1406717</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr"/>
+          <t>1346621</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Festive Christmas Magnetic Brooch</t>
+        </is>
+      </c>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>myposhshop</t>
+        </is>
+      </c>
       <c r="E51" t="n">
         <v>2</v>
       </c>
-      <c r="F51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/festive-christmas-magnetic-brooch</t>
+        </is>
+      </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1406717&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1346621&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1412709</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr"/>
+          <t>1354859</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Ceramic Little Book Of Flowers Vase</t>
+        </is>
+      </c>
       <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
       <c r="E52" t="n">
         <v>3</v>
       </c>
-      <c r="F52" t="inlineStr"/>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/ceramic-little-book-of-flowers-vase</t>
+        </is>
+      </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412709&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1417133</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr"/>
+          <t>1365394</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>uniques</t>
+        </is>
+      </c>
       <c r="E53" t="n">
-        <v>3</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
+        </is>
+      </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1417133&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1422330</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr"/>
+          <t>1366698</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Christening Gift Personalised Book Words Of Wisdom</t>
+        </is>
+      </c>
       <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>mymagicname</t>
+        </is>
+      </c>
       <c r="E54" t="n">
         <v>2</v>
       </c>
-      <c r="F54" t="inlineStr"/>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-gift-personalised-book-words-of-wisdom</t>
+        </is>
+      </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422330&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1366698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1438876</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
+          <t>1368436</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Special Granddaughter Personalised Birthday Card</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>paperscene</t>
+        </is>
+      </c>
       <c r="E55" t="n">
         <v>2</v>
       </c>
-      <c r="F55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/paperscene/product/special-granddaughter-personalised-birthday-card</t>
+        </is>
+      </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368436&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1448523</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr"/>
+          <t>1372919</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1965 Personalised 60th Diamond Wedding Anniversary Poster</t>
+        </is>
+      </c>
       <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>thewordshack</t>
+        </is>
+      </c>
       <c r="E56" t="n">
-        <v>2</v>
-      </c>
-      <c r="F56" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-60th-diamond-wedding-anniversary-poster</t>
+        </is>
+      </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1448523&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372919&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1462298</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
+          <t>1376487</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Tiny Turtle Strength Bracelet</t>
+        </is>
+      </c>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>letterboxlove</t>
+        </is>
+      </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/tiny-turtle-strength-bracelet</t>
+        </is>
+      </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1462298&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1466040</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
+          <t>1381151</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
+        </is>
+      </c>
       <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>theforestandco</t>
+        </is>
+      </c>
       <c r="E58" t="n">
-        <v>2</v>
-      </c>
-      <c r="F58" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
+        </is>
+      </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1470930</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
+          <t>1384152</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Personalised Elephant Money Box For Christening Baptism</t>
+        </is>
+      </c>
       <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>mirrorin</t>
+        </is>
+      </c>
       <c r="E59" t="n">
-        <v>4</v>
-      </c>
-      <c r="F59" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-elephant-money-box-for-christening-baptism</t>
+        </is>
+      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470930&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1384152&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1478443</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
+          <t>1389021</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1st Birthday Book Of Nursery Rhymes And Poems</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>mygivenname</t>
+        </is>
+      </c>
       <c r="E60" t="n">
         <v>2</v>
       </c>
-      <c r="F60" t="inlineStr"/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/1st-birthday-book-of-nursery-rhymes-and-poems</t>
+        </is>
+      </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1478663</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
+          <t>1394198</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Formula One F1 2025 Calendar Track Mug Gift For Him</t>
+        </is>
+      </c>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>iconiccoasters</t>
+        </is>
+      </c>
       <c r="E61" t="n">
         <v>2</v>
       </c>
-      <c r="F61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/iconiccoasters/product/formula-one-f1-2024-calendar-track-mug-gift-for-him</t>
+        </is>
+      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1489678</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
+          <t>1401190</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Sterling Silver Little Daisy Flower Drop Hook Earrings</t>
+        </is>
+      </c>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>silverrainsilver</t>
+        </is>
+      </c>
       <c r="E62" t="n">
         <v>2</v>
       </c>
-      <c r="F62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/little-daisy-flower-drop-hook-earrings</t>
+        </is>
+      </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1491886</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr"/>
+          <t>1408415</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Personalised 60th Birthday Wine Bottle Gift Set</t>
+        </is>
+      </c>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>thealphabetgiftshop</t>
+        </is>
+      </c>
       <c r="E63" t="n">
-        <v>3</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-60th-birthday-wine-bottle-gift-set</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1408415&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1496544</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
+          <t>1409309</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>60th Birthday Bracelet, Kate, Sterling Silver</t>
+        </is>
+      </c>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>wishedfor</t>
+        </is>
+      </c>
       <c r="E64" t="n">
         <v>2</v>
       </c>
-      <c r="F64" t="inlineStr"/>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/wishedfor/product/60th-birthday-bracelet-kate-sterling-silver</t>
+        </is>
+      </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496544&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1409309&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1497862</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
+          <t>1410229</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Personalised 40th Ruby Anniversary Card For Husband/Wife</t>
+        </is>
+      </c>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>hopeandlove</t>
+        </is>
+      </c>
       <c r="E65" t="n">
         <v>2</v>
       </c>
-      <c r="F65" t="inlineStr"/>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hopeandlove/product/personalised-40th-ruby-anniversary-card-for-husband-wife</t>
+        </is>
+      </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497862&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1503694</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
+          <t>1410750</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Multi Strand 18ct Gold Plated Heart Necklace</t>
+        </is>
+      </c>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>baronessa</t>
+        </is>
+      </c>
       <c r="E66" t="n">
-        <v>4</v>
-      </c>
-      <c r="F66" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/baronessa/product/multi-strand-gold-plated-heart-necklace</t>
+        </is>
+      </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410750&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>260606</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
+          <t>1421647</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Sterling Silver Turquoise Anklet</t>
+        </is>
+      </c>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>marthajackson</t>
+        </is>
+      </c>
       <c r="E67" t="n">
         <v>2</v>
       </c>
-      <c r="F67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-turquoise-anklet</t>
+        </is>
+      </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421647&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>307261</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
+          <t>1433224</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Silver Graduation Cap Necklace Personalised Birthday Gift</t>
+        </is>
+      </c>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>theuniquechocolate</t>
+        </is>
+      </c>
       <c r="E68" t="n">
         <v>2</v>
       </c>
-      <c r="F68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/theuniquechocolate/product/silver-graduation-cap-necklace-personalised-christmas-gift</t>
+        </is>
+      </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=307261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1433224&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>380275</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
+          <t>1435032</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>nappyhead</t>
+        </is>
+      </c>
       <c r="E69" t="n">
         <v>2</v>
       </c>
-      <c r="F69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
+        </is>
+      </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>421466</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr"/>
+          <t>1435766</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>silverrainsilver</t>
+        </is>
+      </c>
       <c r="E70" t="n">
-        <v>6</v>
-      </c>
-      <c r="F70" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
+        </is>
+      </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>446429</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
+          <t>1436809</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Spitfire And Lancaster Double Garden Art</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>gapgardenproducts</t>
+        </is>
+      </c>
       <c r="E71" t="n">
-        <v>5</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/gapgardenproducts/product/spitfire-lancaster-double-garden-art</t>
+        </is>
+      </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>469358</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
+          <t>1456952</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Flower Slippers</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>thealphabetgiftshop</t>
+        </is>
+      </c>
       <c r="E72" t="n">
-        <v>6</v>
-      </c>
-      <c r="F72" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/flower-slippers</t>
+        </is>
+      </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>486442</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
+          <t>1475693</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Mum To Be Gift Growing Tiny Humans Is Exhausting</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>hallby</t>
+        </is>
+      </c>
       <c r="E73" t="n">
         <v>2</v>
       </c>
-      <c r="F73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hallby/product/mum-to-be-gift-growing-tiny-humans-is-exhausting</t>
+        </is>
+      </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486442&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>492043</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr"/>
+          <t>1480114</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Wedding Gift, Gift For Couples</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>thatlittlebagshop</t>
+        </is>
+      </c>
       <c r="E74" t="n">
         <v>2</v>
       </c>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thatlittlebagshop/product/wedding-gift-gift-for-couples</t>
+        </is>
+      </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=492043&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1480114&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>493192</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
+          <t>1486025</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Personalised Friendship Flower Pot</t>
+        </is>
+      </c>
       <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>sophiavictoriajoy</t>
+        </is>
+      </c>
       <c r="E75" t="n">
         <v>2</v>
       </c>
-      <c r="F75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-friendship-flower-pot</t>
+        </is>
+      </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=493192&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486025&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>510573</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
+          <t>1496888</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Petsentials Super Clumping Cat Litter 10 L</t>
+        </is>
+      </c>
       <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>noahsark</t>
+        </is>
+      </c>
       <c r="E76" t="n">
         <v>2</v>
       </c>
-      <c r="F76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-10l</t>
+        </is>
+      </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=510573&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496888&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>533246</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr"/>
+          <t>1497676</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Personalised Boarding Pass Scratch Reveal Ticket</t>
+        </is>
+      </c>
       <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>personalisednpretty</t>
+        </is>
+      </c>
       <c r="E77" t="n">
-        <v>3</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/personalisednpretty/product/boarding-pass-scratch-reveal-ticket</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>545355</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr"/>
+          <t>1498299</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Personalised 2nd Cotton Anniversary Frame Gift</t>
+        </is>
+      </c>
       <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>amysgiftstudio</t>
+        </is>
+      </c>
       <c r="E78" t="n">
-        <v>7</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/amysgiftstudio/product/personalised-2nd-cotton-anniversary-frame-gift</t>
+        </is>
+      </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498299&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>581579</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
+          <t>1502372</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Personalised 18th Birthday Card In Pink</t>
+        </is>
+      </c>
       <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>littlesentiments</t>
+        </is>
+      </c>
       <c r="E79" t="n">
         <v>2</v>
       </c>
-      <c r="F79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/littlesentiments/product/personalised-18th-birthday-card-in-pink</t>
+        </is>
+      </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=581579&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502372&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>621809</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
+          <t>1503687</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Nine Caramel Filled Chocolate Tennis Balls</t>
+        </is>
+      </c>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>chocolateonchocolate</t>
+        </is>
+      </c>
       <c r="E80" t="n">
-        <v>5</v>
-      </c>
-      <c r="F80" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/chocolateonchocolate/product/nine-caramel-filled-chocolate-tennis-balls</t>
+        </is>
+      </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>684433</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
+          <t>1503694</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company</t>
+        </is>
+      </c>
       <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>thelyndoncompany</t>
+        </is>
+      </c>
       <c r="E81" t="n">
         <v>2</v>
       </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
+        </is>
+      </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684433&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>689351</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr"/>
+          <t>1508206</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Set Of Three Copper Rain Catchers - Tangerine, Green And Red Garden Sculpture On Curved Iron Pole</t>
+        </is>
+      </c>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>thelondongardentradingco</t>
+        </is>
+      </c>
       <c r="E82" t="n">
         <v>2</v>
       </c>
-      <c r="F82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thelondongardentradingco/product/set-of-3-copper-rain-catchers-tangerine-green-red-garden-sculpture-on-curved-iron-pole</t>
+        </is>
+      </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508206&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>706455</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
+          <t>1508229</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Personalised 2025 Graduation Keyring, Graduation Cap</t>
+        </is>
+      </c>
       <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>wildwarestudio</t>
+        </is>
+      </c>
       <c r="E83" t="n">
         <v>2</v>
       </c>
-      <c r="F83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/wildwarestudio/product/personalised-2025-graduation-keyring-graduation-cap</t>
+        </is>
+      </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=706455&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>722492</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
+          <t>1509775</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Sterling Silver Birthstone Beaded Bracelet</t>
+        </is>
+      </c>
       <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>wishedfor</t>
+        </is>
+      </c>
       <c r="E84" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/wishedfor/product/sterling-silver-birthstone-beaded-bracelet</t>
+        </is>
+      </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>761621</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
+          <t>1512669</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Personalised Teacher Thank You Mug</t>
+        </is>
+      </c>
       <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>arrowgiftco</t>
+        </is>
+      </c>
       <c r="E85" t="n">
         <v>2</v>
       </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-teacher-thank-you-mug</t>
+        </is>
+      </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=761621&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512669&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>764151</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
+          <t>298443</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Personalised Metal Street Sign</t>
+        </is>
+      </c>
       <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>oakdenedesigns</t>
+        </is>
+      </c>
       <c r="E86" t="n">
         <v>2</v>
       </c>
-      <c r="F86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
+        </is>
+      </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>771041</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
+          <t>350209</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Sterling Silver April Shower Drop Earrings</t>
+        </is>
+      </c>
       <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>marthajackson</t>
+        </is>
+      </c>
       <c r="E87" t="n">
-        <v>3</v>
-      </c>
-      <c r="F87" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+        </is>
+      </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>785952</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
+          <t>380275</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>White Cotton Victorian Styled Panel Nightdress</t>
+        </is>
+      </c>
       <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>minilunn</t>
+        </is>
+      </c>
       <c r="E88" t="n">
-        <v>2</v>
-      </c>
-      <c r="F88" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/minilunn/product/front-panel</t>
+        </is>
+      </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=785952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>804990</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
+          <t>408467</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Sterling Silver Falling Leaves Necklace</t>
+        </is>
+      </c>
       <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>marthajackson</t>
+        </is>
+      </c>
       <c r="E89" t="n">
         <v>2</v>
       </c>
-      <c r="F89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-falling-leaves-necklace</t>
+        </is>
+      </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=408467&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>866983</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
+          <t>421466</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Peridot Quartz Drop Earrings</t>
+        </is>
+      </c>
       <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>sarahhickeyjewellery</t>
+        </is>
+      </c>
       <c r="E90" t="n">
         <v>3</v>
       </c>
-      <c r="F90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+        </is>
+      </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>868202</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
+          <t>446429</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Personalised Teacher Notebook Journal</t>
+        </is>
+      </c>
       <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>catsprintshop</t>
+        </is>
+      </c>
       <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/catsprintshop/product/personalised-teacher-notebook-journal</t>
+        </is>
+      </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>872066</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
+          <t>454128</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Hanging Garden Bird Dish</t>
+        </is>
+      </c>
       <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>dibor</t>
+        </is>
+      </c>
       <c r="E92" t="n">
         <v>2</v>
       </c>
-      <c r="F92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/dibor/product/hanging-heart-bird-dish</t>
+        </is>
+      </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=454128&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>875307</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
+          <t>462337</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Aquamarine Quartz, Moonstone And Pearl Earrings</t>
+        </is>
+      </c>
       <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>sarahhickeyjewellery</t>
+        </is>
+      </c>
       <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/aquamarine-quartz-moonstone-and-pearl-earrings</t>
+        </is>
+      </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=875307&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
+          <t>469358</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Family Birthstone Link Bracelet</t>
+        </is>
+      </c>
       <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>joybycorrinesmith</t>
+        </is>
+      </c>
       <c r="E94" t="n">
-        <v>5</v>
-      </c>
-      <c r="F94" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+        </is>
+      </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>879581</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
+          <t>501290</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>70th Birthday 1955 Farthing Coin Bottle Stopper</t>
+        </is>
+      </c>
       <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>ellieellie</t>
+        </is>
+      </c>
       <c r="E95" t="n">
         <v>2</v>
       </c>
-      <c r="F95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/farthing-70th-1945-coin-bottle-stopper</t>
+        </is>
+      </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879581&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=501290&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>880642</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
+          <t>512405</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Set Of Three Cat Socks In A Gift Box</t>
+        </is>
+      </c>
       <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E96" t="n">
         <v>2</v>
       </c>
-      <c r="F96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/set-of-three-cat-socks-in-a-gift-box</t>
+        </is>
+      </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>881907</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
+          <t>527736</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Personalised Child's Bracelet With Silver Heart Charm</t>
+        </is>
+      </c>
       <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>nest</t>
+        </is>
+      </c>
       <c r="E97" t="n">
         <v>2</v>
       </c>
-      <c r="F97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/nest/product/personalised-childrens-bracelet-with-silver-heart-charm</t>
+        </is>
+      </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=527736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>905169</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
+          <t>533246</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Wedding Song Lyrics Record Print</t>
+        </is>
+      </c>
       <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>yoursforkeeps</t>
+        </is>
+      </c>
       <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/yoursforkeeps/product/wedding-song-print</t>
+        </is>
+      </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>909642</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
+          <t>610619</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
+        </is>
+      </c>
       <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>mygivenname</t>
+        </is>
+      </c>
       <c r="E99" t="n">
-        <v>2</v>
-      </c>
-      <c r="F99" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+        </is>
+      </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=909642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
+          <t>621809</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Friendship Knot Bangle</t>
+        </is>
+      </c>
       <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>joybycorrinesmith</t>
+        </is>
+      </c>
       <c r="E100" t="n">
         <v>2</v>
       </c>
-      <c r="F100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+        </is>
+      </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>940836</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr"/>
+          <t>643101</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>'A New Chapter Begins...' Bookmark</t>
+        </is>
+      </c>
       <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>kutuu</t>
+        </is>
+      </c>
       <c r="E101" t="n">
-        <v>2</v>
-      </c>
-      <c r="F101" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
+        </is>
+      </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=940836&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>941353</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr"/>
+          <t>684208</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Hanging Tea Light Holders Gift Set</t>
+        </is>
+      </c>
       <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>dibor</t>
+        </is>
+      </c>
       <c r="E102" t="n">
         <v>2</v>
       </c>
-      <c r="F102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/dibor/product/champagne-glass-dimple-candle-holder</t>
+        </is>
+      </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=941353&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>944163</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr"/>
+          <t>703615</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Personalised Graduation Skyline Art Print Unframed</t>
+        </is>
+      </c>
       <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>beckagriffinillustration</t>
+        </is>
+      </c>
       <c r="E103" t="n">
         <v>2</v>
       </c>
-      <c r="F103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/beckagriffinillustration/product/personalised-graduation-skyline-art-print</t>
+        </is>
+      </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944163&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=703615&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>950557</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr"/>
+          <t>717260</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Personalised Sterling Silver Graduation Charm Bracelet</t>
+        </is>
+      </c>
       <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>hurleyburley</t>
+        </is>
+      </c>
       <c r="E104" t="n">
         <v>2</v>
       </c>
-      <c r="F104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-sterling-silver-graduation-charm-bracelet</t>
+        </is>
+      </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950557&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=717260&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>950712</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr"/>
+          <t>722492</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Personalised Graduation Gift City Print</t>
+        </is>
+      </c>
       <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>handmadebytessagalloway</t>
+        </is>
+      </c>
       <c r="E105" t="n">
         <v>2</v>
       </c>
-      <c r="F105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/handmadebytessagalloway/product/personalised-graduation-gift-city-print</t>
+        </is>
+      </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>950732</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr"/>
+          <t>738289</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Personalised Head Chef Apron, Cooking Gift</t>
+        </is>
+      </c>
       <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>weaselandstoat</t>
+        </is>
+      </c>
       <c r="E106" t="n">
-        <v>3</v>
-      </c>
-      <c r="F106" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
+        </is>
+      </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>976980</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+        </is>
+      </c>
       <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>therusticdish</t>
+        </is>
+      </c>
       <c r="E107" t="n">
         <v>2</v>
       </c>
-      <c r="F107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+        </is>
+      </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>982044</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr"/>
+          <t>771041</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
+        </is>
+      </c>
       <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>bankslyonbotanical</t>
+        </is>
+      </c>
       <c r="E108" t="n">
         <v>2</v>
       </c>
-      <c r="F108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
+        </is>
+      </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>990259</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr"/>
+          <t>786480</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Sterling Silver Family Birthstones Sliding Bracelet</t>
+        </is>
+      </c>
       <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>gaamaa</t>
+        </is>
+      </c>
       <c r="E109" t="n">
         <v>2</v>
       </c>
-      <c r="F109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-family-birthstone-bracelet</t>
+        </is>
+      </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=990259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786480&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>991741</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr"/>
+          <t>793949</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Personalised Happy Birthday Keepsake Book</t>
+        </is>
+      </c>
       <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>mygivenname</t>
+        </is>
+      </c>
       <c r="E110" t="n">
         <v>2</v>
       </c>
-      <c r="F110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/personalised-happy-birthday-keepsake-book</t>
+        </is>
+      </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=793949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
+          <t>801933</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Personalised Pull Out Photo Album Token Gift</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>sophiavictoriajoy</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>2</v>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>828426</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="n">
+        <v>2</v>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>848232</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Personalised 60 Th Birthday Book 'Memory Lane'</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>lucysworld</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>2</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-60th-birthday-book-memory-lane</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=848232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>857942</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>2</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>860698</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Personalised 70th Birthday Book 'Memory Lane'</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>lucysworld</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>2</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-70th-birthday-book-memory-lane</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>874166</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Graduation Cap Silver Charm Bracelet Gift For Her</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>lhgdesigns</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>2</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lhgdesigns/product/graduation-cap-silver-charm-bracelet-gift-for-her</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=874166&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>903313</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Mother And Child Birthstone Charm Necklace</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>joybycorrinesmith</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>2</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/mother-and-child-birthstone-charm-necklace</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903313&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>90344</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Personalised Rag Doll</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>thealphabetgiftshop</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>2</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-rag-doll</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=90344&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>923932</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Happy Birthday Celebration Hamper</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>lottieshaws</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>2</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lottieshaws/product/birthday-hamper-box</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=923932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>930044</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>'Floral Summer' Mixed Pack Of Ten Greeting Cards</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>faysstudio</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>2</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/faysstudio/product/floral-summer-pack-of-ten-greeting-cards</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=930044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>950712</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Elephant Good Fortune Foil Scarf</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>2</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/elephant-raised-trunk-good-fortune-scarf-letterbox-gift</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>984487</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Personalised Men's Woven Vegan Bracelet With Clasp</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>lisaangeljewellery</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>2</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-men-s-woven-vegan-bracelet-with-clasp</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
           <t>999592</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="n">
-        <v>3</v>
-      </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr">
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>2</v>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-07-28T01:54:04Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1029102</t>
+          <t>1035825</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Hiking Walking Boot Boot Tag</t>
+          <t>Personalised Treat Pot For Him</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,24 +492,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/personalised-hiking-walking-boot-boot-tag</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-father-s-day-treat-pot</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1029102&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1030998</t>
+          <t>1047473</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Name Among Stars Personalised Luxury Notebook Journal</t>
+          <t>Personalised Brilliant Teacher Notebook Journal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -519,34 +519,34 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/betsybenn/product/name-among-stars-personalised-luxury-notebook-journal</t>
+          <t>https://www.notonthehighstreet.com/betsybenn/product/personalised-brilliant-teacher-notebook-journal</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1030998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047473&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1031001</t>
+          <t>1057279</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adventure Personalised Travel Journal Notebook</t>
+          <t>Personalised Wooden Bamboo Pen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>betsybenn</t>
+          <t>giftsonline4u</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/betsybenn/product/adventure-personalised-travel-journal-notebook</t>
+          <t>https://www.notonthehighstreet.com/giftsonline4u/product/personalised-wooden-bamboo-pen</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1031001&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1057279&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1033155</t>
+          <t>1061155</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Floral Birthday Card</t>
+          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>daisymaison</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,154 +585,154 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1035850</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Graduation Hinged Wooden Bottle Gift Box</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>dreamstoreality</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dreamstoreality/product/personalised-graduation-hinged-wooden-bottle-gift-box</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035850&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1036840</t>
+          <t>1067493</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13th Lace Wedding Anniversary Personalised Card</t>
+          <t>Natural Flowers Summer Door Wreath</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>thehummingbirdcardcompany</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thehummingbirdcardcompany/product/13th-lace-wedding-anniversary-card</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1036840&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1037522</t>
+          <t>1084722</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Graduation Map Card</t>
+          <t>Wedding Gift Personalised Map Print Of Wedding Venue</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>monoscape</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
+          <t>https://www.notonthehighstreet.com/monoscape/product/wedding-gift-personalised-map-print-of-wedding-venue</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1084722&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1047473</t>
+          <t>1104597</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Brilliant Teacher Notebook Journal</t>
+          <t>Personalised Vintage Copper Garden Bucket Planter</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>betsybenn</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/betsybenn/product/personalised-brilliant-teacher-notebook-journal</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-vintage-copper-garden-bucket-planter</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047473&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1104597&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1047587</t>
+          <t>1107283</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Van Gogh Print Silk Scarf</t>
+          <t>Personalised Embroidered Initials Washbag</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,30 +740,30 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/van-gogh-almond-blossom-silk-scarf</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-embroidered-initials-washbag</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047587&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1107283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1051200</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Locket Necklace</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,30 +771,30 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-birth-flower-locket-necklace</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1051200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1053070</t>
+          <t>1158505</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Birth Flower Scarf And Card In A Gift Box</t>
+          <t>Personalised Graduation Map Gift, University Print</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>hooddesignsco</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -802,61 +802,61 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/birth-flower-scarf-and-card-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-graduation-map-gift-university-print</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053070&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158505&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1060664</t>
+          <t>1171326</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Personalised Garden Sign</t>
+          <t>Dog Breed ID Tag Personalised Realistic Illustrations</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>hoobynoo</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-garden-sign</t>
+          <t>https://www.notonthehighstreet.com/hoobynoo/product/dog-breed-id-tag-personalised-realistic-illustrations</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1060664&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1171326&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1061842</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Family Street Sign</t>
+          <t>Personalised Birth Flower Stoneware Mug</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -864,61 +864,61 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-family-street-sign</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1182639</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>bubblebusinessuk</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1065178</t>
+          <t>1190985</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Personalised Wedding Planner And Organiser</t>
+          <t>Personalised Birth Month Flower Printed Can Glass</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>marthabrook</t>
+          <t>propergoose</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -926,30 +926,30 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-wedding-planner-and-organiser</t>
+          <t>https://www.notonthehighstreet.com/propergoose/product/personalised-birth-month-flower-printed-can-glass</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1065178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1194413</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Natural Flowers Summer Door Wreath</t>
+          <t>Thank You Teacher Personalised Coloured Enamel Mug</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -957,61 +957,61 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/thank-you-teacher-personalised-coloured-enamel-mug</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1194413&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1091599</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Graduation Silver Plated Certificate Holder</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>bellapersonalisedgiftsltd</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bellapersonalisedgiftsltd/product/personalised-silver-plated-certificate-holder-gift</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1091599&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1095606</t>
+          <t>1210491</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Edinburgh Graduation Skyline Personalised Card</t>
+          <t>Silver Plated Star Friendship Bracelet</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>mooandsnip</t>
+          <t>letterboxlove</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1019,30 +1019,30 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mooandsnip/product/edinburgh-graduation-skyline-personalised-card</t>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/silver-friendship-bracelet</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1095606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210491&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>109904</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tabletop Garden Oil Torch Steel Ltzaf152</t>
+          <t>Sterling Silver Twist Ball Dangly Earrings</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>thelondongardentradingco</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,185 +1050,185 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelondongardentradingco/product/glass-and-steel-oil-burning-torch-red</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=109904&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1238724</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Mug 'Good Luck Finding Better Colleagues'</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>arrowgiftco</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/good-luck-personalised-mug</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1238724&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1154280</t>
+          <t>1245502</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Personalised Oak Road Sign Style Plaque</t>
+          <t>Sterling Silver And Gold Daisy April Birth Flower Earrings</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-oak-road-sign-style-plaque</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1246450</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+          <t>Weekly Positivity Floral Desktop Flip Chart</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1179458</t>
+          <t>1247679</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Long Wildflower Amazing Friend Trinket Dish</t>
+          <t>Silver Plated Anxiety Fidget Bracelet Adjustable Worry School Exam Gcse Sats</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>wishuponastring</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
+          <t>https://www.notonthehighstreet.com/wishuponastring/product/925-sterling-silver-anxiety-fidget-bracelet-adjustable</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1247679&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1248592</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Personalised Women's Technology Travel Case Gift</t>
+          <t>Personalised Sterling Silver Cross Necklace</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-plain-cross-pendant</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1248592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1182280</t>
+          <t>1260374</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Personalised Floral 30th Birthday Card</t>
+          <t>Sterling Silver Blue Forget Me Not Flower Stud Earrings</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>oliviamorgan</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1236,61 +1236,61 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-floral-30th-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1182639</t>
+          <t>1264171</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
+          <t>Personalised Leather Notebook Lined</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>bubblebusinessuk</t>
+          <t>hotdot</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
+          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-leather-notebook-a5-lined</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1271268</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Personalised Best Friends Pebble Picture</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1298,30 +1298,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friendship-pebble-picture</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1200812</t>
+          <t>1272901</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Personalised Wedding Indoor Plant Pot</t>
+          <t>Mens Sterling Silver Flat Curb Bracelet</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>letterfest</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,92 +1329,92 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-wedding-indoor-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/4mm-sterling-silver-flat-curb-chain-bracelet</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1200812&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1211012</t>
+          <t>1276718</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sterling Silver Bold Coil Drop Earrings</t>
+          <t>Metallic Personalised Record Song Lyrics Print</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>spincollective</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/spincollective/product/metallic-personalised-record-song-lyrics-print</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1212257</t>
+          <t>1278602</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Personalised Birthday Card Day You Were Born Music</t>
+          <t>Birth Flower Birthday Gift Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>elevencorners</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/elevencorners/product/personalised-birthday-card-day-you-were-born-music</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birth-flower-personalised-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1212257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1234030</t>
+          <t>1290822</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Baltic Amber Bumble Bee Necklace</t>
+          <t>Personalised Wedding Anniversary Gift Candle Holder Set</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>mirrorin</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1422,30 +1422,30 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
+          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-anniversary-candle-holder-set</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1244126</t>
+          <t>1305083</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>60th Birthday Sterling Silver Bracelet</t>
+          <t>Personalised Striped Tote Bag</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1453,61 +1453,61 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/60th-birthday-sterling-silver-bracelet</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-striped-tote-bag</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1245502</t>
+          <t>1317092</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Daisy April Birth Flower Earrings</t>
+          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1246450</t>
+          <t>1319990</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Weekly Positivity Floral Desktop Flip Chart</t>
+          <t>Heart Cocktail Glass With Personalised Metal Straw</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>myleelondon</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,92 +1515,92 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
+          <t>https://www.notonthehighstreet.com/myleelondon/product/heart-cocktail-glass</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1319990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1246966</t>
+          <t>1320832</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mustard Ginkgo Print Scarf</t>
+          <t>Sterling Silver Name Necklace</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>potiega</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/ginkgo-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/potiega/product/sterling-silver-name-necklace</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1269933</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sunshine Jewellery Stand With Terrazzo Base</t>
+          <t>Sheep Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/sunshine-jewellery-stand-with-terrazzo-base</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1269933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1276721</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Metallic Personalised Record Player Song Lyrics Print</t>
+          <t>Fabric Name Peekaboo Memory Box</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>spincollective</t>
+          <t>modocreative</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,92 +1608,92 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/spincollective/product/metallic-personalised-record-player-song-lyrics-print</t>
+          <t>https://www.notonthehighstreet.com/modocreative/product/fabric-peekaboo-keepsake-box</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1290822</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Personalised Wedding Anniversary Gift Candle Holder Set</t>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>mirrorin</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-anniversary-candle-holder-set</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1301141</t>
+          <t>1354859</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Set Of Two Wire Robin Decorative Ornament</t>
+          <t>Ceramic Little Book Of Flowers Vase</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>paperhigh</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/paperhigh/product/set-of-two-wire-robin-decorative-ornament</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/ceramic-little-book-of-flowers-vase</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1301141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1302008</t>
+          <t>1357569</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Your Own Words Block Text Personalised Notebook</t>
+          <t>Swarovski Crystal Single Row Choker Necklace</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>betsybenn</t>
+          <t>dynastylondon</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,61 +1701,61 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/betsybenn/product/your-own-words-block-text-personalised-notebook</t>
+          <t>https://www.notonthehighstreet.com/dynastylondon/product/swarovski-crystal-single-row-choker-necklace</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1302008&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1304639</t>
+          <t>1362911</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Personalised Teacher Pebble Picture</t>
+          <t>Personalised Brownie Box</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>rubythecakeartist</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-teacher-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1304639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1307555</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Personalised Graduation Pebble Picture</t>
+          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>iconiccoasters</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1763,30 +1763,30 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-graduation-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1314094</t>
+          <t>1372560</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sterling Silver Sewing Button Stud Earrings</t>
+          <t>Personalised Tractor Keepsake Birthday Card</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>noordinarygiftcompany</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1794,92 +1794,92 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/round-sewing-button-earrings-in-sterling-silver</t>
+          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/personalised-tractor-keepsake-birthday-card</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1314094&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1317092</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
+          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1326272</t>
+          <t>1396397</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Orange Sunflower Motif Scarf</t>
+          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/orange-sunflower-motif-scarf-in-a-box</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1330966</t>
+          <t>1402097</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Handmade Personalised Leather Curved Corner Bookmark</t>
+          <t>Puff Heart Bracelet With Heart Charm</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>parkerandco</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1887,185 +1887,185 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/parkerandco/product/handmade-personalised-leather-curved-corner-bookmark</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/puff-heart-bracelet-with-heart-charm</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402097&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1412559</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+          <t>Personalised Teacher Gift - Thank You Flower Vase</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>laurastanleydesigns</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-teacher-gift-thank-you-flower-vase</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412559&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1345526</t>
+          <t>1416296</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle With Birthstone Hearts</t>
+          <t>Women's White Cotton Victorian Short Sleeve Nightdress Front Panel</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle-with-birthstone-hearts</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/white-cotton-victorian-short-sleeve-nightdress-front-panel</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416296&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1419917</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
+          <t>Personalised Champagne Retirement Card</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>wholeinthemiddle</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
+          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/personalised-champagne-retirement-card</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419917&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1346621</t>
+          <t>1420726</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Festive Christmas Magnetic Brooch</t>
+          <t>Personalised Metal Music Sheet Page Holder</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/festive-christmas-magnetic-brooch</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-music-sheet-page-holder</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1346621&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1354859</t>
+          <t>1422513</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Ceramic Little Book Of Flowers Vase</t>
+          <t>Sterling Silver Paw Print Adjustable Ring</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>feelsilkstudio</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/ceramic-little-book-of-flowers-vase</t>
+          <t>https://www.notonthehighstreet.com/feelsilkstudio/product/sterling-silver-paw-print-adjustable-ring</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1365394</t>
+          <t>1435032</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
+          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2073,30 +2073,30 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1366698</t>
+          <t>1443868</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Christening Gift Personalised Book Words Of Wisdom</t>
+          <t>Silver Jade Gemstone Acorn Earrings</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>mymagicname</t>
+          <t>silkpursesowsear</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2104,30 +2104,30 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-gift-personalised-book-words-of-wisdom</t>
+          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/silver-gemstone-acorn-earrings</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1366698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1368436</t>
+          <t>1486088</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Special Granddaughter Personalised Birthday Card</t>
+          <t>Janhvi The Small Quacking Duck Wire Garden Ornament</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>paperscene</t>
+          <t>paperhigh</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2135,61 +2135,61 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/paperscene/product/special-granddaughter-personalised-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/paperhigh/product/janhvi-the-small-quacking-duck-wire-garden-ornament</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368436&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486088&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1372919</t>
+          <t>1486376</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1965 Personalised 60th Diamond Wedding Anniversary Poster</t>
+          <t>Teacher Thank You Candle - 'Difference Maker' Definition</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-60th-diamond-wedding-anniversary-poster</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/teacher-thank-you-candle-difference-maker-definition</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372919&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486376&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1376487</t>
+          <t>1496888</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tiny Turtle Strength Bracelet</t>
+          <t>Petsentials Super Clumping Cat Litter 10 L</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>letterboxlove</t>
+          <t>noahsark</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2197,61 +2197,61 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterboxlove/product/tiny-turtle-strength-bracelet</t>
+          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-10l</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496888&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1498809</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
+          <t>New Home Heart Shaped Ceramic Keepsake Gift</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>pinkstrawberry</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/pinkstrawberry/product/new-home-heart-shaped-ceramic-keepsake-gift</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1384152</t>
+          <t>1499827</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Personalised Elephant Money Box For Christening Baptism</t>
+          <t>Personalised Cartoon Anniversary And Birthday Card</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>mirrorin</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-elephant-money-box-for-christening-baptism</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-3d-animated-greeting-card</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1384152&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1389021</t>
+          <t>1500474</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1st Birthday Book Of Nursery Rhymes And Poems</t>
+          <t>Personalised Big Sister Bracelet</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>nameitwhatyoulike</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,30 +2290,30 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/1st-birthday-book-of-nursery-rhymes-and-poems</t>
+          <t>https://www.notonthehighstreet.com/nameitwhatyoulike/product/personalised-big-sister-charm-bracelet</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500474&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1394198</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Formula One F1 2025 Calendar Track Mug Gift For Him</t>
+          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>iconiccoasters</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2321,30 +2321,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/iconiccoasters/product/formula-one-f1-2024-calendar-track-mug-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1401190</t>
+          <t>1507466</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sterling Silver Little Daisy Flower Drop Hook Earrings</t>
+          <t>2025 Graduation Keyring, Personalised Gift Keepsake</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>wildwarestudio</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2352,92 +2352,92 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/little-daisy-flower-drop-hook-earrings</t>
+          <t>https://www.notonthehighstreet.com/wildwarestudio/product/2025-graduation-keyring-personalised-gift-keepsake</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1507466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1408415</t>
+          <t>1508460</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Wine Bottle Gift Set</t>
+          <t>Personalised Saturday Night Snacks Bowl</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>thealphabetgiftshop</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-60th-birthday-wine-bottle-gift-set</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-saturday-night-snacks-bowl</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1408415&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1409309</t>
+          <t>1512669</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>60th Birthday Bracelet, Kate, Sterling Silver</t>
+          <t>Personalised Teacher Thank You Mug</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>wishedfor</t>
+          <t>arrowgiftco</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wishedfor/product/60th-birthday-bracelet-kate-sterling-silver</t>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-teacher-thank-you-mug</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1409309&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512669&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1410229</t>
+          <t>1523637</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Personalised 40th Ruby Anniversary Card For Husband/Wife</t>
+          <t>Pink Candyfloss Marshmallow</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>hopeandlove</t>
+          <t>scouseafricansweetery</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2445,30 +2445,30 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hopeandlove/product/personalised-40th-ruby-anniversary-card-for-husband-wife</t>
+          <t>https://www.notonthehighstreet.com/scouseafricansweetery/product/pink-candyfloss-marshmallow</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523637&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1410750</t>
+          <t>152410</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Multi Strand 18ct Gold Plated Heart Necklace</t>
+          <t>Personalised Treasured Location Print</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>baronessa</t>
+          <t>brambler</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2476,30 +2476,30 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/baronessa/product/multi-strand-gold-plated-heart-necklace</t>
+          <t>https://www.notonthehighstreet.com/brambler/product/giclee-bespoke-treasured-location</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410750&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=152410&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1421647</t>
+          <t>177216</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sterling Silver Turquoise Anklet</t>
+          <t>Baby Hand And Foot Inkless Print Kit</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>elizabethjane</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2507,154 +2507,154 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-turquoise-anklet</t>
+          <t>https://www.notonthehighstreet.com/elizabethjane/product/baby-hand-and-foot-inkless-print</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421647&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=177216&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>1433224</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Silver Graduation Cap Necklace Personalised Birthday Gift</t>
+          <t>Personalised Metal Street Sign</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>theuniquechocolate</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theuniquechocolate/product/silver-graduation-cap-necklace-personalised-christmas-gift</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1433224&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1435032</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
+          <t>Sterling Silver April Shower Drop Earrings</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>1435766</t>
+          <t>412675</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
+          <t>Literary Paper 1st Anniversary Rose</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>cot2totandbeyond</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
+          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>1436809</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Spitfire And Lancaster Double Garden Art</t>
+          <t>Peridot Quartz Drop Earrings</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>gapgardenproducts</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gapgardenproducts/product/spitfire-lancaster-double-garden-art</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1456952</t>
+          <t>433785</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Flower Slippers</t>
+          <t>White Cotton Short Sleeve Nightdress 18th Century</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>thealphabetgiftshop</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2662,61 +2662,61 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/flower-slippers</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/18th-century-cotton-nightdress</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>1475693</t>
+          <t>446429</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Mum To Be Gift Growing Tiny Humans Is Exhausting</t>
+          <t>Personalised Teacher Notebook Journal</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>hallby</t>
+          <t>catsprintshop</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hallby/product/mum-to-be-gift-growing-tiny-humans-is-exhausting</t>
+          <t>https://www.notonthehighstreet.com/catsprintshop/product/personalised-teacher-notebook-journal</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>1480114</t>
+          <t>462337</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Wedding Gift, Gift For Couples</t>
+          <t>Aquamarine Quartz, Moonstone And Pearl Earrings</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>thatlittlebagshop</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2724,92 +2724,92 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatlittlebagshop/product/wedding-gift-gift-for-couples</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/aquamarine-quartz-moonstone-and-pearl-earrings</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1480114&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>1486025</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Personalised Friendship Flower Pot</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-friendship-flower-pot</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486025&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1496888</t>
+          <t>488356</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Petsentials Super Clumping Cat Litter 10 L</t>
+          <t>Sterling Silver Secret Message Ring</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>noahsark</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-10l</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496888&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>1497676</t>
+          <t>512405</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Personalised Boarding Pass Scratch Reveal Ticket</t>
+          <t>Set Of Three Cat Socks In A Gift Box</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>personalisednpretty</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2817,30 +2817,30 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/personalisednpretty/product/boarding-pass-scratch-reveal-ticket</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/set-of-three-cat-socks-in-a-gift-box</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>1498299</t>
+          <t>520238</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Personalised 2nd Cotton Anniversary Frame Gift</t>
+          <t>Silver St Christopher Double Heart Charm Necklace</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>amysgiftstudio</t>
+          <t>hurleyburleyjunior</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2848,30 +2848,30 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/amysgiftstudio/product/personalised-2nd-cotton-anniversary-frame-gift</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/silver-st-christopher-double-heart-charm-necklace</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498299&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=520238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>1502372</t>
+          <t>607975</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Personalised 18th Birthday Card In Pink</t>
+          <t>Mineral Bath Infusions Gift Collection</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>littlesentiments</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2879,92 +2879,92 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/littlesentiments/product/personalised-18th-birthday-card-in-pink</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/mineral-bath-infusions-gift-collection</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502372&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>1503687</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Nine Caramel Filled Chocolate Tennis Balls</t>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>chocolateonchocolate</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/chocolateonchocolate/product/nine-caramel-filled-chocolate-tennis-balls</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503687&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company</t>
+          <t>Friendship Knot Bangle</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>thelyndoncompany</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>1508206</t>
+          <t>643101</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Set Of Three Copper Rain Catchers - Tangerine, Green And Red Garden Sculpture On Curved Iron Pole</t>
+          <t>'A New Chapter Begins...' Bookmark</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>thelondongardentradingco</t>
+          <t>kutuu</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2972,30 +2972,30 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelondongardentradingco/product/set-of-3-copper-rain-catchers-tangerine-green-red-garden-sculpture-on-curved-iron-pole</t>
+          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508206&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>1508229</t>
+          <t>695129</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Personalised 2025 Graduation Keyring, Graduation Cap</t>
+          <t>Personalised Vintage Garden Bird Dish</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>wildwarestudio</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3003,30 +3003,30 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wildwarestudio/product/personalised-2025-graduation-keyring-graduation-cap</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/love-birds-6th-anniverary-iron-hanging-heart-bird-dish</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>1509775</t>
+          <t>707031</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Beaded Bracelet</t>
+          <t>Graduation Charm Bracelet</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>wishedfor</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -3034,55 +3034,55 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wishedfor/product/sterling-silver-birthstone-beaded-bracelet</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/graduation-charm-bracelet</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=707031&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>1512669</t>
+          <t>722492</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Personalised Teacher Thank You Mug</t>
+          <t>Personalised Graduation Gift City Print</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>arrowgiftco</t>
+          <t>handmadebytessagalloway</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-teacher-thank-you-mug</t>
+          <t>https://www.notonthehighstreet.com/handmadebytessagalloway/product/personalised-graduation-gift-city-print</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512669&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>298443</t>
+          <t>760714</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Personalised Metal Street Sign</t>
+          <t>Personalised Name Bottle Opener</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -3096,61 +3096,61 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-name-bottle-opener</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760714&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>764045</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Sterling Silver April Shower Drop Earrings</t>
+          <t>Personalised Birthstone Disc Stretch Bracelet</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>380275</t>
+          <t>770939</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>White Cotton Victorian Styled Panel Nightdress</t>
+          <t>Metallic Bee Print Scarf</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -3158,30 +3158,30 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/front-panel</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-bee-print-scarf</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770939&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>408467</t>
+          <t>772232</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sterling Silver Falling Leaves Necklace</t>
+          <t>Personalised Moon And Star Necklace</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -3189,92 +3189,92 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-falling-leaves-necklace</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/moon-and-star-necklace-with-personalised-box</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=408467&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>773419</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Gunmetal Pearl And Cashmere Blend Scarf</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/gun-metal-pearl-cashmere-shawl</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=773419&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>446429</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Personalised Teacher Notebook Journal</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
-          <t>catsprintshop</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/catsprintshop/product/personalised-teacher-notebook-journal</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>454128</t>
+          <t>797444</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Hanging Garden Bird Dish</t>
+          <t>Personalised Graduation Necklace</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -3282,92 +3282,92 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/hanging-heart-bird-dish</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-graduation-necklace</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=454128&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=797444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>828426</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Aquamarine Quartz, Moonstone And Pearl Earrings</t>
+          <t>Personalised 'Promises To You' Book For Godchild</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>lucysworld</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/aquamarine-quartz-moonstone-and-pearl-earrings</t>
+          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-promises-to-you-book-for-godchild</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>501290</t>
+          <t>868202</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>70th Birthday 1955 Farthing Coin Bottle Stopper</t>
+          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -3375,30 +3375,30 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/farthing-70th-1945-coin-bottle-stopper</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=501290&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>512405</t>
+          <t>872048</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Set Of Three Cat Socks In A Gift Box</t>
+          <t>Sterling Silver Dangly Crescent Earrings</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -3406,61 +3406,61 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/set-of-three-cat-socks-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-crescent-drop-earrings</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872048&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>527736</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Personalised Child's Bracelet With Silver Heart Charm</t>
+          <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr">
         <is>
-          <t>nest</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nest/product/personalised-childrens-bracelet-with-silver-heart-charm</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=527736&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>533246</t>
+          <t>882796</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Wedding Song Lyrics Record Print</t>
+          <t>Stainforth Large Blue Ceramic Jug Vase</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr">
         <is>
-          <t>yoursforkeeps</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3468,55 +3468,55 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/yoursforkeeps/product/wedding-song-print</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/stainforth-large-blue-ceramic-ribbed-jug</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>893548</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
+          <t>Personalised Luxury Leather Two Part Wash Bag</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>hurleyburleyman</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-luxury-leather-two-part-washbag</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=893548&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>903313</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle</t>
+          <t>Mother And Child Birthstone Charm Necklace</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -3530,61 +3530,61 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/mother-and-child-birthstone-charm-necklace</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903313&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>643101</t>
+          <t>905169</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>'A New Chapter Begins...' Bookmark</t>
+          <t>Birthstone Bracelet</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr">
         <is>
-          <t>kutuu</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>684208</t>
+          <t>907471</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Hanging Tea Light Holders Gift Set</t>
+          <t>Personalised Motorhome Travel Journal Notebook</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -3592,30 +3592,30 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/champagne-glass-dimple-candle-holder</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-motorhome-travel-journal-notebook</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=907471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>703615</t>
+          <t>917605</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Personalised Graduation Skyline Art Print Unframed</t>
+          <t>Personalised Couples Large Matchbox</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
         <is>
-          <t>beckagriffinillustration</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -3623,30 +3623,30 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/beckagriffinillustration/product/personalised-graduation-skyline-art-print</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=703615&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>717260</t>
+          <t>918435</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Graduation Charm Bracelet</t>
+          <t>Family Birth Month Flower Print</t>
         </is>
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>vintagedesignsreborn</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -3654,30 +3654,30 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-sterling-silver-graduation-charm-bracelet</t>
+          <t>https://www.notonthehighstreet.com/vintagedesignsreborn/product/family-birth-month-flower-print</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=717260&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=918435&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>722492</t>
+          <t>934374</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Personalised Graduation Gift City Print</t>
+          <t>Personalised Luxury Extra Deep A4 Blush Pink Gift Box</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr">
         <is>
-          <t>handmadebytessagalloway</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -3685,30 +3685,30 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handmadebytessagalloway/product/personalised-graduation-gift-city-print</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/hug-in-a-box-personalised-luxury-gift-box</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=934374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>738289</t>
+          <t>948800</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Personalised Head Chef Apron, Cooking Gift</t>
+          <t>Large Butterfly Print Scarf</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
         <is>
-          <t>weaselandstoat</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -3716,61 +3716,61 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>950732</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+          <t>Dragonfly Foil Scarf Letterbox Gift</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>771041</t>
+          <t>971121</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Personalised Relaxation And Wellness Pamper Gift Set</t>
+          <t>Personalised Alphabet Zoo Story Book</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr">
         <is>
-          <t>bankslyonbotanical</t>
+          <t>letterfest</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -3778,30 +3778,30 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/relaxation-gift-set</t>
+          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-alphabet-zoo-story-book</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=971121&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>786480</t>
+          <t>976980</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Sterling Silver Family Birthstones Sliding Bracelet</t>
+          <t>Personalised Wedding Or Anniversary Flower Pot</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>letterfest</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -3809,30 +3809,30 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-family-birthstone-bracelet</t>
+          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-anniversary-flower-pot</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786480&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>793949</t>
+          <t>984075</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Personalised Happy Birthday Keepsake Book</t>
+          <t>Personalised Large Green Garden Welly Boots Planter</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -3840,401 +3840,72 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/personalised-happy-birthday-keepsake-book</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-little-gardener-s-welly-boot-planters</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=793949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984075&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>801933</t>
+          <t>989575</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Personalised Pull Out Photo Album Token Gift</t>
+          <t>Strong Woman Sterling Silver Morse Code Chain Bracelet</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/strong-woman-sterling-silver-morse-code-chain-bracelet</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=989575&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>828426</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr"/>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+        </is>
+      </c>
       <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
       <c r="E112" t="n">
         <v>2</v>
       </c>
-      <c r="F112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
+        </is>
+      </c>
       <c r="G112" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>848232</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Personalised 60 Th Birthday Book 'Memory Lane'</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>lucysworld</t>
-        </is>
-      </c>
-      <c r="E113" t="n">
-        <v>2</v>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-60th-birthday-book-memory-lane</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=848232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>857942</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E114" t="n">
-        <v>2</v>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>860698</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Personalised 70th Birthday Book 'Memory Lane'</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>lucysworld</t>
-        </is>
-      </c>
-      <c r="E115" t="n">
-        <v>2</v>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-70th-birthday-book-memory-lane</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860698&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>874166</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Graduation Cap Silver Charm Bracelet Gift For Her</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>lhgdesigns</t>
-        </is>
-      </c>
-      <c r="E116" t="n">
-        <v>2</v>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lhgdesigns/product/graduation-cap-silver-charm-bracelet-gift-for-her</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=874166&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>903313</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Mother And Child Birthstone Charm Necklace</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>joybycorrinesmith</t>
-        </is>
-      </c>
-      <c r="E117" t="n">
-        <v>2</v>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/mother-and-child-birthstone-charm-necklace</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903313&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>90344</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Personalised Rag Doll</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>thealphabetgiftshop</t>
-        </is>
-      </c>
-      <c r="E118" t="n">
-        <v>2</v>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-rag-doll</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=90344&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>923932</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Happy Birthday Celebration Hamper</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>lottieshaws</t>
-        </is>
-      </c>
-      <c r="E119" t="n">
-        <v>2</v>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lottieshaws/product/birthday-hamper-box</t>
-        </is>
-      </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=923932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>930044</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>'Floral Summer' Mixed Pack Of Ten Greeting Cards</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>faysstudio</t>
-        </is>
-      </c>
-      <c r="E120" t="n">
-        <v>2</v>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/faysstudio/product/floral-summer-pack-of-ten-greeting-cards</t>
-        </is>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=930044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>950712</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Elephant Good Fortune Foil Scarf</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E121" t="n">
-        <v>2</v>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/elephant-raised-trunk-good-fortune-scarf-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950712&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>984487</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>Personalised Men's Woven Vegan Bracelet With Clasp</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>lisaangeljewellery</t>
-        </is>
-      </c>
-      <c r="E122" t="n">
-        <v>2</v>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-men-s-woven-vegan-bracelet-with-clasp</t>
-        </is>
-      </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>999592</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E123" t="n">
-        <v>2</v>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G123" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-08-04T01:55:42Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1035825</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Treat Pot For Him</t>
+          <t>Map Engagement Card</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,123 +492,123 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-father-s-day-treat-pot</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1047473</t>
+          <t>1037522</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Brilliant Teacher Notebook Journal</t>
+          <t>Graduation Map Card</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>betsybenn</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/betsybenn/product/personalised-brilliant-teacher-notebook-journal</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047473&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1057279</t>
+          <t>1061155</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Personalised Wooden Bamboo Pen</t>
+          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>giftsonline4u</t>
+          <t>daisymaison</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/giftsonline4u/product/personalised-wooden-bamboo-pen</t>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1057279&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1061155</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1069900</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Personalised Hand Drawn Wedding Venue Illustration</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>placesandspacesartco</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/placesandspacesartco/product/personalised-wedding-venue-illustration</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1069900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1076937</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Natural Flowers Summer Door Wreath</t>
+          <t>Dandelion Sketch Scarf</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,61 +647,61 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/dandelion-sketch-scarf</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076937&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1084722</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Wedding Gift Personalised Map Print Of Wedding Venue</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>monoscape</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/monoscape/product/wedding-gift-personalised-map-print-of-wedding-venue</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1084722&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1104597</t>
+          <t>1176405</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Vintage Copper Garden Bucket Planter</t>
+          <t>Personalised Christening Pocket Watch Celtic Cross</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>giftsonline4u</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,61 +709,61 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-vintage-copper-garden-bucket-planter</t>
+          <t>https://www.notonthehighstreet.com/giftsonline4u/product/personalised-christening-pocket-watch-celtic-cross</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1104597&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1176405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1107283</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Embroidered Initials Washbag</t>
+          <t>Personalised Birth Flower Stoneware Mug</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-embroidered-initials-washbag</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1107283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1182421</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Wedding Day Floral Magnet And Card</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>oliviamorgan</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,92 +771,92 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-wedding-day-floral-magnet-and-card</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1158505</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalised Graduation Map Gift, University Print</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>hooddesignsco</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-graduation-map-gift-university-print</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158505&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1171326</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dog Breed ID Tag Personalised Realistic Illustrations</t>
+          <t>Dog And Owner Personalised Walking Socks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>hoobynoo</t>
+          <t>alphabetinteriors</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hoobynoo/product/dog-breed-id-tag-personalised-realistic-illustrations</t>
+          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1171326&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Stoneware Mug</t>
+          <t>Christening Keepsake Gift Book Personalised For Baby</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>mymagicname</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -864,61 +864,61 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
+          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1182639</t>
+          <t>1211012</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Personalised Wedding Gift Wallet, Money Or Voucher Envelope</t>
+          <t>Sterling Silver Bold Coil Drop Earrings</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>bubblebusinessuk</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bubblebusinessuk/product/wedding-gift-flowers-in-a-balloon</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182639&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1190985</t>
+          <t>1234030</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Personalised Birth Month Flower Printed Can Glass</t>
+          <t>Personalised Sterling Silver Baltic Amber Bumble Bee Necklace</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>propergoose</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -926,30 +926,30 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/propergoose/product/personalised-birth-month-flower-printed-can-glass</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1194413</t>
+          <t>1246450</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Thank You Teacher Personalised Coloured Enamel Mug</t>
+          <t>Weekly Positivity Floral Desktop Flip Chart</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -957,61 +957,61 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/thank-you-teacher-personalised-coloured-enamel-mug</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1194413&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Large Tropical Leaf Scarf</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1210491</t>
+          <t>1272569</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Silver Plated Star Friendship Bracelet</t>
+          <t>Personalised 21st Birthday Bracelet With Heart</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>letterboxlove</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1019,30 +1019,30 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterboxlove/product/silver-friendship-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-birthday-bracelet</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210491&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1281098</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sterling Silver Twist Ball Dangly Earrings</t>
+          <t>Oak Slot Doorstop - Handmade Windproof Holder For Patio, Bi Fold And External Doors</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>naturalwoodcompany</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,30 +1050,30 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
+          <t>https://www.notonthehighstreet.com/naturalwoodcompany/product/oak-door-stop-with-a-slot-for-patio-doors</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1281098&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1238724</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Mug 'Good Luck Finding Better Colleagues'</t>
+          <t>Personalised Vintage Map Picture With Stitched Heart</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>arrowgiftco</t>
+          <t>poshtottydesignscreates</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1081,30 +1081,30 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/good-luck-personalised-mug</t>
+          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1238724&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1245502</t>
+          <t>1305389</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Daisy April Birth Flower Earrings</t>
+          <t>Huggie Hoop Earrings Sterling Silver Everyday Jewellery</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>onnanokojewellery</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1112,61 +1112,61 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
+          <t>https://www.notonthehighstreet.com/onnanokojewellery/product/huggie-hoop-earrings-sterling-silver-everyday-jewellery</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305389&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1246450</t>
+          <t>1309827</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Weekly Positivity Floral Desktop Flip Chart</t>
+          <t>Personalised Baby Dungarees - Embroidered Baby Romper Gift For Newborn, Boy Or Girl</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>cublifeclothing</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
+          <t>https://www.notonthehighstreet.com/cublifeclothing/product/personalised-baby-dungarees-romper-embroidered</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1247679</t>
+          <t>1317092</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Silver Plated Anxiety Fidget Bracelet Adjustable Worry School Exam Gcse Sats</t>
+          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>wishuponastring</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1174,61 +1174,61 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wishuponastring/product/925-sterling-silver-anxiety-fidget-bracelet-adjustable</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1247679&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1248592</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Cross Necklace</t>
+          <t>Sheep Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-plain-cross-pendant</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1248592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1260374</t>
+          <t>1339169</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sterling Silver Blue Forget Me Not Flower Stud Earrings</t>
+          <t>Women's Rfid Secure Large Blue Leather Purse</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>handbagsdirect2u</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1236,30 +1236,30 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-rfid-secure-large-blue-leather-purse</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1339169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1264171</t>
+          <t>1340011</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Personalised Leather Notebook Lined</t>
+          <t>Personalised Scottish Highland Brown Cow, Gift Boxed</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>hotdot</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1267,61 +1267,61 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-leather-notebook-a5-lined</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/personalised-highland-brown-cow-free-delivery</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1340011&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1271268</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Personalised Best Friends Pebble Picture</t>
+          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friendship-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1272901</t>
+          <t>1350143</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Mens Sterling Silver Flat Curb Bracelet</t>
+          <t>'Bean Married' Personalised 2nd Anniversary Tea Towel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>arrowgiftco</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,92 +1329,92 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/4mm-sterling-silver-flat-curb-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/bean-married-personalised-2nd-anniversary-tea-towel</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1276718</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Metallic Personalised Record Song Lyrics Print</t>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>spincollective</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/spincollective/product/metallic-personalised-record-song-lyrics-print</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1278602</t>
+          <t>1357472</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Birth Flower Birthday Gift Terracotta Plant Pot</t>
+          <t>Pink Heart Hoop Earrings</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>rabal</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birth-flower-personalised-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/rabal/product/pink-heart-hoop-valentines-day</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357472&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1290822</t>
+          <t>1359483</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Personalised Wedding Anniversary Gift Candle Holder Set</t>
+          <t>Personalised Open Flat Washbag</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>mirrorin</t>
+          <t>thealphabetgiftshop</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1422,30 +1422,30 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-anniversary-candle-holder-set</t>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1305083</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Personalised Striped Tote Bag</t>
+          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1453,61 +1453,61 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-striped-tote-bag</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1317092</t>
+          <t>1382559</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
+          <t>Sterling Silver Paua Shell Star Stud Earrings</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/mini-sterling-silver-blue-star-stud-earrings</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1382559&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1319990</t>
+          <t>1384307</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Heart Cocktail Glass With Personalised Metal Straw</t>
+          <t>Personalised Silver Plated Photo Frame -5x7</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>myleelondon</t>
+          <t>loveloxlockets</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,92 +1515,92 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myleelondon/product/heart-cocktail-glass</t>
+          <t>https://www.notonthehighstreet.com/loveloxlockets/product/personalised-silver-plated-photo-frame-5x7</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1319990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1384307&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1320832</t>
+          <t>1392422</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sterling Silver Name Necklace</t>
+          <t>Personalised Seven Tea Tea Towel 70th Birthday Gift</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>potiega</t>
+          <t>afewhometruths</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/potiega/product/sterling-silver-name-necklace</t>
+          <t>https://www.notonthehighstreet.com/afewhometruths/product/personalised-seven-tea-tea-towel-70th-birthday-present</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392422&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1396397</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1399911</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fabric Name Peekaboo Memory Box</t>
+          <t>Personalised Initials Wedding Card</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>modocreative</t>
+          <t>momoandboo</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,92 +1608,92 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/modocreative/product/fabric-peekaboo-keepsake-box</t>
+          <t>https://www.notonthehighstreet.com/momoandboo/product/personalised-initials-wedding-card</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1399911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1400456</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Personalised Wedding Anniversary Coaster</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-wedding-anniversary-coaster</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1354859</t>
+          <t>1415152</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ceramic Little Book Of Flowers Vase</t>
+          <t>Personalised 60th Birthday Milestone Newspaper Book</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>historicnewspapers</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/ceramic-little-book-of-flowers-vase</t>
+          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-60th-birthday-milestone-newspaper-book</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354859&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415152&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1357569</t>
+          <t>1415175</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Swarovski Crystal Single Row Choker Necklace</t>
+          <t>Personalised 80th Birthday Milestone Newspaper Book</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>dynastylondon</t>
+          <t>historicnewspapers</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,61 +1701,61 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dynastylondon/product/swarovski-crystal-single-row-choker-necklace</t>
+          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-80th-birthday-milestone-newspaper-book</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415175&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1362911</t>
+          <t>1434628</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Personalised Brownie Box</t>
+          <t>Women's Genuine Leather Shopper, Handbag, Shoulder Bag</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>rubythecakeartist</t>
+          <t>handbagsdirect2u</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
+          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-genuine-leather-shopper-handbag-shoulder-bag</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1456123</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
+          <t>Women's White Cotton Nightdress Luxury Embroidered Juliet Chemise</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>iconiccoasters</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1763,30 +1763,30 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-luxury-embroidered-juliet-chemise</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456123&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1372560</t>
+          <t>145704</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Personalised Tractor Keepsake Birthday Card</t>
+          <t>Personalised Storyteller Bracelet Or Necklace</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>noordinarygiftcompany</t>
+          <t>sallyclayjewellerydesign</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1794,92 +1794,92 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/personalised-tractor-keepsake-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/sallyclayjewellerydesign/product/personalised-your-story-bracelet-necklace</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=145704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1387361</t>
+          <t>1465032</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
+          <t>Sterling Silver Art Deco Inspired Cz Crawler Earrings</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-art-deco-inspired-cz-crawler-earrings</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1396397</t>
+          <t>1475946</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
+          <t>Personalised New Baby Grandson, Nephew Any Relation Greeting Card</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>kittyandfin</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
+          <t>https://www.notonthehighstreet.com/kittyandfin/product/personalised-new-baby-grandson-nephew-any-relation-greeting-card</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1402097</t>
+          <t>1485292</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Puff Heart Bracelet With Heart Charm</t>
+          <t>Personalised 60th Birthday Card For Special Friend</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>acecards</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1887,30 +1887,30 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/puff-heart-bracelet-with-heart-charm</t>
+          <t>https://www.notonthehighstreet.com/acecards/product/personalised-60th-birthday-card-for-special-friend</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402097&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1485292&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1412559</t>
+          <t>1486376</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Personalised Teacher Gift - Thank You Flower Vase</t>
+          <t>Teacher Thank You Candle - 'Difference Maker' Definition</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>laurastanleydesigns</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1918,61 +1918,61 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-teacher-gift-thank-you-flower-vase</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/teacher-thank-you-candle-difference-maker-definition</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1412559&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486376&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1416296</t>
+          <t>1493887</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Women's White Cotton Victorian Short Sleeve Nightdress Front Panel</t>
+          <t>Personalised Football Shirt Can Cooler</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/white-cotton-victorian-short-sleeve-nightdress-front-panel</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-football-shirt-can-cooler</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416296&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1493887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1419917</t>
+          <t>1504689</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Personalised Champagne Retirement Card</t>
+          <t>You Are Amazing Silver Plated Bracelet Gift</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>wholeinthemiddle</t>
+          <t>withlovejewellerylimited</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1980,24 +1980,24 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/personalised-champagne-retirement-card</t>
+          <t>https://www.notonthehighstreet.com/withlovejewellerylimited/product/silver-plated-you-are-amazing-bracelet</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419917&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1504689&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1420726</t>
+          <t>1523668</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Personalised Metal Music Sheet Page Holder</t>
+          <t>Personalised Couples 10th Tin Anniversary Street Sign</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -2007,65 +2007,65 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-music-sheet-page-holder</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-10th-tin-anniversary-street-sign</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523668&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1422513</t>
+          <t>255970</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sterling Silver Paw Print Adjustable Ring</t>
+          <t>White Sleeveless Cotton Nightdress Lizzie</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>feelsilkstudio</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/feelsilkstudio/product/sterling-silver-paw-print-adjustable-ring</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1422513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1435032</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
+          <t>Rose Bouquet Personalised Card</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>karriebarroncards</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2073,61 +2073,61 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1443868</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Silver Jade Gemstone Acorn Earrings</t>
+          <t>Personalised Metal Street Sign</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>silkpursesowsear</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/silver-gemstone-acorn-earrings</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1486088</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Janhvi The Small Quacking Duck Wire Garden Ornament</t>
+          <t>Sterling Silver April Shower Drop Earrings</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>paperhigh</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2135,30 +2135,30 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/paperhigh/product/janhvi-the-small-quacking-duck-wire-garden-ornament</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486088&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1486376</t>
+          <t>355476</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Teacher Thank You Candle - 'Difference Maker' Definition</t>
+          <t>Vintage Cast Iron Heart Shaped Bird Seed Feeder</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>selections</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2166,61 +2166,61 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/teacher-thank-you-candle-difference-maker-definition</t>
+          <t>https://www.notonthehighstreet.com/selections/product/decorative-cow-solar-light-ornament</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486376&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1496888</t>
+          <t>412675</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Petsentials Super Clumping Cat Litter 10 L</t>
+          <t>Literary Paper 1st Anniversary Rose</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>noahsark</t>
+          <t>cot2totandbeyond</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-10l</t>
+          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496888&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1498809</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>New Home Heart Shaped Ceramic Keepsake Gift</t>
+          <t>Peridot Quartz Drop Earrings</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>pinkstrawberry</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2228,30 +2228,30 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pinkstrawberry/product/new-home-heart-shaped-ceramic-keepsake-gift</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1499827</t>
+          <t>427505</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Personalised Cartoon Anniversary And Birthday Card</t>
+          <t>Seriously Good Large Hamper</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>lottieshaws</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-3d-animated-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/lottieshaws/product/fabulous-treat-hamper</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=427505&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1500474</t>
+          <t>439136</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Personalised Big Sister Bracelet</t>
+          <t>70th Birthday Silver Bangle</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>nameitwhatyoulike</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,61 +2290,61 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nameitwhatyoulike/product/personalised-big-sister-charm-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/70th-birthday-silver-bangle</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500474&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=439136&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>thelyndoncompany</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1507466</t>
+          <t>486000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025 Graduation Keyring, Personalised Gift Keepsake</t>
+          <t>'Baby Crap... I Used To Be Fun' Tote Bag</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>wildwarestudio</t>
+          <t>lolaandgilbertlondon</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2352,123 +2352,123 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wildwarestudio/product/2025-graduation-keyring-personalised-gift-keepsake</t>
+          <t>https://www.notonthehighstreet.com/lolaandgilbertlondon/product/baby-crap-i-used-to-be-fun-tote-bag</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1507466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1508460</t>
+          <t>597661</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Personalised Saturday Night Snacks Bowl</t>
+          <t>Personalised 'Classroom Creatures' Teacher's Mug</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>thisisnessie</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-saturday-night-snacks-bowl</t>
+          <t>https://www.notonthehighstreet.com/thisisnessie/product/personalised-teacher-s-busy-bees-mug</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=597661&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1512669</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Personalised Teacher Thank You Mug</t>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>arrowgiftco</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-teacher-thank-you-mug</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512669&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1523637</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Pink Candyfloss Marshmallow</t>
+          <t>Friendship Knot Bangle</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>scouseafricansweetery</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/scouseafricansweetery/product/pink-candyfloss-marshmallow</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523637&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>152410</t>
+          <t>643101</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Personalised Treasured Location Print</t>
+          <t>'A New Chapter Begins...' Bookmark</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>brambler</t>
+          <t>kutuu</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2476,30 +2476,30 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/brambler/product/giclee-bespoke-treasured-location</t>
+          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=152410&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>177216</t>
+          <t>689351</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Baby Hand And Foot Inkless Print Kit</t>
+          <t>Family Birthstone Link Necklace</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>elizabethjane</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2507,216 +2507,216 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/elizabethjane/product/baby-hand-and-foot-inkless-print</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-necklace</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=177216&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>298443</t>
+          <t>706756</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Personalised Metal Street Sign</t>
+          <t>Personalised Leather Wash Bag</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>paperhigh</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
+          <t>https://www.notonthehighstreet.com/paperhigh/product/handmade-leather-wash-bag</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=706756&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>764045</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sterling Silver April Shower Drop Earrings</t>
+          <t>Personalised Birthstone Disc Stretch Bracelet</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Literary Paper 1st Anniversary Rose</t>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>cot2totandbeyond</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>770318</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Personalised 21st Necklace With Birthstone</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>433785</t>
+          <t>770939</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>White Cotton Short Sleeve Nightdress 18th Century</t>
+          <t>Metallic Bee Print Scarf</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/18th-century-cotton-nightdress</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-bee-print-scarf</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770939&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>446429</t>
+          <t>779785</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Personalised Teacher Notebook Journal</t>
+          <t>Metallic Silver Bee Scarf</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>catsprintshop</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/catsprintshop/product/personalised-teacher-notebook-journal</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-silver-bee-scarf</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=446429&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=779785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Aquamarine Quartz, Moonstone And Pearl Earrings</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2724,61 +2724,61 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/aquamarine-quartz-moonstone-and-pearl-earrings</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>798716</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>Personalised Wool Mix Poncho</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-lightweight-wool-mix-summer-poncho</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=798716&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>488356</t>
+          <t>801933</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Sterling Silver Secret Message Ring</t>
+          <t>Personalised Pull Out Photo Album Token Gift</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2786,61 +2786,61 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>512405</t>
+          <t>824634</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Set Of Three Cat Socks In A Gift Box</t>
+          <t>Personalised Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/set-of-three-cat-socks-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>520238</t>
+          <t>837190</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Silver St Christopher Double Heart Charm Necklace</t>
+          <t>Dinosaur Glow In The Dark T Shirt</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>hurleyburleyjunior</t>
+          <t>glowgalaxyart</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2848,30 +2848,30 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/silver-st-christopher-double-heart-charm-necklace</t>
+          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=520238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>607975</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Mineral Bath Infusions Gift Collection</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>bankslyonbotanical</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2879,123 +2879,123 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/mineral-bath-infusions-gift-collection</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
+          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle</t>
+          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>643101</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>'A New Chapter Begins...' Bookmark</t>
+          <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>kutuu</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>695129</t>
+          <t>886944</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Personalised Vintage Garden Bird Dish</t>
+          <t>Personalised Leather And Silver St Christopher Bracelet</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>hurleyburleyman</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3003,92 +3003,92 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/love-birds-6th-anniverary-iron-hanging-heart-bird-dish</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>707031</t>
+          <t>905169</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Graduation Charm Bracelet</t>
+          <t>Birthstone Bracelet</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/graduation-charm-bracelet</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=707031&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>722492</t>
+          <t>915034</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Personalised Graduation Gift City Print</t>
+          <t>Personalised Wedding Day / First Anniversary Card</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>handmadebytessagalloway</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handmadebytessagalloway/product/personalised-graduation-gift-city-print</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=722492&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>760714</t>
+          <t>920040</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Personalised Name Bottle Opener</t>
+          <t>Personalised Snack Bowl</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -3096,92 +3096,92 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-name-bottle-opener</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-snack-bowl</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760714&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>764045</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Personalised Birthstone Disc Stretch Bracelet</t>
+          <t>Dandelion Foil Birthday Gift Scarf</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>770939</t>
+          <t>940836</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Metallic Bee Print Scarf</t>
+          <t>'Rainbow Floral' Mixed Pack Of Ten Birthday Cards</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>faysstudio</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-bee-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/faysstudio/product/rainbow-floral-mixed-pack-of-ten-birthday-cards</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770939&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=940836&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>772232</t>
+          <t>944875</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Personalised Moon And Star Necklace</t>
+          <t>Toe Ring Hammered Texture</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>serin</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -3189,123 +3189,123 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/moon-and-star-necklace-with-personalised-box</t>
+          <t>https://www.notonthehighstreet.com/serin/product/toe-ring-hammered-texture</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=772232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944875&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>773419</t>
+          <t>948800</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Gunmetal Pearl And Cashmere Blend Scarf</t>
+          <t>Large Butterfly Print Scarf</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/gun-metal-pearl-cashmere-shawl</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=773419&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>950732</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
+          <t>Dragonfly Foil Scarf Letterbox Gift</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>797444</t>
+          <t>968713</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Personalised Graduation Necklace</t>
+          <t>Personalised Birth Flower Birthstone Keyring</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-graduation-necklace</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-keyring</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=797444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>828426</t>
+          <t>999592</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Personalised 'Promises To You' Book For Godchild</t>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>lucysworld</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -3313,601 +3313,43 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-promises-to-you-book-for-godchild</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>866983</t>
+          <t>999606</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
+          <t>Personalised Chocolate Treats Bowl</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-chocolate-treats-bowl</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>868202</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
-        <v>2</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>872048</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Sterling Silver Dangly Crescent Earrings</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>marthajackson</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
-        <v>2</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-crescent-drop-earrings</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872048&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Personalised Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>theforestandco</t>
-        </is>
-      </c>
-      <c r="E97" t="n">
-        <v>4</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>882796</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Stainforth Large Blue Ceramic Jug Vase</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>dibor</t>
-        </is>
-      </c>
-      <c r="E98" t="n">
-        <v>3</v>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/stainforth-large-blue-ceramic-ribbed-jug</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>893548</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Personalised Luxury Leather Two Part Wash Bag</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>hurleyburleyman</t>
-        </is>
-      </c>
-      <c r="E99" t="n">
-        <v>2</v>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-luxury-leather-two-part-washbag</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=893548&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>903313</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Mother And Child Birthstone Charm Necklace</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>joybycorrinesmith</t>
-        </is>
-      </c>
-      <c r="E100" t="n">
-        <v>2</v>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/mother-and-child-birthstone-charm-necklace</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903313&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>905169</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Birthstone Bracelet</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>attic</t>
-        </is>
-      </c>
-      <c r="E101" t="n">
-        <v>2</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>907471</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Personalised Motorhome Travel Journal Notebook</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>oakdenedesigns</t>
-        </is>
-      </c>
-      <c r="E102" t="n">
-        <v>2</v>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-motorhome-travel-journal-notebook</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=907471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>917605</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Personalised Couples Large Matchbox</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>oakdenedesigns</t>
-        </is>
-      </c>
-      <c r="E103" t="n">
-        <v>2</v>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>918435</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Family Birth Month Flower Print</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>vintagedesignsreborn</t>
-        </is>
-      </c>
-      <c r="E104" t="n">
-        <v>2</v>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/vintagedesignsreborn/product/family-birth-month-flower-print</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=918435&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>934374</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Personalised Luxury Extra Deep A4 Blush Pink Gift Box</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>dibor</t>
-        </is>
-      </c>
-      <c r="E105" t="n">
-        <v>2</v>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/hug-in-a-box-personalised-luxury-gift-box</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=934374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>948800</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Large Butterfly Print Scarf</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E106" t="n">
-        <v>2</v>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>950732</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Dragonfly Foil Scarf Letterbox Gift</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E107" t="n">
-        <v>4</v>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>971121</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Personalised Alphabet Zoo Story Book</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>letterfest</t>
-        </is>
-      </c>
-      <c r="E108" t="n">
-        <v>2</v>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-alphabet-zoo-story-book</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=971121&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>976980</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Or Anniversary Flower Pot</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>letterfest</t>
-        </is>
-      </c>
-      <c r="E109" t="n">
-        <v>2</v>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-anniversary-flower-pot</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>984075</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Personalised Large Green Garden Welly Boots Planter</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>dibor</t>
-        </is>
-      </c>
-      <c r="E110" t="n">
-        <v>2</v>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-little-gardener-s-welly-boot-planters</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=984075&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>989575</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Strong Woman Sterling Silver Morse Code Chain Bracelet</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>charlieboots</t>
-        </is>
-      </c>
-      <c r="E111" t="n">
-        <v>3</v>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/strong-woman-sterling-silver-morse-code-chain-bracelet</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=989575&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>999592</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E112" t="n">
-        <v>2</v>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-08-11T01:40:54Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1006901</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Map Engagement Card</t>
+          <t>Abstract Flower Print Scarf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,24 +492,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/valentines-abstract-flowers-scarf</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1006901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1037522</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Graduation Map Card</t>
+          <t>Map Engagement Card</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/graduation-map-card</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1037522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1061155</t>
+          <t>1035825</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
+          <t>Personalised Treat Pot For Him</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,123 +554,123 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-father-s-day-treat-pot</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Star Sign Constellation Earrings Studs</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1069900</t>
+          <t>1050164</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Hand Drawn Wedding Venue Illustration</t>
+          <t>Personalised Welly Plant Pot Gift</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>placesandspacesartco</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/placesandspacesartco/product/personalised-wedding-venue-illustration</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-welly-plant-pot-thank-you-teacher-gift</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1069900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1050164&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1076937</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dandelion Sketch Scarf</t>
+          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/dandelion-sketch-scarf</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076937&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1067493</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Natural Flowers Summer Door Wreath</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,92 +678,92 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1176405</t>
+          <t>1107283</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Christening Pocket Watch Celtic Cross</t>
+          <t>Personalised Embroidered Initials Washbag</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>giftsonline4u</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/giftsonline4u/product/personalised-christening-pocket-watch-celtic-cross</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-embroidered-initials-washbag</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1176405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1107283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1112053</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Stoneware Mug</t>
+          <t>Personalised 1965 60th Birthday Sixpence Necklace</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/personalised-1961-60th-birthday-sixpence-necklace</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1112053&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1182421</t>
+          <t>1119514</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Wedding Day Floral Magnet And Card</t>
+          <t>Personalised Golf Set With Golf Balls And Tees</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>oliviamorgan</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,216 +771,216 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oliviamorgan/product/personalised-wedding-day-floral-magnet-and-card</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-golf-set-with-golf-balls-and-tees</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1182421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1119514&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1158875</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Wedding Iced Biscuit Box</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>julietstallwoodcakesandbiscuits</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/julietstallwoodcakesandbiscuits/product/wedding-iced-biscuit-gift-box</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158875&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dog And Owner Personalised Walking Socks</t>
+          <t>Personalised Women's Technology Travel Case Gift</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>alphabetinteriors</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Christening Keepsake Gift Book Personalised For Baby</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>mymagicname</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1211012</t>
+          <t>1205131</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sterling Silver Bold Coil Drop Earrings</t>
+          <t>Wildflower Seed Balls For Bees Pack Of Three</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>seedball</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/seedball/product/bee-wildflower-seed-ball-set-of-three-packets</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1234030</t>
+          <t>1211012</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Baltic Amber Bumble Bee Necklace</t>
+          <t>Sterling Silver Bold Coil Drop Earrings</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1246450</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Weekly Positivity Floral Desktop Flip Chart</t>
+          <t>Sterling Silver Twist Ball Dangly Earrings</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/weekly-positivity-floral-desktop-flip-chart</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1229228</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Large Tropical Leaf Scarf</t>
+          <t>Personalised Entwined Wedding Rings Card</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>wholeinthemiddle</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -988,61 +988,61 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
+          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/personalised-entwined-wedding-rings-card</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1272569</t>
+          <t>1234030</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Personalised 21st Birthday Bracelet With Heart</t>
+          <t>Personalised Sterling Silver Amber Bee Pendant Necklace</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-birthday-bracelet</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1281098</t>
+          <t>1246964</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Oak Slot Doorstop - Handmade Windproof Holder For Patio, Bi Fold And External Doors</t>
+          <t>Floating Petal Print Scarf</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>naturalwoodcompany</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,61 +1050,61 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/naturalwoodcompany/product/oak-door-stop-with-a-slot-for-patio-doors</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/floating-petal-print-scarf</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1281098&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Vintage Map Picture With Stitched Heart</t>
+          <t>Large Tropical Leaf Scarf</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>poshtottydesignscreates</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1305389</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Huggie Hoop Earrings Sterling Silver Everyday Jewellery</t>
+          <t>Personalised Birth Year Football Club Print</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>onnanokojewellery</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1112,30 +1112,30 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/onnanokojewellery/product/huggie-hoop-earrings-sterling-silver-everyday-jewellery</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-birth-year-football-club-print</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305389&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1309827</t>
+          <t>1260374</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Personalised Baby Dungarees - Embroidered Baby Romper Gift For Newborn, Boy Or Girl</t>
+          <t>Sterling Silver Blue Forget Me Not Stud Earrings - 5mm</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>cublifeclothing</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1143,24 +1143,24 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cublifeclothing/product/personalised-baby-dungarees-romper-embroidered</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1317092</t>
+          <t>1261865</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fuck Cancer Sterling Silver Morse Code Chain Bracelet</t>
+          <t>60th Birthday Vintage Sixpence Locket Necklace</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1170,96 +1170,96 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-chain-bracelet</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/1963-60th-birthday-vintage-sixpence-locket-necklace</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1317092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1261865&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1271268</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+          <t>Personalised Best Friends Pebble Picture</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friendship-pebble-picture</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1339169</t>
+          <t>1277784</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Women's Rfid Secure Large Blue Leather Purse</t>
+          <t>Personalised Sterling Silver St Christopher Necklace</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>handbagsdirect2u</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-rfid-secure-large-blue-leather-purse</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-large-st-christopher-necklace</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1339169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1340011</t>
+          <t>1278602</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Personalised Scottish Highland Brown Cow, Gift Boxed</t>
+          <t>Birth Flower Birthday Gift Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1267,61 +1267,61 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/personalised-highland-brown-cow-free-delivery</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birth-flower-personalised-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1340011&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
+          <t>Personalised Vintage Map Picture With Stitched Heart</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>poshtottydesignscreates</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
+          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1350143</t>
+          <t>1298104</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>'Bean Married' Personalised 2nd Anniversary Tea Towel</t>
+          <t>Personalised Lego Brick Landscape Photo Block Puzzle</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>arrowgiftco</t>
+          <t>brickbybrick23</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,61 +1329,61 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/bean-married-personalised-2nd-anniversary-tea-towel</t>
+          <t>https://www.notonthehighstreet.com/brickbybrick23/product/personalised-landscape-photo-block-puzzle</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1298104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1313730</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Highland Cow Cream Cushion, Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/highland-cow-sofa-tidy-organiser-keep-your-remote-safe</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1357472</t>
+          <t>1330966</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Pink Heart Hoop Earrings</t>
+          <t>Handmade Personalised Leather Curved Corner Bookmark</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>rabal</t>
+          <t>parkerandco</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1391,61 +1391,61 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/rabal/product/pink-heart-hoop-valentines-day</t>
+          <t>https://www.notonthehighstreet.com/parkerandco/product/handmade-personalised-leather-curved-corner-bookmark</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1357472&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1359483</t>
+          <t>133151</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Personalised Open Flat Washbag</t>
+          <t>Sheep Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>thealphabetgiftshop</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-open-flat-washbag</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1359483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>1337443</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
+          <t>Genuine Leather Small Shoulder Bag, Cross Body Bag</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>handbagsdirect2u</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1453,61 +1453,61 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
+          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/genuine-leather-small-shoulder-bag-cross-body-bag</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1337443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1382559</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sterling Silver Paua Shell Star Stud Earrings</t>
+          <t>No Words Just Hugs Candle Gift Set</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/mini-sterling-silver-blue-star-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/no-words-just-hugs-candle-gift-set</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1382559&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1384307</t>
+          <t>1345852</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Personalised Silver Plated Photo Frame -5x7</t>
+          <t>Personalised Birthday Newspaper Book Daily Telegraph Edition</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>loveloxlockets</t>
+          <t>historicnewspapers</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,92 +1515,92 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/loveloxlockets/product/personalised-silver-plated-photo-frame-5x7</t>
+          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-telegraph-birthday-newspaper-book</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1384307&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345852&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1392422</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Personalised Seven Tea Tea Towel 70th Birthday Gift</t>
+          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>afewhometruths</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/afewhometruths/product/personalised-seven-tea-tea-towel-70th-birthday-present</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392422&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1396397</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
+          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>iconiccoasters</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
+          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1399911</t>
+          <t>1365394</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Personalised Initials Wedding Card</t>
+          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>momoandboo</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,30 +1608,30 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/momoandboo/product/personalised-initials-wedding-card</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1399911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1400456</t>
+          <t>1376067</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Personalised Wedding Anniversary Coaster</t>
+          <t>Deluxe Relaxation And Wellness Pamper Gift Set</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>marigoldcharms</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1639,61 +1639,61 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-wedding-anniversary-coaster</t>
+          <t>https://www.notonthehighstreet.com/marigoldcharms/product/deluxe-relaxation-wellness-pamper-gift-set</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376067&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1415152</t>
+          <t>1381151</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Milestone Newspaper Book</t>
+          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>historicnewspapers</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-60th-birthday-milestone-newspaper-book</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415152&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1415175</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Personalised 80th Birthday Milestone Newspaper Book</t>
+          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>historicnewspapers</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,30 +1701,30 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-80th-birthday-milestone-newspaper-book</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415175&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1434628</t>
+          <t>1388105</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Women's Genuine Leather Shopper, Handbag, Shoulder Bag</t>
+          <t>Nursery Rhymes And Personalised Poems In Adorable Pink</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>handbagsdirect2u</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1732,61 +1732,61 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-genuine-leather-shopper-handbag-shoulder-bag</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-in-adorable-pink</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1388105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1456123</t>
+          <t>1392508</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Women's White Cotton Nightdress Luxury Embroidered Juliet Chemise</t>
+          <t>Personalised Six Tea Tea Towel 60th Birthday Gift</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>afewhometruths</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/women-s-white-cotton-nightdress-luxury-embroidered-juliet-chemise</t>
+          <t>https://www.notonthehighstreet.com/afewhometruths/product/personalised-six-tea-tea-towel-60th-birthday-present</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456123&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392508&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>145704</t>
+          <t>1396397</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Personalised Storyteller Bracelet Or Necklace</t>
+          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>sallyclayjewellerydesign</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1794,30 +1794,30 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sallyclayjewellerydesign/product/personalised-your-story-bracelet-necklace</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=145704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1465032</t>
+          <t>1397555</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sterling Silver Art Deco Inspired Cz Crawler Earrings</t>
+          <t>Opal Turquoise Wing Stud Earrings</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>silkpursesowsear</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1825,30 +1825,30 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-art-deco-inspired-cz-crawler-earrings</t>
+          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/opal-turquoise-wing-stud-earrings</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1465032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1475946</t>
+          <t>141541</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Personalised New Baby Grandson, Nephew Any Relation Greeting Card</t>
+          <t>Extra Large Personalised Leather Photo Album</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>kittyandfin</t>
+          <t>begolden</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1856,61 +1856,61 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/kittyandfin/product/personalised-new-baby-grandson-nephew-any-relation-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/begolden/product/large-leather-photo-album-gold</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=141541&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1485292</t>
+          <t>1416578</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Card For Special Friend</t>
+          <t>Personalised Bride Metal Shoe Tags</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>acecards</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/acecards/product/personalised-60th-birthday-card-for-special-friend</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-bride-metal-shoe-tags</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1485292&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1486376</t>
+          <t>1420726</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Teacher Thank You Candle - 'Difference Maker' Definition</t>
+          <t>Personalised Metal Music Sheet Page Holder</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1918,30 +1918,30 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/teacher-thank-you-candle-difference-maker-definition</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-music-sheet-page-holder</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486376&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1493887</t>
+          <t>1431321</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Personalised Football Shirt Can Cooler</t>
+          <t>Personalised Treasured Memories Photo Box</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1949,30 +1949,30 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-football-shirt-can-cooler</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-treasured-memories-photo-box</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1493887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431321&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1504689</t>
+          <t>1435032</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>You Are Amazing Silver Plated Bracelet Gift</t>
+          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>withlovejewellerylimited</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1980,30 +1980,30 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/withlovejewellerylimited/product/silver-plated-you-are-amazing-bracelet</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1504689&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1523668</t>
+          <t>1435766</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Personalised Couples 10th Tin Anniversary Street Sign</t>
+          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2011,61 +2011,61 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-10th-tin-anniversary-street-sign</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523668&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>255970</t>
+          <t>1447257</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>White Sleeveless Cotton Nightdress Lizzie</t>
+          <t>Sterling Silver August Birthstone Necklace - Peridot</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>thelittlekeepsakecompany</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
+          <t>https://www.notonthehighstreet.com/thelittlekeepsakecompany/product/sterling-silver-august-birthstone-necklace-peridot</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1447257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1448731</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Rose Bouquet Personalised Card</t>
+          <t>Personalised Russian Ring Necklace</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>karriebarroncards</t>
+          <t>abiza</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2073,61 +2073,61 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/abiza/product/personalised-russian-ring-necklace</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1448731&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>298443</t>
+          <t>1466041</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Personalised Metal Street Sign</t>
+          <t>Grow Your Own August Birth Flower Personalised Name Tin</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>alphabetgifting</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
+          <t>https://www.notonthehighstreet.com/alphabetgifting/product/grow-your-own-august-birth-flower-personalised-name-tin</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>1470941</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Sterling Silver April Shower Drop Earrings</t>
+          <t>Porcelain Bird Earrings French Vintage Charm</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2135,30 +2135,30 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>355476</t>
+          <t>1476087</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Vintage Cast Iron Heart Shaped Bird Seed Feeder</t>
+          <t>Spa Gift Box For Women</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>selections</t>
+          <t>hallby</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2166,92 +2166,92 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/selections/product/decorative-cow-solar-light-ornament</t>
+          <t>https://www.notonthehighstreet.com/hallby/product/spa-gift-box-for-women</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>1482117</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Literary Paper 1st Anniversary Rose</t>
+          <t>Hand Cream With Hibiscus Flowers Worth £20</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>cot2totandbeyond</t>
+          <t>upcircle</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
+          <t>https://www.notonthehighstreet.com/upcircle/product/hand-cream-with-hibiscus-flowers</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Birthday Gift Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birthday-gift-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>427505</t>
+          <t>1494976</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Seriously Good Large Hamper</t>
+          <t>Personalised Winthorpe Floral Wreath</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>lottieshaws</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lottieshaws/product/fabulous-treat-hamper</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=427505&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>439136</t>
+          <t>1496914</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>70th Birthday Silver Bangle</t>
+          <t>Petsentials Super Clumping Cat Litter Bag Active Carbon 20 L</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>noahsark</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,61 +2290,61 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/70th-birthday-silver-bangle</t>
+          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-bag-active-carbon</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=439136&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496914&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1497603</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>Personalised 60th Wedding Anniversary Gift - Diamond Heart Plaque</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/personalised-60th-anniversary-gift-diamond-heart-plaque</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497603&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>486000</t>
+          <t>1498337</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>'Baby Crap... I Used To Be Fun' Tote Bag</t>
+          <t>20th China Anniversary Heart Shaped Keepsake Ceramic Gift</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>lolaandgilbertlondon</t>
+          <t>pinkstrawberry</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2352,30 +2352,30 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lolaandgilbertlondon/product/baby-crap-i-used-to-be-fun-tote-bag</t>
+          <t>https://www.notonthehighstreet.com/pinkstrawberry/product/20th-china-anniversary-heart-shaped-keepsake-ceramic-gift</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=486000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>597661</t>
+          <t>1502932</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Personalised 'Classroom Creatures' Teacher's Mug</t>
+          <t>Christening Star Night Light</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>thisisnessie</t>
+          <t>looppa</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2383,92 +2383,92 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thisisnessie/product/personalised-teacher-s-busy-bees-mug</t>
+          <t>https://www.notonthehighstreet.com/looppa/product/christening-star-night-light</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=597661&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
+          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company Silver Small</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1508460</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle</t>
+          <t>Personalised Saturday Night Snacks Bowl</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-saturday-night-snacks-bowl</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>643101</t>
+          <t>255970</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>'A New Chapter Begins...' Bookmark</t>
+          <t>White Sleeveless Cotton Nightdress Lizzie</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>kutuu</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2476,30 +2476,30 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/kutuu/product/a-new-chapter-begins-bookmark</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>689351</t>
+          <t>258082</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Necklace</t>
+          <t>Personalised Tablet Stand In Oak Or Walnut</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>mijmoj</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2507,123 +2507,123 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-necklace</t>
+          <t>https://www.notonthehighstreet.com/mijmoj/product/oak-ipad-stand</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=258082&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>706756</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Personalised Leather Wash Bag</t>
+          <t>Sterling Silver April Shower Drop Earrings</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>paperhigh</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/paperhigh/product/handmade-leather-wash-bag</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=706756&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>764045</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Personalised Birthstone Disc Stretch Bracelet</t>
+          <t>Peridot Quartz Drop Earrings</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>451823</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+          <t>Personalised Hearts Wedding Card</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>eggbertanddaisy</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/eggbertanddaisy/product/personalised-hearts-wedding-card</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=451823&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>770318</t>
+          <t>46761</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Personalised 21st Necklace With Birthstone</t>
+          <t>Personalised Wooden Letter Name Train</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>wheniwasakid</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2631,61 +2631,61 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
+          <t>https://www.notonthehighstreet.com/wheniwasakid/product/handmade_wooden_alphabet_train</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=46761&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>770939</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Metallic Bee Print Scarf</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-bee-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770939&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>779785</t>
+          <t>482198</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Metallic Silver Bee Scarf</t>
+          <t>Busy Butterfly, Bee, Bug And Beneficial Insect Habitat</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>selections</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2693,30 +2693,30 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-silver-bee-scarf</t>
+          <t>https://www.notonthehighstreet.com/selections/product/pollinating-bee-nesting-log</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=779785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>488356</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
+          <t>Sterling Silver Secret Message Ring</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2724,30 +2724,30 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>798716</t>
+          <t>510573</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Personalised Wool Mix Poncho</t>
+          <t>Baby's Personalised Silver Christening Bracelet</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>hurleyburleyjunior</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2755,61 +2755,61 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/personalised-lightweight-wool-mix-summer-poncho</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/baby-s-personalised-sterling-silver-id-bracelet</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=798716&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=510573&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>801933</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Personalised Pull Out Photo Album Token Gift</t>
+          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>824634</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Personalised Birthstone And Initial Necklace</t>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2817,61 +2817,61 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-birthstone-and-initial-necklace</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>837190</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Dinosaur Glow In The Dark T Shirt</t>
+          <t>Friendship Knot Bangle</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>glowgalaxyart</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>711157</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
+          <t>Personalised Ceramic Plate Pearl Wedding Anniversary</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>melissachoroszewskaceramics</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2879,30 +2879,30 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
+          <t>https://www.notonthehighstreet.com/melissachoroszewskaceramics/product/personalised-ceramic-pearl-plate</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=711157&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>719727</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
+          <t>Skinny Thumb Ring</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2910,30 +2910,30 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/skinny-thumb-ring</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=719727&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>866983</t>
+          <t>760421</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
+          <t>Personalised Family Names Heart Necklace</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2941,30 +2941,30 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mixed-metal-heart-necklace</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>764045</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Scarf</t>
+          <t>Personalised Birthstone Disc Stretch Bracelet</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2972,30 +2972,30 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>886944</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Personalised Leather And Silver St Christopher Bracelet</t>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>hurleyburleyman</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3003,61 +3003,61 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Birthstone Bracelet</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>915034</t>
+          <t>798315</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Personalised Wedding Day / First Anniversary Card</t>
+          <t>Personalised Friendship Knot Bracelet</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3065,92 +3065,92 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-friendship-knot-bracelet</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=798315&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>920040</t>
+          <t>799432</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Personalised Snack Bowl</t>
+          <t>Personalised Football Ball Customise With Any Name</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>nameyourball</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-snack-bowl</t>
+          <t>https://www.notonthehighstreet.com/nameyourball/product/personalised-football-ball-style-v4</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=799432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>804990</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Dandelion Foil Birthday Gift Scarf</t>
+          <t>Personalised Enamel Snack Pot</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>940836</t>
+          <t>837190</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>'Rainbow Floral' Mixed Pack Of Ten Birthday Cards</t>
+          <t>Dinosaur Glow In The Dark T Shirt</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>faysstudio</t>
+          <t>glowgalaxyart</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -3158,30 +3158,30 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/faysstudio/product/rainbow-floral-mixed-pack-of-ten-birthday-cards</t>
+          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=940836&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>944875</t>
+          <t>837561</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Toe Ring Hammered Texture</t>
+          <t>Personalised Metal Shoe Tags</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>serin</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -3189,61 +3189,61 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/serin/product/toe-ring-hammered-texture</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-shoe-tags</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944875&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837561&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>948800</t>
+          <t>841037</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Large Butterfly Print Scarf</t>
+          <t>Personalised Leather Tool Belt For Dad</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>hotdot</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-tool-belt</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=841037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>950732</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Dragonfly Foil Scarf Letterbox Gift</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -3251,61 +3251,61 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>968713</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Birthstone Keyring</t>
+          <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-keyring</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>876946</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+          <t>Multi Stranded Magnet Bracelet</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>lovethelinks</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -3313,43 +3313,291 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
+          <t>https://www.notonthehighstreet.com/lovethelinks/product/three-coloured-stranded-bracelet</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>999606</t>
+          <t>898792</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Personalised Chocolate Treats Bowl</t>
+          <t>Personalised Quote Wire Word Art</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>greyfoxdesign</t>
         </is>
       </c>
       <c r="E94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/greyfoxdesign/product/personalised-quote-wire-word-art</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898792&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>905169</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Birthstone Bracelet</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>attic</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>5</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>915034</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Day / First Anniversary Card</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>sascreative</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>917605</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Personalised Couples Large Matchbox</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>oakdenedesigns</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>919273</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Gold Plated Or Sterling Silver Initial Tbar Necklace</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>hurleyburley</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-or-sterling-silver-initial-tbar-necklace</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=919273&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Dandelion Foil Birthday Gift Scarf</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>2</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>948800</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Large Butterfly Print Scarf</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>myposhshop</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
         <v>3</v>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-chocolate-treats-bowl</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>950732</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Dragonfly Foil Scarf Letterbox Gift</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>studiohop</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>3</v>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-08-18T01:37:10Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,49 +535,49 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1035825</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Personalised Treat Pot For Him</t>
+          <t>Star Sign Constellation Earrings Studs</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-father-s-day-treat-pot</t>
+          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1035825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1061155</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Star Sign Constellation Earrings Studs</t>
+          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>daisymaison</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1050164</t>
+          <t>1061842</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Welly Plant Pot Gift</t>
+          <t>Personalised Family Street Sign</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>daisymaison</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,55 +616,55 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-welly-plant-pot-thank-you-teacher-gift</t>
+          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-family-street-sign</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1050164&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1073729</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tree Of Life Rose Gold Foil Scarf Gift</t>
+          <t>Personalised Dog Breed Pocket Treat Tin</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/tree-of-life-foil-scarf-letterbox-gift</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-dog-breed-treat-tin</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1073729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1121511</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Natural Flowers Summer Door Wreath</t>
+          <t>Personalised Large Forest Green Welly Boots Planter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -674,34 +674,34 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/natural-flowers-autumn-door-wreath</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/large-forest-green-welly-boots-planter</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1121511&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1107283</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Embroidered Initials Washbag</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,30 +709,30 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-embroidered-initials-washbag</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1107283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1112053</t>
+          <t>1154129</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised 1965 60th Birthday Sixpence Necklace</t>
+          <t>Personalised Pet Memorial Decoration</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>laurastanleydesigns</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,61 +740,61 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/personalised-1961-60th-birthday-sixpence-necklace</t>
+          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1112053&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1119514</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Golf Set With Golf Balls And Tees</t>
+          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-golf-set-with-golf-balls-and-tees</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1119514&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1158875</t>
+          <t>1169016</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Wedding Iced Biscuit Box</t>
+          <t>Personalised Graduation Coaster, Graduation Keepsake</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>julietstallwoodcakesandbiscuits</t>
+          <t>studioyelle</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -802,185 +802,185 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/julietstallwoodcakesandbiscuits/product/wedding-iced-biscuit-gift-box</t>
+          <t>https://www.notonthehighstreet.com/studioyelle/product/personalised-graduation-coaster-graduation-keepsake</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158875&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1169016&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1172066</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Personalised Women's Technology Travel Case Gift</t>
+          <t>Personalised Linen Photo Album</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>stori</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
+          <t>https://www.notonthehighstreet.com/stori/product/personalised-linen-photo-album</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1180755</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Personalised Wedding Pebble Picture</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-swing-pebble-picture</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180755&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1205131</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wildflower Seed Balls For Bees Pack Of Three</t>
+          <t>Personalised Women's Technology Travel Case Gift</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>seedball</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/seedball/product/bee-wildflower-seed-ball-set-of-three-packets</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1211012</t>
+          <t>1191887</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sterling Silver Bold Coil Drop Earrings</t>
+          <t>Trio Of Fabulous Fruit Cakes</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>theoriginalcakecompany</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-bold-coil-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/theoriginalcakecompany/product/fruit-cake-selection</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1191887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sterling Silver Twist Ball Dangly Earrings</t>
+          <t>Dog And Owner Personalised Walking Socks</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>alphabetinteriors</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
+          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1229228</t>
+          <t>1245502</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Entwined Wedding Rings Card</t>
+          <t>Sterling Silver And Gold Daisy Stud Earrings - 10mm</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>wholeinthemiddle</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -988,55 +988,55 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/personalised-entwined-wedding-rings-card</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1234030</t>
+          <t>1246966</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Amber Bee Pendant Necklace</t>
+          <t>Mustard Ginkgo Print Scarf</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-baltic-amber-bee-pendant-necklace</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/ginkgo-print-scarf</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234030&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1246964</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Floating Petal Print Scarf</t>
+          <t>Large Tropical Leaf Scarf</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1046,28 +1046,28 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/floating-petal-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1277229</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Large Tropical Leaf Scarf</t>
+          <t>Westie Dog Print Scarf</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1077,34 +1077,34 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/leopard-print-black-border-and-stripes-scarf</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1290018</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Personalised Birth Year Football Club Print</t>
+          <t>Sterling Silver Rectangular Huggie Hoop Earrings - 15mm</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1112,92 +1112,92 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-birth-year-football-club-print</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-rectangular-huggie-hoop-earrings</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1260374</t>
+          <t>1313730</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sterling Silver Blue Forget Me Not Stud Earrings - 5mm</t>
+          <t>Highland Cow Cream Cushion, Sofa Tidy, Remote Control Holder</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/highland-cow-sofa-tidy-organiser-keep-your-remote-safe</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1261865</t>
+          <t>1320773</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>60th Birthday Vintage Sixpence Locket Necklace</t>
+          <t>Funny Wise Womans Words Keyring Gift</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/1963-60th-birthday-vintage-sixpence-locket-necklace</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/funny-wise-womans-words-keyring-gift</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1261865&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320773&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1271268</t>
+          <t>1322572</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Personalised Best Friends Pebble Picture</t>
+          <t>Personalised Train Station Railway Totem Sign</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1205,61 +1205,61 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friendship-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-train-station-railway-sign</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1322572&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1277784</t>
+          <t>1340963</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver St Christopher Necklace</t>
+          <t>Personalised Men's Leather Rfid Bifold Wallet</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>parkerandco</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-large-st-christopher-necklace</t>
+          <t>https://www.notonthehighstreet.com/parkerandco/product/personalised-black-men-s-rfid-leather-bifold-wallet</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1340963&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1278602</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Birth Flower Birthday Gift Terracotta Plant Pot</t>
+          <t>Fabric Name Peekaboo Memory Box</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>modocreative</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1267,30 +1267,30 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birth-flower-personalised-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/modocreative/product/fabric-peekaboo-keepsake-box</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278602&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Personalised Vintage Map Picture With Stitched Heart</t>
+          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>poshtottydesignscreates</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1298,30 +1298,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1298104</t>
+          <t>1369741</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Personalised Lego Brick Landscape Photo Block Puzzle</t>
+          <t>Personalised 80th Birthday Card For Him</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>brickbybrick23</t>
+          <t>hopeandlove</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,30 +1329,30 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/brickbybrick23/product/personalised-landscape-photo-block-puzzle</t>
+          <t>https://www.notonthehighstreet.com/hopeandlove/product/personalised-80th-birthday-card-for-him</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1298104&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1369741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1313730</t>
+          <t>1376487</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Highland Cow Cream Cushion, Sofa Tidy, Remote Control Holder</t>
+          <t>Tiny Turtle Strength Bracelet</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>letterboxlove</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1360,30 +1360,30 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/highland-cow-sofa-tidy-organiser-keep-your-remote-safe</t>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/tiny-turtle-strength-bracelet</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1330966</t>
+          <t>1381151</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Handmade Personalised Leather Curved Corner Bookmark</t>
+          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>parkerandco</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1391,61 +1391,61 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/parkerandco/product/handmade-personalised-leather-curved-corner-bookmark</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>133151</t>
+          <t>1386556</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sheep Sofa Tidy, Remote Control Holder</t>
+          <t>Anniversary Scented Candle With Personalised Metal Lid</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>myleelondon</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/sheepey-sofa-tidy-coffe</t>
+          <t>https://www.notonthehighstreet.com/myleelondon/product/anniversary-scented-candle-with-personalised-metal-lid</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=133151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1386556&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1337443</t>
+          <t>1389021</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Genuine Leather Small Shoulder Bag, Cross Body Bag</t>
+          <t>1st Birthday Book Of Nursery Rhymes And Poems</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>handbagsdirect2u</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1453,61 +1453,61 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/genuine-leather-small-shoulder-bag-cross-body-bag</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/1st-birthday-book-of-nursery-rhymes-and-poems</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1337443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1344943</t>
+          <t>1397711</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>No Words Just Hugs Candle Gift Set</t>
+          <t>Sterling Silver Opal Droplet Drop Hook Earrings</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/no-words-just-hugs-candle-gift-set</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/aqua-green-opal-droplet-hook-earrings</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397711&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1345852</t>
+          <t>1402302</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Personalised Birthday Newspaper Book Daily Telegraph Edition</t>
+          <t>Funny 40 50 60 70 80 90th T Shirt Birthday Gift For Him</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>historicnewspapers</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,61 +1515,61 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/historicnewspapers/product/personalised-telegraph-birthday-newspaper-book</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/funny-40-50-60-70-80-t-shirt-birthday-gift-for-him</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345852&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402302&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1410676</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
+          <t>Personalised Wedding Gift Oak Keepsake Box</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>mirrorin</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
+          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-gift-oak-keepsake-box</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1418825</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
+          <t>Camares Wood Organic Pebble Mirror</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>iconiccoasters</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1577,30 +1577,30 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/camares-wood-organic-pebble-mirror</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1365394</t>
+          <t>1421445</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
+          <t>Sterling Silver Daisy Chain Adjustable Ring</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>feelsilkstudio</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,30 +1608,30 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
+          <t>https://www.notonthehighstreet.com/feelsilkstudio/product/sterling-silver-daisy-chain-adjustable-ring</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421445&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1376067</t>
+          <t>1429998</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Deluxe Relaxation And Wellness Pamper Gift Set</t>
+          <t>Women's Leather Rfid Purse</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>marigoldcharms</t>
+          <t>handbagsdirect2u</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1639,61 +1639,61 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marigoldcharms/product/deluxe-relaxation-wellness-pamper-gift-set</t>
+          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-blue-leather-rfid-purse</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376067&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1429998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1436809</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
+          <t>Spitfire And Lancaster Double Garden Art</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>gapgardenproducts</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/gapgardenproducts/product/spitfire-lancaster-double-garden-art</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1387361</t>
+          <t>1454208</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
+          <t>Fuck Cancer Morse Code Bracelet</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,30 +1701,30 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-morse-code-bracelet</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1454208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1388105</t>
+          <t>1456391</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems In Adorable Pink</t>
+          <t>Personalised Mum And Daughter Pebble Picture</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1732,30 +1732,30 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-in-adorable-pink</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-mum-and-daughter-pebble-picture</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1388105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1392508</t>
+          <t>1470941</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Personalised Six Tea Tea Towel 60th Birthday Gift</t>
+          <t>Porcelain Bird Earrings French Vintage Charm</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>afewhometruths</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1763,61 +1763,61 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/afewhometruths/product/personalised-six-tea-tea-towel-60th-birthday-present</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1392508&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1396397</t>
+          <t>1478663</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
+          <t>Porcelain Bird French Vintage Charm Bracelet</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-french-vintage-charm-bracelet</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1397555</t>
+          <t>1483273</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Opal Turquoise Wing Stud Earrings</t>
+          <t>Personalised Wooden Pink Bunny Stacking Toy</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>silkpursesowsear</t>
+          <t>giftspersonalised</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1825,92 +1825,92 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silkpursesowsear/product/opal-turquoise-wing-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/giftspersonalised/product/personalised-wooden-pink-bunny-stacking-toy</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1483273&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>141541</t>
+          <t>1494709</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Extra Large Personalised Leather Photo Album</t>
+          <t>Turquoise Huggie Earrings</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>begolden</t>
+          <t>bysamjewellery</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/begolden/product/large-leather-photo-album-gold</t>
+          <t>https://www.notonthehighstreet.com/bysamjewellery/product/turquoise-huggie-earrings</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=141541&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494709&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1416578</t>
+          <t>1494976</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Personalised Bride Metal Shoe Tags</t>
+          <t>Personalised Winthorpe Floral Wreath</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-bride-metal-shoe-tags</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416578&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1420726</t>
+          <t>1503694</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Personalised Metal Music Sheet Page Holder</t>
+          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company Silver Small</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1918,30 +1918,30 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-music-sheet-page-holder</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1431321</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Personalised Treasured Memories Photo Box</t>
+          <t>Rose Bouquet Personalised Card</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>karriebarroncards</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1949,123 +1949,123 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-treasured-memories-photo-box</t>
+          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431321&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1435032</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lawn Enforcement Officer Funny Men's Gardening T Shirt</t>
+          <t>Sterling Silver April Shower Drop Earrings</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/lawn-enforcement-officer-funny-men-s-gardening-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435032&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1435766</t>
+          <t>412675</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sterling Silver Enamel Bluebell Flower Drop Hook Earrings</t>
+          <t>Literary Paper 1st Anniversary Rose</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>cot2totandbeyond</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-enamel-bluebell-flower-drop-hook-earrings</t>
+          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1447257</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sterling Silver August Birthstone Necklace - Peridot</t>
+          <t>Peridot Quartz Drop Earrings</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>thelittlekeepsakecompany</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelittlekeepsakecompany/product/sterling-silver-august-birthstone-necklace-peridot</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1447257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1448731</t>
+          <t>431704</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Personalised Russian Ring Necklace</t>
+          <t>Personalised Map Wedding Anniversary Silver Cufflinks</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>abiza</t>
+          <t>bombus</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2073,61 +2073,61 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/abiza/product/personalised-russian-ring-necklace</t>
+          <t>https://www.notonthehighstreet.com/bombus/product/bespoke-map-cufflinks</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1448731&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=431704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1466041</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Grow Your Own August Birth Flower Personalised Name Tin</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>alphabetgifting</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetgifting/product/grow-your-own-august-birth-flower-personalised-name-tin</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1466041&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1470941</t>
+          <t>535503</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Porcelain Bird Earrings French Vintage Charm</t>
+          <t>Sterling Silver Tree Of Life Round Necklace</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2135,123 +2135,123 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-tree-of-life-round-necklace</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=535503&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1476087</t>
+          <t>539718</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Spa Gift Box For Women</t>
+          <t>Personalised Wooden Pot Planter</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>hallby</t>
+          <t>netalternative</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hallby/product/spa-gift-box-for-women</t>
+          <t>https://www.notonthehighstreet.com/netalternative/product/personalised-white-wooden-planter</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=539718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1482117</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hand Cream With Hibiscus Flowers Worth £20</t>
+          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>upcircle</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/upcircle/product/hand-cream-with-hibiscus-flowers</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>589037</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Birthday Gift Terracotta Plant Pot</t>
+          <t>Personalised Leather Washbag</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>vidavida</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birthday-gift-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/vidavida/product/leather-washbag</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=589037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1494976</t>
+          <t>607975</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Personalised Winthorpe Floral Wreath</t>
+          <t>Mineral Bath Infusions Gift Collection</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/mineral-bath-infusions-gift-collection</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1496914</t>
+          <t>608655</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Petsentials Super Clumping Cat Litter Bag Active Carbon 20 L</t>
+          <t>Personalised House Portrait Line Drawing Print</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>noahsark</t>
+          <t>mollymoodesigns</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,92 +2290,92 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noahsark/product/petsentials-super-clumping-cat-litter-bag-active-carbon</t>
+          <t>https://www.notonthehighstreet.com/mollymoodesigns/product/personalised-house-line-drawing-print</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496914&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=608655&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1497603</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Personalised 60th Wedding Anniversary Gift - Diamond Heart Plaque</t>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/personalised-60th-anniversary-gift-diamond-heart-plaque</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497603&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1498337</t>
+          <t>618130</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>20th China Anniversary Heart Shaped Keepsake Ceramic Gift</t>
+          <t>Personalised Women's Floral Print Kimono Dressing Gown</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>pinkstrawberry</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pinkstrawberry/product/20th-china-anniversary-heart-shaped-keepsake-ceramic-gift</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/blossom-kimono</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=618130&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1502932</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Christening Star Night Light</t>
+          <t>Friendship Knot Bangle</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>looppa</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2383,61 +2383,61 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/looppa/product/christening-star-night-light</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>631040</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company Silver Small</t>
+          <t>Silver Friendship Knot Earrings</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>thelyndoncompany</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/silver-friendship-knot-earrings</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1508460</t>
+          <t>64050</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Personalised Saturday Night Snacks Bowl</t>
+          <t>Wedding Card, Personalised, Embroidered</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>simonseabright</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2445,61 +2445,61 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-saturday-night-snacks-bowl</t>
+          <t>https://www.notonthehighstreet.com/simonseabright/product/wedding_card</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=64050&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>255970</t>
+          <t>758994</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>White Sleeveless Cotton Nightdress Lizzie</t>
+          <t>Personalised Papercut Golden Wedding Anniversary Card</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>pogofandango</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
+          <t>https://www.notonthehighstreet.com/pogofandango/product/personalised-papercut-golden-wedding-anniversary-card</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=758994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>258082</t>
+          <t>760421</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Personalised Tablet Stand In Oak Or Walnut</t>
+          <t>Personalised Family Names Heart Necklace</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>mijmoj</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2507,92 +2507,92 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mijmoj/product/oak-ipad-stand</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mixed-metal-heart-necklace</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=258082&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>770318</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sterling Silver April Shower Drop Earrings</t>
+          <t>Personalised 21st Necklace With Birthstone</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>779785</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Metallic Silver Bee Scarf</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-silver-bee-scarf</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=779785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>451823</t>
+          <t>785952</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Personalised Hearts Wedding Card</t>
+          <t>Sterling Silver Birthstone Initial Sliding Bracelet</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>eggbertanddaisy</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2600,216 +2600,216 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/eggbertanddaisy/product/personalised-hearts-wedding-card</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-initial-sliding-bracelet</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=451823&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=785952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>46761</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Personalised Wooden Letter Name Train</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>wheniwasakid</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wheniwasakid/product/handmade_wooden_alphabet_train</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=46761&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>801933</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>Personalised Pull Out Photo Album Token Gift</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>482198</t>
+          <t>804990</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Busy Butterfly, Bee, Bug And Beneficial Insect Habitat</t>
+          <t>Personalised Enamel Snack Pot</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>selections</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/selections/product/pollinating-bee-nesting-log</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>488356</t>
+          <t>837190</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sterling Silver Secret Message Ring</t>
+          <t>Dinosaur Glow In The Dark T Shirt</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>glowgalaxyart</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
+          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>510573</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Baby's Personalised Silver Christening Bracelet</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>hurleyburleyjunior</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/baby-s-personalised-sterling-silver-id-bracelet</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=510573&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
+          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>twentyseven</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
+          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2817,61 +2817,61 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>868202</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle</t>
+          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>711157</t>
+          <t>871013</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Personalised Ceramic Plate Pearl Wedding Anniversary</t>
+          <t>Personalised Pack Of Six Wooden Heart Coasters</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>melissachoroszewskaceramics</t>
+          <t>thealphabetgiftshop</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2879,30 +2879,30 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/melissachoroszewskaceramics/product/personalised-ceramic-pearl-plate</t>
+          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-pack-of-six-wooden-heart-coasters</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=711157&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=871013&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>719727</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Skinny Thumb Ring</t>
+          <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2910,30 +2910,30 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/skinny-thumb-ring</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=719727&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>760421</t>
+          <t>892259</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Personalised Family Names Heart Necklace</t>
+          <t>Silver Blue And Green Leaf Earrings</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>vintagelane</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2941,61 +2941,61 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mixed-metal-heart-necklace</t>
+          <t>https://www.notonthehighstreet.com/vintagelane/product/vintage-blue-and-green-flower-earrings</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=892259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>764045</t>
+          <t>894608</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Personalised Birthstone Disc Stretch Bracelet</t>
+          <t>Personalised Train Ticket Anniversary Card</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>oflifeandlemons</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
+          <t>https://www.notonthehighstreet.com/oflifeandlemons/product/together-in-spritz-card-for-friend</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=894608&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>898576</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+          <t>Personalised Sixty Things To Do When You Are 60 Gift</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>ayearofdates</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -3003,61 +3003,61 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/ayearofdates/product/personalised-sixty-things-to-do-when-you-are-60-gift</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>905169</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
+          <t>Birthstone Bracelet</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>798315</t>
+          <t>905996</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Personalised Friendship Knot Bracelet</t>
+          <t>Personalised Girl's Luxury Navy Silky Pyjama's</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3065,92 +3065,92 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-friendship-knot-bracelet</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/personalised-girl-s-navy-satin-pyjama-s</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=798315&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905996&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>799432</t>
+          <t>917605</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Personalised Football Ball Customise With Any Name</t>
+          <t>Personalised Couples Large Matchbox</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>nameyourball</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nameyourball/product/personalised-football-ball-style-v4</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=799432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>804990</t>
+          <t>944805</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Personalised Enamel Snack Pot</t>
+          <t>Personalised Carry All Travel Purse</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>penelopetom</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
+          <t>https://www.notonthehighstreet.com/penelopetom/product/personalised-carry-all-travel-purse</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>837190</t>
+          <t>975970</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Dinosaur Glow In The Dark T Shirt</t>
+          <t>From This Day Personalised Wedding Card</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>glowgalaxyart</t>
+          <t>wholeinthemiddle</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -3158,444 +3158,41 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/from-this-day-personalised-wedding-card</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=975970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>837561</t>
+          <t>999592</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Personalised Metal Shoe Tags</t>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-shoe-tags</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837561&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>841037</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Personalised Leather Tool Belt For Dad</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>hotdot</t>
-        </is>
-      </c>
-      <c r="E90" t="n">
-        <v>2</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-tool-belt</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=841037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>856677</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Personalised Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>theforestandco</t>
-        </is>
-      </c>
-      <c r="E92" t="n">
-        <v>7</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>876946</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Multi Stranded Magnet Bracelet</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>lovethelinks</t>
-        </is>
-      </c>
-      <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lovethelinks/product/three-coloured-stranded-bracelet</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876946&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>898792</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Personalised Quote Wire Word Art</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>greyfoxdesign</t>
-        </is>
-      </c>
-      <c r="E94" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/greyfoxdesign/product/personalised-quote-wire-word-art</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898792&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>905169</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Birthstone Bracelet</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>attic</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
-        <v>5</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>915034</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Day / First Anniversary Card</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>sascreative</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
-        <v>2</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>917605</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Personalised Couples Large Matchbox</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>oakdenedesigns</t>
-        </is>
-      </c>
-      <c r="E97" t="n">
-        <v>2</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>919273</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Gold Plated Or Sterling Silver Initial Tbar Necklace</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>hurleyburley</t>
-        </is>
-      </c>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-or-sterling-silver-initial-tbar-necklace</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=919273&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Dandelion Foil Birthday Gift Scarf</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E99" t="n">
-        <v>2</v>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>948800</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Large Butterfly Print Scarf</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E100" t="n">
-        <v>3</v>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-butterfly-print-scarf</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>950732</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Dragonfly Foil Scarf Letterbox Gift</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E101" t="n">
-        <v>3</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/dragonfly-foil-scarf-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=950732&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>999592</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E102" t="n">
-        <v>3</v>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-08-25T01:31:22Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1006901</t>
+          <t>102177</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Abstract Flower Print Scarf</t>
+          <t>Personalised Cotton Or Linen Napkin</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>bigstitch</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/valentines-abstract-flowers-scarf</t>
+          <t>https://www.notonthehighstreet.com/bigstitch/product/personalised-white-linen-napkin</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1006901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=102177&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1039459</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Map Engagement Card</t>
+          <t>Personalised Wedding Day Celebration Card</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-celebration-card</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039459&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1053070</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Star Sign Constellation Earrings Studs</t>
+          <t>Birth Flower Scarf And Card In A Gift Box</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/birth-flower-scarf-and-card-in-a-gift-box</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053070&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1061155</t>
+          <t>1071124</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised 'BBQ &amp; Grill' Garden Sign</t>
+          <t>Personalised Couples Heart Wedding Gift Chopping Board</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-bbq-grill-garden-sign</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-couples-heart-wedding-gift-chopping-board</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1071124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1061842</t>
+          <t>1084447</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Personalised Family Street Sign</t>
+          <t>Engagement Gift Personalised Proposal Location Print</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>daisymaison</t>
+          <t>monoscape</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/daisymaison/product/personalised-family-street-sign</t>
+          <t>https://www.notonthehighstreet.com/monoscape/product/engagement-gift-personalised-proposal-location-print</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1061842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1084447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1073729</t>
+          <t>1130264</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Dog Breed Pocket Treat Tin</t>
+          <t>Personalised Family Bench Pebble Picture</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-dog-breed-treat-tin</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-family-bench-pebble-picture</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1073729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130264&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1121511</t>
+          <t>1130576</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Large Forest Green Welly Boots Planter</t>
+          <t>Personalised Burnt Orange To Grey Cashmere Blend Scarf</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,61 +678,61 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/large-forest-green-welly-boots-planter</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-and-grey-colour-block-scarf</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1121511&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1143803</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>Personalised Plantable Wedding Card And Plant A Tree</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>cardbee</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/cardbee/product/personalised-plantable-wedding-card-and-plant-a-tree</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1143803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1154129</t>
+          <t>1147645</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Pet Memorial Decoration</t>
+          <t>Mouse Opening Red Door Fairy Garden Decoration With Bag</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>laurastanleydesigns</t>
+          <t>animalcrackers</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,92 +740,92 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
+          <t>https://www.notonthehighstreet.com/animalcrackers/product/cute-mouse-opening-red-door-fairy-garden-decoration</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1147645&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1154129</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Enamelled Birth Flower Brooch In A Gift Box</t>
+          <t>Personalised Pet Memorial Decoration</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>laurastanleydesigns</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/enamelled-birth-flower-brooch-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1169016</t>
+          <t>1154598</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalised Graduation Coaster, Graduation Keepsake</t>
+          <t>Delicate Tree Print Scarf</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>studioyelle</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studioyelle/product/personalised-graduation-coaster-graduation-keepsake</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1169016&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1172066</t>
+          <t>1159266</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Personalised Linen Photo Album</t>
+          <t>Men's Personalised Brushed Stainless Steel Wide Spinner Ring - 8mm</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>stori</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -833,30 +833,30 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/stori/product/personalised-linen-photo-album</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172066&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1180755</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Wedding Pebble Picture</t>
+          <t>Personalised Birth Flower Stoneware Mug</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -864,92 +864,92 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-swing-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180755&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1190985</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Personalised Women's Technology Travel Case Gift</t>
+          <t>Personalised Birth Month Flower Printed Can Glass</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>propergoose</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
+          <t>https://www.notonthehighstreet.com/propergoose/product/personalised-birth-month-flower-printed-can-glass</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1191887</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Trio Of Fabulous Fruit Cakes</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>theoriginalcakecompany</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theoriginalcakecompany/product/fruit-cake-selection</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1191887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Dog And Owner Personalised Walking Socks</t>
+          <t>Christening Keepsake Gift Book Personalised For Baby</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>alphabetinteriors</t>
+          <t>mymagicname</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -957,61 +957,61 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetinteriors/product/dog-and-owner-personalised-walking-socks</t>
+          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1245502</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Daisy Stud Earrings - 10mm</t>
+          <t>Sterling Silver Twist Ball Dangly Earrings</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1246966</t>
+          <t>1211471</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mustard Ginkgo Print Scarf</t>
+          <t>Sterling Silver Chunky Hoop Earrings</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1019,61 +1019,61 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/ginkgo-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-plated-or-sterling-silver-hoop-earrings</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1217412</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Large Tropical Leaf Scarf</t>
+          <t>Personalised Sterling Silver Blue Opal Spinner Ring - 5mm</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/large-tropical-leaf-scarf</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-sterling-silver-opal-spinner-ring</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1217412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1277229</t>
+          <t>1226971</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Westie Dog Print Scarf</t>
+          <t>Personalised Wedding Anniversary Greeting Card</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1081,24 +1081,24 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/leopard-print-black-border-and-stripes-scarf</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-anniversary-greeting-card</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1226971&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1290018</t>
+          <t>1232841</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sterling Silver Rectangular Huggie Hoop Earrings - 15mm</t>
+          <t>Personalised Sterling Silver Jade Necklace</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1112,92 +1112,92 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-rectangular-huggie-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-jade-teardrop-pendant-necklace</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1313730</t>
+          <t>1244120</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Highland Cow Cream Cushion, Sofa Tidy, Remote Control Holder</t>
+          <t>50th Birthday Sterling Silver Bracelet</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/highland-cow-sofa-tidy-organiser-keep-your-remote-safe</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/50th-birthday-sterling-silver-bracelet</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244120&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1320773</t>
+          <t>1245502</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Funny Wise Womans Words Keyring Gift</t>
+          <t>Sterling Silver And Gold Daisy Stud Earrings - 10mm</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/funny-wise-womans-words-keyring-gift</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320773&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1322572</t>
+          <t>1260374</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Personalised Train Station Railway Totem Sign</t>
+          <t>Sterling Silver Blue Forget Me Not Stud Earrings - 5mm</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1205,30 +1205,30 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-train-station-railway-sign</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1322572&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1340963</t>
+          <t>1264171</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Personalised Men's Leather Rfid Bifold Wallet</t>
+          <t>Personalised Leather Notebook Lined</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>parkerandco</t>
+          <t>hotdot</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1236,61 +1236,61 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/parkerandco/product/personalised-black-men-s-rfid-leather-bifold-wallet</t>
+          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-leather-notebook-a5-lined</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1340963&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1272569</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fabric Name Peekaboo Memory Box</t>
+          <t>Personalised 21st Birthday Bracelet With Heart</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>modocreative</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/modocreative/product/fabric-peekaboo-keepsake-box</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-birthday-bracelet</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1277156</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>F1 Formula One 2025 Calendar Track T Shirt Gift For Him</t>
+          <t>Milestone Birthday Personalised Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1298,30 +1298,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/milestone-birthday-personalised-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1369741</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Personalised 80th Birthday Card For Him</t>
+          <t>Personalised Vintage Map Picture With Stitched Heart</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>hopeandlove</t>
+          <t>poshtottydesignscreates</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,30 +1329,30 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hopeandlove/product/personalised-80th-birthday-card-for-him</t>
+          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1369741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1376487</t>
+          <t>1309827</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Tiny Turtle Strength Bracelet</t>
+          <t>Personalised Baby Dungarees - Embroidered Baby Romper Gift For Newborn, Boy Or Girl</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>letterboxlove</t>
+          <t>cublifeclothing</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1360,61 +1360,61 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterboxlove/product/tiny-turtle-strength-bracelet</t>
+          <t>https://www.notonthehighstreet.com/cublifeclothing/product/personalised-baby-dungarees-romper-embroidered</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376487&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1320832</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Gold Jewel Inlay Hoop Earrings In A Gift Box</t>
+          <t>Sterling Silver Name Necklace</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>potiega</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/gold-jewell-inlay-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/potiega/product/sterling-silver-name-necklace</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1386556</t>
+          <t>1330774</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Anniversary Scented Candle With Personalised Metal Lid</t>
+          <t>Sterling Silver Little Twinkle Stars Charm Anklet</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>myleelondon</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1422,30 +1422,30 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myleelondon/product/anniversary-scented-candle-with-personalised-metal-lid</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-little-twinkle-stars-charm-anklet</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1386556&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1389021</t>
+          <t>1341083</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1st Birthday Book Of Nursery Rhymes And Poems</t>
+          <t>Personalised Golden Anniversary 50 Years Pebble Picture</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1453,30 +1453,30 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/1st-birthday-book-of-nursery-rhymes-and-poems</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-golden-anniversary-50-years-pebble-picture</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1397711</t>
+          <t>1341118</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sterling Silver Opal Droplet Drop Hook Earrings</t>
+          <t>Personalised Wedding Mr And Mrs Pebble Picture</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1484,61 +1484,61 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/aqua-green-opal-droplet-hook-earrings</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-mr-mrs-pebble-picture</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397711&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341118&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1402302</t>
+          <t>1347117</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Funny 40 50 60 70 80 90th T Shirt Birthday Gift For Him</t>
+          <t>60th Birthday 1965 Sixpence Coin Compact Mirror</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>nappyhead</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nappyhead/product/funny-40-50-60-70-80-t-shirt-birthday-gift-for-him</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/60th-birthday-1963-sixpence-coin-compact-mirror</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1402302&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1410676</t>
+          <t>1347156</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Personalised Wedding Gift Oak Keepsake Box</t>
+          <t>70th Birthday 1955 Sixpence Coin Compact Mirror</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>mirrorin</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1546,61 +1546,61 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mirrorin/product/personalised-wedding-gift-oak-keepsake-box</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/70th-birthday-1953-sixpence-coin-compact-mirror</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410676&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1418825</t>
+          <t>1362911</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Camares Wood Organic Pebble Mirror</t>
+          <t>Personalised Brownie Box</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>rubythecakeartist</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/camares-wood-organic-pebble-mirror</t>
+          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418825&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1421445</t>
+          <t>1372560</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sterling Silver Daisy Chain Adjustable Ring</t>
+          <t>Personalised Tractor Keepsake Birthday Card</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>feelsilkstudio</t>
+          <t>noordinarygiftcompany</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,30 +1608,30 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/feelsilkstudio/product/sterling-silver-daisy-chain-adjustable-ring</t>
+          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/personalised-tractor-keepsake-birthday-card</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421445&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1429998</t>
+          <t>1372931</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Women's Leather Rfid Purse</t>
+          <t>1985 Personalised 40th Ruby Wedding Anniversary Poster</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>handbagsdirect2u</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1639,30 +1639,30 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/handbagsdirect2u/product/women-s-blue-leather-rfid-purse</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-40th-ruby-wedding-anniversary-poster</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1429998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372931&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1436809</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Spitfire And Lancaster Double Garden Art</t>
+          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>gapgardenproducts</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1670,30 +1670,30 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gapgardenproducts/product/spitfire-lancaster-double-garden-art</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1436809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1454208</t>
+          <t>1378864</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fuck Cancer Morse Code Bracelet</t>
+          <t>Personalised Wedding Day Card Gold And White Floral</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>thedogscollarsuk</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,123 +1701,123 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-morse-code-bracelet</t>
+          <t>https://www.notonthehighstreet.com/thedogscollarsuk/product/personalised-wedding-day-card-gold-and-white-floral</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1454208&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1456391</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Personalised Mum And Daughter Pebble Picture</t>
+          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-mum-and-daughter-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1470941</t>
+          <t>1394107</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Porcelain Bird Earrings French Vintage Charm</t>
+          <t>Personalised Leather Key Holder</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>vidavida</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
+          <t>https://www.notonthehighstreet.com/vidavida/product/personalised-leather-key-holder</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1478663</t>
+          <t>1395590</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Porcelain Bird French Vintage Charm Bracelet</t>
+          <t>Personalised Where It All Began, Anniversary Gift Print</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>hooddesignsco</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-french-vintage-charm-bracelet</t>
+          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-where-it-all-began-anniversary-gift-print</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395590&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1483273</t>
+          <t>1405402</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Personalised Wooden Pink Bunny Stacking Toy</t>
+          <t>Jewellery Organiser With Personalised Handle Gift Set</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>giftspersonalised</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1825,61 +1825,61 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/giftspersonalised/product/personalised-wooden-pink-bunny-stacking-toy</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/jewellery-organiser-with-personalised-handle-gift-set</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1483273&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1405402&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1494709</t>
+          <t>1470924</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Turquoise Huggie Earrings</t>
+          <t>Adjustable Anklet Bracelet With Fish Charm</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>bysamjewellery</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bysamjewellery/product/turquoise-huggie-earrings</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/adjustable-anklet-bracelet-with-fish-charm</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494709&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470924&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1494976</t>
+          <t>1476087</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Personalised Winthorpe Floral Wreath</t>
+          <t>Spa Gift Box For Women</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>hallby</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1887,30 +1887,30 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
+          <t>https://www.notonthehighstreet.com/hallby/product/spa-gift-box-for-women</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1503694</t>
+          <t>1489678</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Luxury Waffle Cotton Bathrobe The Lyndon Company Silver Small</t>
+          <t>Birthday Gift Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>thelyndoncompany</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1918,30 +1918,30 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/luxury-waffle-cotton-bathrobe-the-lyndon-company</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birthday-gift-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503694&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1500488</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Rose Bouquet Personalised Card</t>
+          <t>Personalised Horse Charm Bracelet</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>karriebarroncards</t>
+          <t>nameitwhatyoulike</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1949,123 +1949,123 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/nameitwhatyoulike/product/personalised-horse-pony-charm-bracelet</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>1509775</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sterling Silver April Shower Drop Earrings</t>
+          <t>Sterling Silver Birthstone Beaded Bracelet</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>wishedfor</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
+          <t>https://www.notonthehighstreet.com/wishedfor/product/sterling-silver-birthstone-beaded-bracelet</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>1513080</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Literary Paper 1st Anniversary Rose</t>
+          <t>To My Daughter Necklace - Heart Infinity Charm, Sterling Silver Jewellery Gift, Personalised Birthday Keepsake</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>cot2totandbeyond</t>
+          <t>lunity</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cot2totandbeyond/product/book-page-roses</t>
+          <t>https://www.notonthehighstreet.com/lunity/product/to-my-daughter-necklace-heart-infinity-charm-sterling-silver-jewellery-gift-personalised-birthday-keepsake</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>1514040</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Personalised BBQ Serving Tray</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-bbq-serving-tray</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>431704</t>
+          <t>1514805</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Personalised Map Wedding Anniversary Silver Cufflinks</t>
+          <t>Guinness Lover's Gift Hamper With Chocolate And Snacks</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>bombus</t>
+          <t>bottleinabox</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2073,154 +2073,154 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bombus/product/bespoke-map-cufflinks</t>
+          <t>https://www.notonthehighstreet.com/bottleinabox/product/guinness-lover-s-gift-hamper-with-chocolate-snacks</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=431704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>255970</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Family Birthstone Link Bracelet</t>
+          <t>White Sleeveless Cotton Nightdress Lizzie</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>535503</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Sterling Silver Tree Of Life Round Necklace</t>
+          <t>Rose Bouquet Personalised Card</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>karriebarroncards</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-tree-of-life-round-necklace</t>
+          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=535503&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>539718</t>
+          <t>307533</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Personalised Wooden Pot Planter</t>
+          <t>Personalised Entwined Letters Wedding Card</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>netalternative</t>
+          <t>hickorydickory</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/netalternative/product/personalised-white-wooden-planter</t>
+          <t>https://www.notonthehighstreet.com/hickorydickory/product/personalised-wedding-card</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=539718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=307533&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>330009</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
+          <t>Personalised Papercut Wedding Card</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>twentyseven</t>
+          <t>pogofandango</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
+          <t>https://www.notonthehighstreet.com/pogofandango/product/personalised-papercut-wedding-card</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=330009&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>589037</t>
+          <t>355476</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Personalised Leather Washbag</t>
+          <t>Vintage Cast Iron Heart Shaped Bird Seed Feeder</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>vidavida</t>
+          <t>selections</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2228,30 +2228,30 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/vidavida/product/leather-washbag</t>
+          <t>https://www.notonthehighstreet.com/selections/product/decorative-cow-solar-light-ornament</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=589037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>607975</t>
+          <t>421466</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Mineral Bath Infusions Gift Collection</t>
+          <t>Peridot Quartz Drop Earrings</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>bankslyonbotanical</t>
+          <t>sarahhickeyjewellery</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/mineral-bath-infusions-gift-collection</t>
+          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>608655</t>
+          <t>433785</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Personalised House Portrait Line Drawing Print</t>
+          <t>White Cotton Short Sleeve Nightdress 18th Century</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>mollymoodesigns</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,92 +2290,92 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mollymoodesigns/product/personalised-house-line-drawing-print</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/18th-century-cotton-nightdress</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=608655&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>455532</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
+          <t>Personalised Solid Brass Cufflinks</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>mangunbear</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
+          <t>https://www.notonthehighstreet.com/mangunbear/product/solid-brass-cufflinks</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=455532&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>618130</t>
+          <t>482198</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Personalised Women's Floral Print Kimono Dressing Gown</t>
+          <t>Busy Butterfly, Bee, Bug And Beneficial Insect Habitat</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>selections</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/blossom-kimono</t>
+          <t>https://www.notonthehighstreet.com/selections/product/pollinating-bee-nesting-log</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=618130&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>488356</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Friendship Knot Bangle</t>
+          <t>Sterling Silver Secret Message Ring</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2383,61 +2383,61 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/friendship-knot-bangle</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>631040</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Silver Friendship Knot Earrings</t>
+          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/silver-friendship-knot-earrings</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>64050</t>
+          <t>565722</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Wedding Card, Personalised, Embroidered</t>
+          <t>Wedding Anniversary Family Art Print</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>simonseabright</t>
+          <t>homegrownprintco</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2445,61 +2445,61 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/simonseabright/product/wedding_card</t>
+          <t>https://www.notonthehighstreet.com/homegrownprintco/product/wedding-anniversary-family-art-print</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=64050&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=565722&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>758994</t>
+          <t>568444</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Personalised Papercut Golden Wedding Anniversary Card</t>
+          <t>Men's Plaited Leather Personalised Clasp Bracelet</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>pogofandango</t>
+          <t>hurleyburleyman</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pogofandango/product/personalised-papercut-golden-wedding-anniversary-card</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/limited-edition-personalised-clasp-bracelet</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=758994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=568444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>760421</t>
+          <t>631040</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Personalised Family Names Heart Necklace</t>
+          <t>Silver Friendship Knot Earrings</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2507,61 +2507,61 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/personalised-mixed-metal-heart-necklace</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/silver-friendship-knot-earrings</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=760421&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>770318</t>
+          <t>647568</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Personalised 21st Necklace With Birthstone</t>
+          <t>Girl's Personalised Sterling Silver Flower Necklace</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>hurleyburleyjunior</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/girl-s-personalised-sterling-silver-flower-necklace</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=647568&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>779785</t>
+          <t>655071</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Metallic Silver Bee Scarf</t>
+          <t>Ginge The Cat, Cuddly Companion Soft Toy</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>jomanda</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2569,24 +2569,24 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/metallic-silver-bee-scarf</t>
+          <t>https://www.notonthehighstreet.com/jomanda/product/cuddly-soft-plush-cat</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=779785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=655071&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>785952</t>
+          <t>712893</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Initial Sliding Bracelet</t>
+          <t>Personalised Pearl Sterling Silver Slide Bracelet</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -2600,61 +2600,61 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-initial-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/personalised-pearl-sterling-silver-slide-bracelet</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=785952&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=712893&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>713987</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
+          <t>Personalised 'Year' Unisex Sweatshirt</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>rockonruby</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/rockonruby/product/personalised-year-sweatshirt</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=713987&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>801933</t>
+          <t>738289</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Personalised Pull Out Photo Album Token Gift</t>
+          <t>Personalised Head Chef Apron, Cooking Gift</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>weaselandstoat</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2662,123 +2662,123 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
+          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>804990</t>
+          <t>764045</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Personalised Enamel Snack Pot</t>
+          <t>Personalised Birthstone Disc Stretch Bracelet</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>837190</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Dinosaur Glow In The Dark T Shirt</t>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>glowgalaxyart</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>793008</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
+          <t>Personalised Rainbow And Flower Bracelet Making Kit</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>studiohop</t>
+          <t>cottontwist</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2786,61 +2786,61 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
+          <t>https://www.notonthehighstreet.com/cottontwist/product/personalised-rainbow-flower-power-bracelet-making-kit</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=793008&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>866983</t>
+          <t>804990</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
+          <t>Personalised Enamel Snack Pot</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>868202</t>
+          <t>806693</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
+          <t>Personalised School Bag Tag Or Badge</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>evanslylane</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2848,30 +2848,30 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
+          <t>https://www.notonthehighstreet.com/evanslylane/product/personalised-school-bag-tag-or-badge</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=806693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>871013</t>
+          <t>807430</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Personalised Pack Of Six Wooden Heart Coasters</t>
+          <t>Carson The Lion, Newborn Baby Companion</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>thealphabetgiftshop</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2879,30 +2879,30 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thealphabetgiftshop/product/personalised-pack-of-six-wooden-heart-coasters</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/carson-the-lion-from-birth-soft-toy</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=871013&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=807430&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>830584</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Scarf</t>
+          <t>60th Birthday 1965 Sixpence Coin Bangle Bracelet</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2910,61 +2910,61 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/sixpence-1958-60th-birthday-coin-bangle-bracelet</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=830584&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>892259</t>
+          <t>837190</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Silver Blue And Green Leaf Earrings</t>
+          <t>Dinosaur Glow In The Dark T Shirt</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>vintagelane</t>
+          <t>glowgalaxyart</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/vintagelane/product/vintage-blue-and-green-flower-earrings</t>
+          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=892259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>894608</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Personalised Train Ticket Anniversary Card</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>oflifeandlemons</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2972,61 +2972,61 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oflifeandlemons/product/together-in-spritz-card-for-friend</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=894608&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>898576</t>
+          <t>879692</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Personalised Sixty Things To Do When You Are 60 Gift</t>
+          <t>Light Weight Wool Mix Poncho</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>ayearofdates</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ayearofdates/product/personalised-sixty-things-to-do-when-you-are-60-gift</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/light-weight-wool-mix-poncho</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>886944</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Birthstone Bracelet</t>
+          <t>Personalised Leather And Silver St Christopher Bracelet</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>hurleyburleyman</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -3034,30 +3034,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>905996</t>
+          <t>899547</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Personalised Girl's Luxury Navy Silky Pyjama's</t>
+          <t>Sterling Silver 18th Birthday Bracelet</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>yatrishomeandgift</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3065,61 +3065,61 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/personalised-girl-s-navy-satin-pyjama-s</t>
+          <t>https://www.notonthehighstreet.com/yatrishomeandgift/product/18th-birthday-bracelet-gift</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905996&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=899547&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>917605</t>
+          <t>905169</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Personalised Couples Large Matchbox</t>
+          <t>Birthstone Bracelet</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-couples-large-matchbox</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=917605&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>944805</t>
+          <t>927522</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Personalised Carry All Travel Purse</t>
+          <t>Personalised Aluminium Metal Photo Booth Bookmark</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>penelopetom</t>
+          <t>atypeofdesign</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -3127,30 +3127,30 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/penelopetom/product/personalised-carry-all-travel-purse</t>
+          <t>https://www.notonthehighstreet.com/atypeofdesign/product/personalised-aluminium-metal-photo-booth-book-mark</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=927522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>975970</t>
+          <t>954762</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>From This Day Personalised Wedding Card</t>
+          <t>Turquoise Drop Hoop Earrings</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>wholeinthemiddle</t>
+          <t>junkjewels</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -3158,41 +3158,103 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wholeinthemiddle/product/from-this-day-personalised-wedding-card</t>
+          <t>https://www.notonthehighstreet.com/junkjewels/product/turquoise-drop-hoop-earrings</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=975970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=954762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>982044</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+          <t>Vintage 21st/30th/40th/50th/60th/70th Birthday Tshirt</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
+          <t>jolly</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/jolly/product/milestone-birthday-30th-40th-50th-60th-vintage-tshirt</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>991741</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Personalised Swarovski Birthstone And Disc Necklace</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>twentyseven</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>2</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-disc-necklace</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
           <t>studiohop</t>
         </is>
       </c>
-      <c r="E89" t="n">
-        <v>3</v>
-      </c>
-      <c r="F89" t="inlineStr">
+      <c r="E91" t="n">
+        <v>2</v>
+      </c>
+      <c r="F91" t="inlineStr">
         <is>
           <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G91" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-09-01T01:37:56Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,18 +473,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>102177</t>
+          <t>1014560</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Personalised Cotton Or Linen Napkin</t>
+          <t>Personalised Book Style Novel Notebook</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>bigstitch</t>
+          <t>marthabrook</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -492,30 +492,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bigstitch/product/personalised-white-linen-napkin</t>
+          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-book-style-novel-notebook</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=102177&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1014560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1039459</t>
+          <t>1019263</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Personalised Wedding Day Celebration Card</t>
+          <t>1955 70th Birthday Sixpence Teardrop Locket Necklace</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-celebration-card</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/1951-70th-birthday-sixpence-teardrop-locket-necklace</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039459&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019263&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1053070</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Birth Flower Scarf And Card In A Gift Box</t>
+          <t>Map Engagement Card</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>lisamariedesigns</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/birth-flower-scarf-and-card-in-a-gift-box</t>
+          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053070&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1071124</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Personalised Couples Heart Wedding Gift Chopping Board</t>
+          <t>Star Sign Constellation Earrings Studs</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-couples-heart-wedding-gift-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1071124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1084447</t>
+          <t>1053446</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Engagement Gift Personalised Proposal Location Print</t>
+          <t>August Birthstone Bracelet Peridot</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>monoscape</t>
+          <t>indivijewels</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/monoscape/product/engagement-gift-personalised-proposal-location-print</t>
+          <t>https://www.notonthehighstreet.com/indivijewels/product/august-birthstone-bracelet-peridot</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1084447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053446&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1130264</t>
+          <t>1062225</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Family Bench Pebble Picture</t>
+          <t>Personalised Child's Name Unicorn School Pencil Case</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>alphabetbespokecreations</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-family-bench-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/alphabetbespokecreations/product/personalised-child-s-name-unicorn-school-pencil-case</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130264&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062225&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1130576</t>
+          <t>1076391</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Personalised Burnt Orange To Grey Cashmere Blend Scarf</t>
+          <t>Adjustable Personalised Ring</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>raspberryripplejewellery</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,30 +678,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-and-grey-colour-block-scarf</t>
+          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1143803</t>
+          <t>1078657</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Plantable Wedding Card And Plant A Tree</t>
+          <t>Personalised Orange To Grey Cashmere Mix Blanket Scarf</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>cardbee</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,30 +709,30 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cardbee/product/personalised-plantable-wedding-card-and-plant-a-tree</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-to-lilic-blanket-scarf</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1143803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1078657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1147645</t>
+          <t>1130576</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mouse Opening Red Door Fairy Garden Decoration With Bag</t>
+          <t>Personalised Burnt Orange To Grey Cashmere Blend Scarf</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>animalcrackers</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,30 +740,30 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/animalcrackers/product/cute-mouse-opening-red-door-fairy-garden-decoration</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-and-grey-colour-block-scarf</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1147645&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1154129</t>
+          <t>1145453</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Personalised Pet Memorial Decoration</t>
+          <t>Meadow Flower Print Scarf</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>laurastanleydesigns</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,61 +771,61 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/mothers-day-peony-navy-flower-scarf</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1145453&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1154598</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Delicate Tree Print Scarf</t>
+          <t>Personalised Road Sign</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/watercolour-butterflies-print-scarf</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1159266</t>
+          <t>1152259</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Men's Personalised Brushed Stainless Steel Wide Spinner Ring - 8mm</t>
+          <t>Personalised Stainless Steel Pizza Cutter</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -833,61 +833,61 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-stainless-steel-wide-spinner-ring</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1159266&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1152471</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalised Birth Flower Stoneware Mug</t>
+          <t>Bright Enamel And Glass Stone Ring</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>lucentstudios</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-birth-flower-stoneware-mug</t>
+          <t>https://www.notonthehighstreet.com/lucentstudios/product/bright-enamel-and-glass-stone-ring</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1190985</t>
+          <t>1154129</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Personalised Birth Month Flower Printed Can Glass</t>
+          <t>Personalised Pet Memorial Decoration</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>propergoose</t>
+          <t>laurastanleydesigns</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -895,154 +895,154 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/propergoose/product/personalised-birth-month-flower-printed-can-glass</t>
+          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1190985&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1179458</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Long Wildflower Amazing Friend Trinket Dish</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1180755</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Christening Keepsake Gift Book Personalised For Baby</t>
+          <t>Personalised Wedding Pebble Picture</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>mymagicname</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mymagicname/product/christening-keepsake-gift-book-personalised-for-baby</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-swing-pebble-picture</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180755&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sterling Silver Twist Ball Dangly Earrings</t>
+          <t>Personalised Women's Technology Travel Case Gift</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>thatsnicethat</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-twist-ball-dangly-earrings</t>
+          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1211471</t>
+          <t>1187498</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sterling Silver Chunky Hoop Earrings</t>
+          <t>Personalised Brass Travellers Compass With Wooden Box</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>hurleyburley</t>
+          <t>jungley</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/18ct-gold-plated-or-sterling-silver-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/jungley/product/personalised-brass-travellers-compass-with-wooden-box</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187498&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1217412</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Blue Opal Spinner Ring - 5mm</t>
+          <t>Personalised Age And Name Happy Birthday Card</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,30 +1050,30 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-sterling-silver-opal-spinner-ring</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1217412&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1226971</t>
+          <t>1201876</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Wedding Anniversary Greeting Card</t>
+          <t>Personalised Blue Heritage Plaque</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>uniqueful</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1081,30 +1081,30 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-anniversary-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/uniqueful/product/personalised-blue-heritage-plaque</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1226971&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1201876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1232841</t>
+          <t>1210524</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Personalised Sterling Silver Jade Necklace</t>
+          <t>Mum To Be Gift</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>letterboxlove</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1112,92 +1112,92 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-silver-jade-teardrop-pendant-necklace</t>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/mum-to-be-gift</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232841&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210524&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1244120</t>
+          <t>1218093</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>50th Birthday Sterling Silver Bracelet</t>
+          <t>Birth Month Flower Earring Studs</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/50th-birthday-sterling-silver-bracelet</t>
+          <t>https://www.notonthehighstreet.com/attic/product/birth-month-flower-earring-studs</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244120&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218093&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1245502</t>
+          <t>1225863</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Daisy Stud Earrings - 10mm</t>
+          <t>Seaside Spaniel Print. Limited Edition Dog Lover's Gift</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>thetypecastgallery</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-and-yellow-gold-plated-daisy-earrings</t>
+          <t>https://www.notonthehighstreet.com/thetypecastgallery/product/seaside-spaniel-print-limited-edition-dog-lover-s-gift</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1225863&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1260374</t>
+          <t>1233585</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sterling Silver Blue Forget Me Not Stud Earrings - 5mm</t>
+          <t>Personalised Multi Photo Leather Case Keyring</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>creategiftlove</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1205,30 +1205,30 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-tiny-blue-flower-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/creategiftlove/product/personalised-multi-photo-leather-case-keyring</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1260374&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1233585&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1264171</t>
+          <t>1256697</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Personalised Leather Notebook Lined</t>
+          <t>1945 80th Birthday Sixpence Compact Mirror</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>hotdot</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1236,61 +1236,61 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-leather-notebook-a5-lined</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/1943-80th-birthday-sixpence-compact-mirror</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264171&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1256697&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1272569</t>
+          <t>1285581</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Personalised 21st Birthday Bracelet With Heart</t>
+          <t>Sterling Silver Beaded Huggie Hoop Earrings</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>penelopetom</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-birthday-bracelet</t>
+          <t>https://www.notonthehighstreet.com/penelopetom/product/silver-beaded-huggie-hoop-earrings</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285581&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1277156</t>
+          <t>1290730</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Milestone Birthday Personalised Terracotta Plant Pot</t>
+          <t>Personalised Vintage Map Picture With Stitched Heart</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>poshtottydesignscreates</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1298,30 +1298,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/milestone-birthday-personalised-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1297326</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Personalised Vintage Map Picture With Stitched Heart</t>
+          <t>Personalised Leather Double Pen Holder</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>poshtottydesignscreates</t>
+          <t>parkerandco</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,30 +1329,30 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
+          <t>https://www.notonthehighstreet.com/parkerandco/product/personalised-leather-double-pen-holder</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1297326&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1309827</t>
+          <t>1314334</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Personalised Baby Dungarees - Embroidered Baby Romper Gift For Newborn, Boy Or Girl</t>
+          <t>Personalised Insulated Dinosaur Bottle School Travel</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>cublifeclothing</t>
+          <t>cribstar</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1360,61 +1360,61 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cublifeclothing/product/personalised-baby-dungarees-romper-embroidered</t>
+          <t>https://www.notonthehighstreet.com/cribstar/product/personalised-insulated-dinosaur-bottle-school-travel</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1314334&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1320832</t>
+          <t>1315899</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sterling Silver Name Necklace</t>
+          <t>Personalised Pookie Kids Bottle School Travel Holidays</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>potiega</t>
+          <t>cribstar</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/potiega/product/sterling-silver-name-necklace</t>
+          <t>https://www.notonthehighstreet.com/cribstar/product/personalised-pookie-kids-bottle-school-travel-holidays</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1315899&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1330774</t>
+          <t>1325196</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sterling Silver Little Twinkle Stars Charm Anklet</t>
+          <t>Personalised Oak Memory Box</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>hotdot</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1422,92 +1422,92 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-little-twinkle-stars-charm-anklet</t>
+          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-oak-memory-box</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1330774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1325196&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1341083</t>
+          <t>1329122</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Personalised Golden Anniversary 50 Years Pebble Picture</t>
+          <t>You Did It Silver Plated Star Bracelet</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>letterboxlove</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-golden-anniversary-50-years-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/you-did-it-silver-plated-star-bracelet</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329122&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1341118</t>
+          <t>1362911</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Personalised Wedding Mr And Mrs Pebble Picture</t>
+          <t>Personalised Brownie Box</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>rubythecakeartist</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-mr-mrs-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341118&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1347117</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>60th Birthday 1965 Sixpence Coin Compact Mirror</t>
+          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>iconiccoasters</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,30 +1515,30 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/60th-birthday-1963-sixpence-coin-compact-mirror</t>
+          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1347156</t>
+          <t>1365394</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>70th Birthday 1955 Sixpence Coin Compact Mirror</t>
+          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1546,61 +1546,61 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/70th-birthday-1953-sixpence-coin-compact-mirror</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1362911</t>
+          <t>1368460</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Personalised Brownie Box</t>
+          <t>The Pasty And Cream Tea Hamper</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>rubythecakeartist</t>
+          <t>thecornishcompany</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
+          <t>https://www.notonthehighstreet.com/thecornishcompany/product/the-pasty-cream-tea-hamper</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1372560</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Personalised Tractor Keepsake Birthday Card</t>
+          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>noordinarygiftcompany</t>
+          <t>thewordshack</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1608,61 +1608,61 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/noordinarygiftcompany/product/personalised-tractor-keepsake-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1372931</t>
+          <t>1378157</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1985 Personalised 40th Ruby Wedding Anniversary Poster</t>
+          <t>Elephant Gift, 14th Ivory Anniversary Gift Idea</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>diamondrosegifts</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-40th-ruby-wedding-anniversary-poster</t>
+          <t>https://www.notonthehighstreet.com/diamondrosegifts/product/elephant-gift-14th-ivory-anniversary-gift-idea</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372931&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378157&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>1381518</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
+          <t>Personalised Dartington Party Prosecco Glass</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>loveloxlockets</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1670,30 +1670,30 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
+          <t>https://www.notonthehighstreet.com/loveloxlockets/product/personalised-dartington-party-prosecco-glass</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381518&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1378864</t>
+          <t>1387073</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Personalised Wedding Day Card Gold And White Floral</t>
+          <t>Sterling Silver Light Snake Chain - 16in To 28in</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>thedogscollarsuk</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1701,61 +1701,61 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thedogscollarsuk/product/personalised-wedding-day-card-gold-and-white-floral</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-light-snake-chain-necklace</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378864&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387073&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1387361</t>
+          <t>1390300</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>My Book Of Nursery Rhymes And Personalised Poems</t>
+          <t>Sterling Silver Paw Print Stud Earrings - 5mm</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>mygivenname</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/my-book-of-nursery-rhymes-personalised-poems</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-cat-paw-stud-earrings</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1390300&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1394107</t>
+          <t>1396397</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Personalised Leather Key Holder</t>
+          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>vidavida</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1763,61 +1763,61 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/vidavida/product/personalised-leather-key-holder</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1395590</t>
+          <t>1397711</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Personalised Where It All Began, Anniversary Gift Print</t>
+          <t>Sterling Silver Opal Droplet Drop Hook Earrings</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>hooddesignsco</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hooddesignsco/product/personalised-where-it-all-began-anniversary-gift-print</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/aqua-green-opal-droplet-hook-earrings</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395590&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397711&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1405402</t>
+          <t>1401131</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Jewellery Organiser With Personalised Handle Gift Set</t>
+          <t>Personalised Friends With Wine Pebble Picture</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>ladedaliving</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1825,123 +1825,123 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/jewellery-organiser-with-personalised-handle-gift-set</t>
+          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1405402&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1470924</t>
+          <t>1401135</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Adjustable Anklet Bracelet With Fish Charm</t>
+          <t>'You Did It' Sterling Silver Star Earrings</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>attic</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/adjustable-anklet-bracelet-with-fish-charm</t>
+          <t>https://www.notonthehighstreet.com/attic/product/you-did-it-sterling-silver-star-earrings</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470924&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401135&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1476087</t>
+          <t>1423447</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Spa Gift Box For Women</t>
+          <t>Men's Personalised Engraved Black Braided Leather Bracelet With Custom Engraving, Artisan Jewellery</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>hallby</t>
+          <t>forgeandfoundry</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hallby/product/spa-gift-box-for-women</t>
+          <t>https://www.notonthehighstreet.com/forgeandfoundry/product/men-s-personalised-engraved-black-braided-leather-bracelet</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1489678</t>
+          <t>1430471</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Birthday Gift Terracotta Plant Pot</t>
+          <t>Grow Your Own Birth Flowers Tin Personalised Name Gift</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>alphabetgifting</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/birthday-gift-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/alphabetgifting/product/grow-your-own-birth-flowers-tin-personalised-name-gift</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1489678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1500488</t>
+          <t>1439080</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Personalised Horse Charm Bracelet</t>
+          <t>Double Sided New Parent Decision Making Coin</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>nameitwhatyoulike</t>
+          <t>prettylittlepresents</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1949,30 +1949,30 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/nameitwhatyoulike/product/personalised-horse-pony-charm-bracelet</t>
+          <t>https://www.notonthehighstreet.com/prettylittlepresents/product/double-sided-new-parent-decision-making-coin</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1439080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1509775</t>
+          <t>1442063</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Beaded Bracelet</t>
+          <t>Sterling Silver Vintage Style Aqua Opal Stud Earrings</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>wishedfor</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1980,30 +1980,30 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/wishedfor/product/sterling-silver-birthstone-beaded-bracelet</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-vintage-style-aqua-opal-stud-earrings</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1442063&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1513080</t>
+          <t>1445138</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>To My Daughter Necklace - Heart Infinity Charm, Sterling Silver Jewellery Gift, Personalised Birthday Keepsake</t>
+          <t>Sterling Silver Mismatched Crab And Lobster Stud Earrings</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>lunity</t>
+          <t>silverrainsilver</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2011,24 +2011,24 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lunity/product/to-my-daughter-necklace-heart-infinity-charm-sterling-silver-jewellery-gift-personalised-birthday-keepsake</t>
+          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-mismatched-crab-and-lobster-stud-earrings</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1445138&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1514040</t>
+          <t>1446457</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Personalised BBQ Serving Tray</t>
+          <t>Personalised Children's Gaming Snack Bowl</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -2038,127 +2038,127 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-bbq-serving-tray</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-children-s-gaming-snack-bowl</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1514805</t>
+          <t>1463308</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Guinness Lover's Gift Hamper With Chocolate And Snacks</t>
+          <t>Soft Cuddly Giant Handwarmer Hootie The Owl</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>bottleinabox</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bottleinabox/product/guinness-lover-s-gift-hamper-with-chocolate-snacks</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/soft-cuddly-giant-handwarmer-hootie-the-owl</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>255970</t>
+          <t>1482438</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>White Sleeveless Cotton Nightdress Lizzie</t>
+          <t>The Spa Self Care Gift Box</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>indulgenthampersuk</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
+          <t>https://www.notonthehighstreet.com/indulgenthampersuk/product/the-spa-self-care-gift-box</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482438&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1492175</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Rose Bouquet Personalised Card</t>
+          <t>Personalised Back Embroidered Childrens Cricket Jumper</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>karriebarroncards</t>
+          <t>toffeemoon</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
+          <t>https://www.notonthehighstreet.com/toffeemoon/product/personalised-back-embroidered-childrens-cricket-jumper</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1492175&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>307533</t>
+          <t>1494901</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Personalised Entwined Letters Wedding Card</t>
+          <t>Personalised Kingsbridge Floral Autumn Wreath</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>hickorydickory</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2166,30 +2166,30 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hickorydickory/product/personalised-wedding-card</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-kingsbridge-floral-wreath</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=307533&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>330009</t>
+          <t>1494976</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Personalised Papercut Wedding Card</t>
+          <t>Personalised Winthorpe Floral Wreath</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>pogofandango</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2197,30 +2197,30 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/pogofandango/product/personalised-papercut-wedding-card</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=330009&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>355476</t>
+          <t>1501314</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Vintage Cast Iron Heart Shaped Bird Seed Feeder</t>
+          <t>Personalised Watercolour Portrait From Photo - Custom Couple Illustration</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>selections</t>
+          <t>acdxlimited</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2228,30 +2228,30 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/selections/product/decorative-cow-solar-light-ornament</t>
+          <t>https://www.notonthehighstreet.com/acdxlimited/product/personalised-watercolour-portrait-from-photo-custom-couple-illustration</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355476&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>421466</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Peridot Quartz Drop Earrings</t>
+          <t>Personalised Sofa Snacks Enamel Bowl</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>sarahhickeyjewellery</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2259,30 +2259,30 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sarahhickeyjewellery/product/parrot-green-quartz-drop-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-sofa-snacks-enamel-bowl</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>433785</t>
+          <t>1512882</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>White Cotton Short Sleeve Nightdress 18th Century</t>
+          <t>Milestone Birthday Gift Terracotta Plant Pot</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>minilunn</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2290,30 +2290,30 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/18th-century-cotton-nightdress</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/milestone-birthday-gift-terracotta-plant-pot</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=433785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>455532</t>
+          <t>1513080</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Personalised Solid Brass Cufflinks</t>
+          <t>To My Daughter Necklace - Heart Infinity Charm, Sterling Silver Jewellery Gift, Personalised Birthday Keepsake</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>mangunbear</t>
+          <t>lunity</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2321,30 +2321,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/mangunbear/product/solid-brass-cufflinks</t>
+          <t>https://www.notonthehighstreet.com/lunity/product/to-my-daughter-necklace-heart-infinity-charm-sterling-silver-jewellery-gift-personalised-birthday-keepsake</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=455532&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>482198</t>
+          <t>1514040</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Busy Butterfly, Bee, Bug And Beneficial Insect Habitat</t>
+          <t>Personalised BBQ Serving Tray</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>selections</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2352,30 +2352,30 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/selections/product/pollinating-bee-nesting-log</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-bbq-serving-tray</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=482198&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>488356</t>
+          <t>1519450</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sterling Silver Secret Message Ring</t>
+          <t>Personalised Birthday Card For Daughter Heartfelt Message</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>marthajackson</t>
+          <t>thestamfordstudio</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2383,92 +2383,92 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-secret-message-ring</t>
+          <t>https://www.notonthehighstreet.com/thestamfordstudio/product/personalised-birthday-card-for-daughter-heartfelt-message</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=488356&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1519450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1526108</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
+          <t>Personalised 2nd Anniversary Cushion</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>twentyseven</t>
+          <t>arrowgiftco</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
+          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-2nd-anniversary-cushion</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1526108&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>565722</t>
+          <t>1527148</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Wedding Anniversary Family Art Print</t>
+          <t>Customisable First Day Of School Card For Girls</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>homegrownprintco</t>
+          <t>lunella</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/homegrownprintco/product/wedding-anniversary-family-art-print</t>
+          <t>https://www.notonthehighstreet.com/lunella/product/customisable-first-day-of-school-card-for-girls</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=565722&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1527148&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>568444</t>
+          <t>1527396</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Men's Plaited Leather Personalised Clasp Bracelet</t>
+          <t>Customisable First Day Of Secondary School Card For Girls</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>hurleyburleyman</t>
+          <t>lunella</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2476,61 +2476,61 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/limited-edition-personalised-clasp-bracelet</t>
+          <t>https://www.notonthehighstreet.com/lunella/product/customisable-first-day-of-secondary-school-year-7-card-for-girls</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=568444&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1527396&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>631040</t>
+          <t>255970</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Silver Friendship Knot Earrings</t>
+          <t>White Sleeveless Cotton Nightdress Lizzie</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>sophiejonesjewellery</t>
+          <t>minilunn</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/silver-friendship-knot-earrings</t>
+          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>647568</t>
+          <t>261422</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Girl's Personalised Sterling Silver Flower Necklace</t>
+          <t>Personalised Silk And Sterling Silver Charm Bangle</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>hurleyburleyjunior</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2538,30 +2538,30 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/girl-s-personalised-sterling-silver-flower-necklace</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/silk-silver-bangle</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=647568&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=261422&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>655071</t>
+          <t>355588</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ginge The Cat, Cuddly Companion Soft Toy</t>
+          <t>Personalised Typewriter Pop Up Card</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>jomanda</t>
+          <t>paperfiction</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2569,61 +2569,61 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jomanda/product/cuddly-soft-plush-cat</t>
+          <t>https://www.notonthehighstreet.com/paperfiction/product/typewriter-pop-up-card</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=655071&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>712893</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Personalised Pearl Sterling Silver Slide Bracelet</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/personalised-pearl-sterling-silver-slide-bracelet</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=712893&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>713987</t>
+          <t>490141</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Personalised 'Year' Unisex Sweatshirt</t>
+          <t>Brown/Yellow Hen</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>rockonruby</t>
+          <t>theneweden</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2631,30 +2631,30 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/rockonruby/product/personalised-year-sweatshirt</t>
+          <t>https://www.notonthehighstreet.com/theneweden/product/yellow-hen</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=713987&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=490141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>738289</t>
+          <t>533780</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Personalised Head Chef Apron, Cooking Gift</t>
+          <t>Girl's Personalised Sterling Silver Ball Bracelet</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>weaselandstoat</t>
+          <t>hurleyburleyjunior</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2662,123 +2662,123 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
+          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/girl-s-personalised-sterling-silver-ball-bracelet</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533780&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>764045</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Personalised Birthstone Disc Stretch Bracelet</t>
+          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>joybycorrinesmith</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-disc-stretch-bracelet</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>554644</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
+          <t>Personalised Birthstone Charm Bracelet</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>therusticdish</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-charm-bracelet</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=554644&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
+          <t>Nursery Rhymes And Personalised Poems Book</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>gaamaa</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>793008</t>
+          <t>738289</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Personalised Rainbow And Flower Bracelet Making Kit</t>
+          <t>Personalised Head Chef Apron, Cooking Gift</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>cottontwist</t>
+          <t>weaselandstoat</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2786,30 +2786,30 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cottontwist/product/personalised-rainbow-flower-power-bracelet-making-kit</t>
+          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=793008&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>804990</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Personalised Enamel Snack Pot</t>
+          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2817,30 +2817,30 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-enamel-snack-pot</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>806693</t>
+          <t>770318</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Personalised School Bag Tag Or Badge</t>
+          <t>Personalised 21st Necklace With Birthstone</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>evanslylane</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2848,148 +2848,148 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/evanslylane/product/personalised-school-bag-tag-or-badge</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=806693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>807430</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Carson The Lion, Newborn Baby Companion</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>bankslyonbotanical</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/carson-the-lion-from-birth-soft-toy</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=807430&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>830584</t>
+          <t>801933</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>60th Birthday 1965 Sixpence Coin Bangle Bracelet</t>
+          <t>Personalised Pull Out Photo Album Token Gift</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>ellieellie</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ellieellie/product/sixpence-1958-60th-birthday-coin-bangle-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=830584&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>837190</t>
+          <t>820333</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Dinosaur Glow In The Dark T Shirt</t>
+          <t>Newcastle Illustrated Black And White Tea Towel</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>glowgalaxyart</t>
+          <t>marthamitchelldesign</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/glowgalaxyart/product/glow-in-the-dark-dinosaur-t-shirt</t>
+          <t>https://www.notonthehighstreet.com/marthamitchelldesign/product/newcastle-illustrated-black-and-white-cotton-tea-towel</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=837190&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=820333&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>828616</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
+          <t>Personalised Wedding Anniversary Bottle Gift Bag</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>modocreative</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
+          <t>https://www.notonthehighstreet.com/modocreative/product/personalised-wedding-anniversary-bottle-gift-bag</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>879692</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Light Weight Wool Mix Poncho</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -3003,30 +3003,30 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/light-weight-wool-mix-poncho</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>886944</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Personalised Leather And Silver St Christopher Bracelet</t>
+          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>hurleyburleyman</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -3034,30 +3034,30 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyman/product/personalised-leather-and-silver-st-christopher-bracelet</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=886944&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>899547</t>
+          <t>866984</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Sterling Silver 18th Birthday Bracelet</t>
+          <t>Sterling Silver Infinity Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>yatrishomeandgift</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -3065,61 +3065,61 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/yatrishomeandgift/product/18th-birthday-bracelet-gift</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-infinity-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=899547&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866984&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>868202</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Birthstone Bracelet</t>
+          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birthstone-bracelet</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>927522</t>
+          <t>871844</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Personalised Aluminium Metal Photo Booth Bookmark</t>
+          <t>Personalised Bar Keyring</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>atypeofdesign</t>
+          <t>lovethelinks</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -3127,61 +3127,61 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/atypeofdesign/product/personalised-aluminium-metal-photo-booth-book-mark</t>
+          <t>https://www.notonthehighstreet.com/lovethelinks/product/dads-personalised-bar-keyring</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=927522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=871844&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>954762</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Turquoise Drop Hoop Earrings</t>
+          <t>Personalised Birth Flower Scarf</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>junkjewels</t>
+          <t>theforestandco</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/junkjewels/product/turquoise-drop-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=954762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>982044</t>
+          <t>880642</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Vintage 21st/30th/40th/50th/60th/70th Birthday Tshirt</t>
+          <t>Engraved Personalised Stoneware Mug</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>jolly</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -3189,74 +3189,291 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jolly/product/milestone-birthday-30th-40th-50th-60th-vintage-tshirt</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pink-stoneware-mug</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>991741</t>
+          <t>915034</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Personalised Swarovski Birthstone And Disc Necklace</t>
+          <t>Personalised Wedding Day / First Anniversary Card</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>twentyseven</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-disc-necklace</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>915286</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Personalised Rose Gold Foil Birth Flower Scarf</t>
+          <t>Engraved Birth Flower Plant Pot Birthday Gift For Her</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
+          <t>letterfest</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>2</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/letterfest/product/engraved-birthflower-plant-pot</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>920040</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Personalised Snack Bowl</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>sophiavictoriajoy</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>3</v>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-snack-bowl</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Dandelion Foil Birthday Gift Scarf</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
           <t>studiohop</t>
         </is>
       </c>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-rose-gold-foil-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+      <c r="E93" t="n">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>939529</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Forget Me Not Letterbox Gift</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>melissachoroszewskaceramics</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/melissachoroszewskaceramics/product/forget-me-not-letterbox-gift</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939529&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>963408</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>September Birthstone Bracelet Sapphire</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>indivijewels</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>2</v>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/indivijewels/product/september-birthstone-bracelet-sapphire</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=963408&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>976980</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Personalised Wedding Or Anniversary Flower Pot</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>letterfest</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>3</v>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-anniversary-flower-pot</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>982044</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Vintage 21st/30th/40th/50th/60th/70th Birthday Tshirt</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>jolly</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/jolly/product/milestone-birthday-30th-40th-50th-60th-vintage-tshirt</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>999606</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Personalised Chocolate Treats Bowl</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>sophiavictoriajoy</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-chocolate-treats-bowl</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-09-08T01:24:44Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -504,18 +504,18 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1019263</t>
+          <t>1039459</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1955 70th Birthday Sixpence Teardrop Locket Necklace</t>
+          <t>Personalised Wedding Day Celebration Card</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>sascreative</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -523,30 +523,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/1951-70th-birthday-sixpence-teardrop-locket-necklace</t>
+          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-celebration-card</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019263&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039459&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1104597</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Map Engagement Card</t>
+          <t>Personalised Vintage Copper Garden Bucket Planter</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lisamariedesigns</t>
+          <t>dibor</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -554,30 +554,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisamariedesigns/product/blossom-map-card-any-location</t>
+          <t>https://www.notonthehighstreet.com/dibor/product/personalised-vintage-copper-garden-bucket-planter</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1104597&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1154280</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Star Sign Constellation Earrings Studs</t>
+          <t>Personalised Oak Road Sign Style Plaque</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>madeforyougifts</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -585,30 +585,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/constellation-earrings-studs</t>
+          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-oak-road-sign-style-plaque</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154280&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1053446</t>
+          <t>1208246</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>August Birthstone Bracelet Peridot</t>
+          <t>Couples Anniversary Lantern With Gift</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>indivijewels</t>
+          <t>ingravia</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -616,30 +616,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/indivijewels/product/august-birthstone-bracelet-peridot</t>
+          <t>https://www.notonthehighstreet.com/ingravia/product/couples-anniversary-lantern-with-gift</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053446&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1208246&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1062225</t>
+          <t>1218428</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Personalised Child's Name Unicorn School Pencil Case</t>
+          <t>Personalised 18th Birthday Card Wooden Number Gift</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>alphabetbespokecreations</t>
+          <t>craftheaven</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -647,30 +647,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetbespokecreations/product/personalised-child-s-name-unicorn-school-pencil-case</t>
+          <t>https://www.notonthehighstreet.com/craftheaven/product/personalised-18th-birthday-card-wooden-number-gift</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062225&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218428&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1076391</t>
+          <t>1234302</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Adjustable Personalised Ring</t>
+          <t>Personalised Insulated Steel Water Bottle</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>raspberryripplejewellery</t>
+          <t>cribstar</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -678,30 +678,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/raspberryripplejewellery/product/adjustable-personalised-ring</t>
+          <t>https://www.notonthehighstreet.com/cribstar/product/personalised-insulated-steel-water-bottle</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1234302&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1078657</t>
+          <t>1257326</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Personalised Orange To Grey Cashmere Mix Blanket Scarf</t>
+          <t>Columbian Cross Body Bag</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>goodeehoo</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,30 +709,30 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-to-lilic-blanket-scarf</t>
+          <t>https://www.notonthehighstreet.com/goodeehoo/product/columbian-cross-body-bag</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1078657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1257326&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1130576</t>
+          <t>1263659</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Personalised Burnt Orange To Grey Cashmere Blend Scarf</t>
+          <t>Blooming Floral Compact Mirror</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>theforestandco</t>
+          <t>lisaangeljewellery</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -740,30 +740,30 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-orange-and-grey-colour-block-scarf</t>
+          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/blooming-floral-compact-mirror</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130576&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1263659&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1145453</t>
+          <t>1277784</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Meadow Flower Print Scarf</t>
+          <t>Personalised Sterling Silver St Christopher Necklace</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>songsofinkandsteel</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -771,61 +771,61 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/mothers-day-peony-navy-flower-scarf</t>
+          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/personalised-large-st-christopher-necklace</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1145453&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1150628</t>
+          <t>1329122</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personalised Road Sign</t>
+          <t>You Did It Silver Plated Star Bracelet</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>madeforyougifts</t>
+          <t>letterboxlove</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/madeforyougifts/product/personalised-metal-road-sign</t>
+          <t>https://www.notonthehighstreet.com/letterboxlove/product/you-did-it-silver-plated-star-bracelet</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329122&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1152259</t>
+          <t>1329904</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Personalised Stainless Steel Pizza Cutter</t>
+          <t>Colourful Fancy Cats Scarf</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>oakdenedesigns</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -833,154 +833,154 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-stainless-steel-pizza-cutter</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/colourful-fancy-cats-scarf</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329904&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1152471</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bright Enamel And Glass Stone Ring</t>
+          <t>Ladies Sterling Silver Or Gold Mesh Bracelet</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>lucentstudios</t>
+          <t>hurleyburley</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lucentstudios/product/bright-enamel-and-glass-stone-ring</t>
+          <t>https://www.notonthehighstreet.com/hurleyburley/product/ladies-sterling-silver-mesh-bracelet</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1154129</t>
+          <t>1350786</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Personalised Pet Memorial Decoration</t>
+          <t>Fuck Cancer Sterling Silver Morse Code Bracelet</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>laurastanleydesigns</t>
+          <t>charlieboots</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/laurastanleydesigns/product/personalised-pet-memorial-decoration</t>
+          <t>https://www.notonthehighstreet.com/charlieboots/product/fuck-cancer-sterling-silver-morse-code-bracelet</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350786&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1179458</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Long Wildflower Amazing Friend Trinket Dish</t>
+          <t>Fabric Name Peekaboo Memory Box</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>lisaangeljewellery</t>
+          <t>modocreative</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lisaangeljewellery/product/long-wildflower-amazing-friend-trinket-dish</t>
+          <t>https://www.notonthehighstreet.com/modocreative/product/fabric-peekaboo-keepsake-box</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1180755</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Personalised Wedding Pebble Picture</t>
+          <t>F1 Formula One 2025 / 2026 Calendar Track T Shirt Gift For Him</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>nappyhead</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-wedding-swing-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/nappyhead/product/formula-1-track-t-shirt-gift-for-him</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180755&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1389021</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Personalised Women's Technology Travel Case Gift</t>
+          <t>1st Birthday Book Of Nursery Rhymes And Poems</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>thatsnicethat</t>
+          <t>mygivenname</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -988,61 +988,61 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thatsnicethat/product/personalised-women-s-technology-travel-case-gift</t>
+          <t>https://www.notonthehighstreet.com/mygivenname/product/1st-birthday-book-of-nursery-rhymes-and-poems</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1187498</t>
+          <t>1408015</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Personalised Brass Travellers Compass With Wooden Box</t>
+          <t>Personalised 10th Tin Anniversary Origami Heart Card</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>jungley</t>
+          <t>helloruth</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/jungley/product/personalised-brass-travellers-compass-with-wooden-box</t>
+          <t>https://www.notonthehighstreet.com/helloruth/product/personalised-10th-tin-anniversary-origami-heart-card</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1187498&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1408015&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1420726</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Personalised Age And Name Happy Birthday Card</t>
+          <t>Personalised Metal Music Sheet Page Holder</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>sascreative</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1050,61 +1050,61 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-age-and-name-happy-birthday-card</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-music-sheet-page-holder</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1420726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1201876</t>
+          <t>1435726</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Personalised Blue Heritage Plaque</t>
+          <t>Funny I May Be Wrong Men's Cotton T Shirt</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>uniqueful</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniqueful/product/personalised-blue-heritage-plaque</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/funny-i-may-be-wrong-men-s-t-shirt</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1201876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1210524</t>
+          <t>1463308</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Mum To Be Gift</t>
+          <t>Soft Cuddly Giant Handwarmer Hootie The Owl</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>letterboxlove</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1112,30 +1112,30 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterboxlove/product/mum-to-be-gift</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/soft-cuddly-giant-handwarmer-hootie-the-owl</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1210524&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1218093</t>
+          <t>1470941</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Birth Month Flower Earring Studs</t>
+          <t>Porcelain Bird Earrings French Vintage Charm</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1143,30 +1143,30 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/birth-month-flower-earring-studs</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-earrings-french-vintage-charm</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218093&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1470941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1225863</t>
+          <t>1477967</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Seaside Spaniel Print. Limited Edition Dog Lover's Gift</t>
+          <t>The Eye Cream + Eye Roller Duo</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>thetypecastgallery</t>
+          <t>upcircle</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1174,30 +1174,30 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thetypecastgallery/product/seaside-spaniel-print-limited-edition-dog-lover-s-gift</t>
+          <t>https://www.notonthehighstreet.com/upcircle/product/the-eye-cream-eye-roller-duo</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1225863&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1477967&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1233585</t>
+          <t>1478384</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Personalised Multi Photo Leather Case Keyring</t>
+          <t>40th Birthday Card With 1985 Coin And Envelope Choose Your Colour</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>creategiftlove</t>
+          <t>coingiftshop</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1205,30 +1205,30 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/creategiftlove/product/personalised-multi-photo-leather-case-keyring</t>
+          <t>https://www.notonthehighstreet.com/coingiftshop/product/40th-birthday-card-with-1985-coin-and-envelope-choose-your-colour</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1233585&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478384&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1256697</t>
+          <t>1478462</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1945 80th Birthday Sixpence Compact Mirror</t>
+          <t>1955 70th Birthday Sixpence Coin Keyring Gift</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>charlieboots</t>
+          <t>coingiftshop</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1236,61 +1236,61 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/charlieboots/product/1943-80th-birthday-sixpence-compact-mirror</t>
+          <t>https://www.notonthehighstreet.com/coingiftshop/product/personalised-1955-70th-birthday-sixpence-keyring-gift</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1256697&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478462&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1285581</t>
+          <t>1478663</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sterling Silver Beaded Huggie Hoop Earrings</t>
+          <t>Porcelain Bird French Vintage Charm Bracelet</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>penelopetom</t>
+          <t>uniques</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/penelopetom/product/silver-beaded-huggie-hoop-earrings</t>
+          <t>https://www.notonthehighstreet.com/uniques/product/porcelain-bird-french-vintage-charm-bracelet</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1285581&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1485087</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Personalised Vintage Map Picture With Stitched Heart</t>
+          <t>Belgian Milk Chocolate Tractor</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>poshtottydesignscreates</t>
+          <t>thegourmetchocolatepizzaco</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1298,30 +1298,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/poshtottydesignscreates/product/personalised-vintage-map-picture-with-stitched-heart</t>
+          <t>https://www.notonthehighstreet.com/thegourmetchocolatepizzaco/product/belgian-milk-chocolate-tractor</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1485087&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1297326</t>
+          <t>1490581</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Personalised Leather Double Pen Holder</t>
+          <t>Pet Portrait Gift Hand Drawn Illustration</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>parkerandco</t>
+          <t>acdxlimited</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1329,30 +1329,30 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/parkerandco/product/personalised-leather-double-pen-holder</t>
+          <t>https://www.notonthehighstreet.com/acdxlimited/product/pet-portrait</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1297326&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1490581&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1314334</t>
+          <t>1491159</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Personalised Insulated Dinosaur Bottle School Travel</t>
+          <t>Gold Or Silver Personalised Boarding Pass</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>cribstar</t>
+          <t>therusticdish</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1360,30 +1360,30 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cribstar/product/personalised-insulated-dinosaur-bottle-school-travel</t>
+          <t>https://www.notonthehighstreet.com/therusticdish/product/gold-or-silver-personalised-boarding-pass</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1314334&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491159&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1315899</t>
+          <t>1499456</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Personalised Pookie Kids Bottle School Travel Holidays</t>
+          <t>Personalised Couple Hand Heart Acrylic Block - Romantic Gift For Anniversary, Engagement, Wedding, Valentine's Day</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>cribstar</t>
+          <t>personalisedbee</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1391,30 +1391,30 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/cribstar/product/personalised-pookie-kids-bottle-school-travel-holidays</t>
+          <t>https://www.notonthehighstreet.com/personalisedbee/product/personalised-couple-hand-heart-acrylic-block-romantic-gift-for-anniversary-engagement-wedding-valentine-s-day</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1315899&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1325196</t>
+          <t>1502178</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Personalised Oak Memory Box</t>
+          <t>Personalised Song Lyrics Print - Wedding Anniversary Gift For Couples</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>hotdot</t>
+          <t>vintagedesignsreborn</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1422,92 +1422,92 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/hotdot/product/personalised-oak-memory-box</t>
+          <t>https://www.notonthehighstreet.com/vintagedesignsreborn/product/personalised-song-lyrics-print-wedding-anniversary-gift-for-couples</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1325196&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1329122</t>
+          <t>1508460</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>You Did It Silver Plated Star Bracelet</t>
+          <t>Personalised Saturday Night Snacks Bowl</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>letterboxlove</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/letterboxlove/product/you-did-it-silver-plated-star-bracelet</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-saturday-night-snacks-bowl</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329122&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1362911</t>
+          <t>1513439</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Personalised Brownie Box</t>
+          <t>Children's Baptism Christening Or Holy Communion Sterling Silver Cross Bracelet Gift</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>rubythecakeartist</t>
+          <t>matildamoonjewellery</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/rubythecakeartist/product/personalised-brownie-box</t>
+          <t>https://www.notonthehighstreet.com/matildamoonjewellery/product/children-s-christening-or-holy-communion-bracelet-gift</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1362911&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513439&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Personalised 60th Birthday Coaster Gift For Him Or Her</t>
+          <t>Soft Cuddly Giant Handwarmer Henry The Hedgehog</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>iconiccoasters</t>
+          <t>thelyndoncompany</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1515,30 +1515,30 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/iconiccoasters/product/personalised-60th-birthday-coaster-gift-for-him-or-her</t>
+          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/soft-cuddly-giant-handwarmer-henry-the-hedgehog</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1365394</t>
+          <t>1525519</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Boho Jewellery Gift Set Layered Earrings And Necklace</t>
+          <t>Handmade Wedding Day Card, Romantic Bride And Groom Design</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>uniques</t>
+          <t>littlesentiments</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1546,30 +1546,30 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/uniques/product/boho-jewellery-gift-set-layered-earrings-necklace</t>
+          <t>https://www.notonthehighstreet.com/littlesentiments/product/handmade-wedding-day-card-romanic-bride-and-groom-design</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1525519&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1368460</t>
+          <t>258510</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>The Pasty And Cream Tea Hamper</t>
+          <t>'You Are Capable Of Amazing Things' Star Keyring</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>thecornishcompany</t>
+          <t>kutuu</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1577,92 +1577,92 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thecornishcompany/product/the-pasty-cream-tea-hamper</t>
+          <t>https://www.notonthehighstreet.com/kutuu/product/star-for-success-keyring</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1368460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=258510&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Personalised 1st Paper Wedding Anniversary Poster Gift</t>
+          <t>Rose Bouquet Personalised Card</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>thewordshack</t>
+          <t>karriebarroncards</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thewordshack/product/personalised-1st-paper-wedding-anniversary-poster-gift</t>
+          <t>https://www.notonthehighstreet.com/karriebarroncards/product/personalised-12-roses-bouquet-3-d-greeting-card</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1378157</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Elephant Gift, 14th Ivory Anniversary Gift Idea</t>
+          <t>Personalised Metal Street Sign</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>diamondrosegifts</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/diamondrosegifts/product/elephant-gift-14th-ivory-anniversary-gift-idea</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-metal-street-sign</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378157&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1381518</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Personalised Dartington Party Prosecco Glass</t>
+          <t>Sterling Silver April Shower Drop Earrings</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>loveloxlockets</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1670,61 +1670,61 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/loveloxlockets/product/personalised-dartington-party-prosecco-glass</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/silver-teardrop-earrings</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381518&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1387073</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Sterling Silver Light Snake Chain - 16in To 28in</t>
+          <t>Family Birthstone Link Bracelet</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>joybycorrinesmith</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-light-snake-chain-necklace</t>
+          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387073&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1390300</t>
+          <t>499724</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sterling Silver Paw Print Stud Earrings - 5mm</t>
+          <t>Sterling Silver Chains</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>songsofinkandsteel</t>
+          <t>marthajackson</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1732,30 +1732,30 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/songsofinkandsteel/product/sterling-silver-cat-paw-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/marthajackson/product/sterling-silver-chains</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1390300&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=499724&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1396397</t>
+          <t>508665</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sterling Silver And Gold Plated Adjustable Knot Ring</t>
+          <t>Personalised Exam Congratulations Or Graduation Card</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>myposhshop</t>
+          <t>millyandpip</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1763,185 +1763,185 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/sterling-silver-and-gold-plated-adjustable-knot-ring</t>
+          <t>https://www.notonthehighstreet.com/millyandpip/product/personalised-congratulations-star-card</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1396397&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=508665&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1397711</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sterling Silver Opal Droplet Drop Hook Earrings</t>
+          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>twentyseven</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/aqua-green-opal-droplet-hook-earrings</t>
+          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397711&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1401131</t>
+          <t>607975</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Personalised Friends With Wine Pebble Picture</t>
+          <t>Mineral Bath Infusions Gift Collection</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ladedaliving</t>
+          <t>bankslyonbotanical</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/ladedaliving/product/personalised-friends-with-wine-pebble-picture</t>
+          <t>https://www.notonthehighstreet.com/bankslyonbotanical/product/mineral-bath-infusions-gift-collection</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1401135</t>
+          <t>670166</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>'You Did It' Sterling Silver Star Earrings</t>
+          <t>Personalised Foiled Reasons I Love You Notes</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>attic</t>
+          <t>marthabrook</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/attic/product/you-did-it-sterling-silver-star-earrings</t>
+          <t>https://www.notonthehighstreet.com/marthabrook/product/personalised-foiled-reasons-i-love-you-notes</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401135&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=670166&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1423447</t>
+          <t>679514</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Men's Personalised Engraved Black Braided Leather Bracelet With Custom Engraving, Artisan Jewellery</t>
+          <t>Personalised Guitar Plectrums</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>forgeandfoundry</t>
+          <t>oakdenedesigns</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/forgeandfoundry/product/men-s-personalised-engraved-black-braided-leather-bracelet</t>
+          <t>https://www.notonthehighstreet.com/oakdenedesigns/product/personalised-guitar-plectrums</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=679514&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1430471</t>
+          <t>684433</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Grow Your Own Birth Flowers Tin Personalised Name Gift</t>
+          <t>Birth Flower Mandala Personalised Print</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>alphabetgifting</t>
+          <t>flossandco</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/alphabetgifting/product/grow-your-own-birth-flowers-tin-personalised-name-gift</t>
+          <t>https://www.notonthehighstreet.com/flossandco/product/birth-flower-mandala-personalised-birthday-print</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=684433&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1439080</t>
+          <t>758994</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Double Sided New Parent Decision Making Coin</t>
+          <t>Personalised Papercut Golden Wedding Anniversary Card</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>prettylittlepresents</t>
+          <t>pogofandango</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1949,92 +1949,92 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/prettylittlepresents/product/double-sided-new-parent-decision-making-coin</t>
+          <t>https://www.notonthehighstreet.com/pogofandango/product/personalised-papercut-golden-wedding-anniversary-card</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1439080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=758994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1442063</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sterling Silver Vintage Style Aqua Opal Stud Earrings</t>
+          <t>Sterling Silver Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-vintage-style-aqua-opal-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1442063&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1445138</t>
+          <t>801933</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sterling Silver Mismatched Crab And Lobster Stud Earrings</t>
+          <t>Personalised Pull Out Photo Album Token Gift</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>silverrainsilver</t>
+          <t>sophiavictoriajoy</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/silverrainsilver/product/sterling-silver-mismatched-crab-and-lobster-stud-earrings</t>
+          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1445138&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1446457</t>
+          <t>823762</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Personalised Children's Gaming Snack Bowl</t>
+          <t>70th Birthday Silver Necklace</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>sophiejonesjewellery</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -2042,61 +2042,61 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-children-s-gaming-snack-bowl</t>
+          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/70th-birthday-silver-necklace</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=823762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1463308</t>
+          <t>830584</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Soft Cuddly Giant Handwarmer Hootie The Owl</t>
+          <t>60th Birthday 1965 Sixpence Coin Bangle Bracelet</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>thelyndoncompany</t>
+          <t>ellieellie</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thelyndoncompany/product/soft-cuddly-giant-handwarmer-hootie-the-owl</t>
+          <t>https://www.notonthehighstreet.com/ellieellie/product/sixpence-1958-60th-birthday-coin-bangle-bracelet</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=830584&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1482438</t>
+          <t>846560</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>The Spa Self Care Gift Box</t>
+          <t>Personalised Train Ticket Wedding Card</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>indulgenthampersuk</t>
+          <t>oflifeandlemons</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2104,30 +2104,30 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/indulgenthampersuk/product/the-spa-self-care-gift-box</t>
+          <t>https://www.notonthehighstreet.com/oflifeandlemons/product/funny-brexit-valentine-s-card</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1482438&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=846560&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1492175</t>
+          <t>848232</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Personalised Back Embroidered Childrens Cricket Jumper</t>
+          <t>Personalised 60 Th Birthday Book 'Memory Lane'</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>toffeemoon</t>
+          <t>lucysworld</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2135,92 +2135,92 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/toffeemoon/product/personalised-back-embroidered-childrens-cricket-jumper</t>
+          <t>https://www.notonthehighstreet.com/lucysworld/product/personalised-60th-birthday-book-memory-lane</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1492175&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=848232&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1494901</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Personalised Kingsbridge Floral Autumn Wreath</t>
+          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>myposhshop</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-kingsbridge-floral-wreath</t>
+          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1494976</t>
+          <t>857801</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Personalised Winthorpe Floral Wreath</t>
+          <t>Personalised Birthstone Chain Bracelet</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>dibor</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/dibor/product/personalised-winthorpe-floral-wreath</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/gold-filled-birthstone-bracelet</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857801&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1501314</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Personalised Watercolour Portrait From Photo - Custom Couple Illustration</t>
+          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>acdxlimited</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2228,92 +2228,92 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/acdxlimited/product/personalised-watercolour-portrait-from-photo-custom-couple-illustration</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1508457</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Personalised Sofa Snacks Enamel Bowl</t>
+          <t>Silver Birthstone Adjustable Sliding Bracelet</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-sofa-snacks-enamel-bowl</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/birthstone-adjustable-sliding-bracelet</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1512882</t>
+          <t>866984</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Milestone Birthday Gift Terracotta Plant Pot</t>
+          <t>Sterling Silver Infinity Birthstone Sliding Bracelet</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>gaamaa</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/milestone-birthday-gift-terracotta-plant-pot</t>
+          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-infinity-birthstone-sliding-bracelet</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866984&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1513080</t>
+          <t>922319</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>To My Daughter Necklace - Heart Infinity Charm, Sterling Silver Jewellery Gift, Personalised Birthday Keepsake</t>
+          <t>21st Nickel Brass Anniversary Oak Initials Artwork</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>lunity</t>
+          <t>littlefoundry</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2321,30 +2321,30 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/lunity/product/to-my-daughter-necklace-heart-infinity-charm-sterling-silver-jewellery-gift-personalised-birthday-keepsake</t>
+          <t>https://www.notonthehighstreet.com/littlefoundry/product/21st-nickel-brass-anniversary-oak-initials-artwork</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513080&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=922319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1514040</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Personalised BBQ Serving Tray</t>
+          <t>Dandelion Foil Birthday Gift Scarf</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>sophiavictoriajoy</t>
+          <t>studiohop</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2352,30 +2352,30 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-bbq-serving-tray</t>
+          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1519450</t>
+          <t>944953</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Personalised Birthday Card For Daughter Heartfelt Message</t>
+          <t>Personalised Vinyl Record Storage Case</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>thestamfordstudio</t>
+          <t>steepletone</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2383,1097 +2383,12 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>https://www.notonthehighstreet.com/thestamfordstudio/product/personalised-birthday-card-for-daughter-heartfelt-message</t>
+          <t>https://www.notonthehighstreet.com/steepletone/product/steepletone-dad-s-vinyl-record-storage-case</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1519450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>1526108</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Personalised 2nd Anniversary Cushion</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>arrowgiftco</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
-        <v>2</v>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/arrowgiftco/product/personalised-2nd-anniversary-cushion</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1526108&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>1527148</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Customisable First Day Of School Card For Girls</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>lunella</t>
-        </is>
-      </c>
-      <c r="E65" t="n">
-        <v>4</v>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lunella/product/customisable-first-day-of-school-card-for-girls</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1527148&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>1527396</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Customisable First Day Of Secondary School Card For Girls</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>lunella</t>
-        </is>
-      </c>
-      <c r="E66" t="n">
-        <v>2</v>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lunella/product/customisable-first-day-of-secondary-school-year-7-card-for-girls</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1527396&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>255970</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>White Sleeveless Cotton Nightdress Lizzie</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>minilunn</t>
-        </is>
-      </c>
-      <c r="E67" t="n">
-        <v>4</v>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/minilunn/product/lizzie-cotton-embroidered-nightdress</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=255970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>261422</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Personalised Silk And Sterling Silver Charm Bangle</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>hurleyburley</t>
-        </is>
-      </c>
-      <c r="E68" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/hurleyburley/product/silk-silver-bangle</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=261422&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>355588</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Personalised Typewriter Pop Up Card</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>paperfiction</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/paperfiction/product/typewriter-pop-up-card</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=355588&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>469358</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Family Birthstone Link Bracelet</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>joybycorrinesmith</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>5</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/family-birthstone-link-bracelet</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>490141</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Brown/Yellow Hen</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>theneweden</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>2</v>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theneweden/product/yellow-hen</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=490141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>533780</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Girl's Personalised Sterling Silver Ball Bracelet</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>hurleyburleyjunior</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>2</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/hurleyburleyjunior/product/girl-s-personalised-sterling-silver-ball-bracelet</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=533780&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>545355</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Personalised Swarovski Birthstone And Initial Necklace</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>twentyseven</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>4</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/twentyseven/product/personalised-swarovski-birthstone-and-initial-necklace</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>554644</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Personalised Birthstone Charm Bracelet</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>joybycorrinesmith</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>2</v>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/joybycorrinesmith/product/personalised-birthstone-charm-bracelet</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=554644&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>610619</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Nursery Rhymes And Personalised Poems Book</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>mygivenname</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>2</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/mygivenname/product/nursery-rhymes-and-personalised-poems-book</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>738289</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Personalised Head Chef Apron, Cooking Gift</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>weaselandstoat</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
-        <v>2</v>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/weaselandstoat/product/personalised-head-chef-apron</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>764151</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Personalised Olive Wood Wedding Gift Chopping Board</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>therusticdish</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>2</v>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/therusticdish/product/personalised-couples-cheese-chopping-board</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>770318</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Personalised 21st Necklace With Birthstone</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>sophiejonesjewellery</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>2</v>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiejonesjewellery/product/personalised-21st-necklace-with-birthstone</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=770318&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Sterling Silver Birthstone Sliding Bracelet</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>gaamaa</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>3</v>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-birthstone-sliding-bracelet</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>801933</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Personalised Pull Out Photo Album Token Gift</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>sophiavictoriajoy</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>4</v>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pull-out-photo-album-token-gift</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>820333</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Newcastle Illustrated Black And White Tea Towel</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>marthamitchelldesign</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>2</v>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/marthamitchelldesign/product/newcastle-illustrated-black-and-white-cotton-tea-towel</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=820333&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>828616</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Anniversary Bottle Gift Bag</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>modocreative</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>2</v>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/modocreative/product/personalised-wedding-anniversary-bottle-gift-bag</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>856677</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Metallic Gold Mulberry Tree Of Life Scarf</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E83" t="n">
-        <v>4</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/silver-foil-tree-cotton-scarf</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>857942</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Personalised Choose Your 'Birth Flower' Scarf</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
-        <v>2</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/personalised-birth-flower-blanket-scarf</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>866984</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Sterling Silver Infinity Birthstone Sliding Bracelet</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>gaamaa</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
-        <v>2</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/gaamaa/product/sterling-silver-infinity-birthstone-sliding-bracelet</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866984&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>868202</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>60th Birthday Solid Sterling Silver Six Star Bracelet</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>myposhshop</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
-        <v>2</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/myposhshop/product/60th-birthday-solid-sterling-silver-six-star-bracelet</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=868202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>871844</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Personalised Bar Keyring</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>lovethelinks</t>
-        </is>
-      </c>
-      <c r="E87" t="n">
-        <v>2</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/lovethelinks/product/dads-personalised-bar-keyring</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=871844&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Personalised Birth Flower Scarf</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>theforestandco</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
-        <v>6</v>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/theforestandco/product/personalised-birth-flower-scarf</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>880642</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Engraved Personalised Stoneware Mug</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>sophiavictoriajoy</t>
-        </is>
-      </c>
-      <c r="E89" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-pink-stoneware-mug</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>915034</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Day / First Anniversary Card</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>sascreative</t>
-        </is>
-      </c>
-      <c r="E90" t="n">
-        <v>3</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sascreative/product/personalised-wedding-day-first-anniversary-card</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>915286</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Engraved Birth Flower Plant Pot Birthday Gift For Her</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>letterfest</t>
-        </is>
-      </c>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/engraved-birthflower-plant-pot</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>920040</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Personalised Snack Bowl</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>sophiavictoriajoy</t>
-        </is>
-      </c>
-      <c r="E92" t="n">
-        <v>3</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-snack-bowl</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Dandelion Foil Birthday Gift Scarf</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>studiohop</t>
-        </is>
-      </c>
-      <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/studiohop/product/thinking-of-you-dandelion-scarf-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>939529</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Forget Me Not Letterbox Gift</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>melissachoroszewskaceramics</t>
-        </is>
-      </c>
-      <c r="E94" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/melissachoroszewskaceramics/product/forget-me-not-letterbox-gift</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=939529&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>963408</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>September Birthstone Bracelet Sapphire</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>indivijewels</t>
-        </is>
-      </c>
-      <c r="E95" t="n">
-        <v>2</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/indivijewels/product/september-birthstone-bracelet-sapphire</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=963408&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>976980</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Personalised Wedding Or Anniversary Flower Pot</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>letterfest</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
-        <v>3</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/letterfest/product/personalised-anniversary-flower-pot</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=976980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>982044</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Vintage 21st/30th/40th/50th/60th/70th Birthday Tshirt</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>jolly</t>
-        </is>
-      </c>
-      <c r="E97" t="n">
-        <v>2</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/jolly/product/milestone-birthday-30th-40th-50th-60th-vintage-tshirt</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>999606</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Personalised Chocolate Treats Bowl</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>sophiavictoriajoy</t>
-        </is>
-      </c>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>https://www.notonthehighstreet.com/sophiavictoriajoy/product/personalised-chocolate-treats-bowl</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=944953&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-09-22T01:28:07Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1008277</t>
+          <t>1001803</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,14 +485,14 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1008277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1001803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1045351</t>
+          <t>1032833</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -504,14 +504,14 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1045351&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1032833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1053070</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,14 +523,14 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1053070&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1099391</t>
+          <t>1055749</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -542,14 +542,14 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1099391&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1055749&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1144592</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -561,14 +561,14 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1144592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1152259</t>
+          <t>1064283</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152259&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1064283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1152471</t>
+          <t>1067493</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,14 +599,14 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1152471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1174183</t>
+          <t>1103211</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -618,33 +618,33 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1174183&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1103211&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1105882</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1105882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1116330</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -656,33 +656,33 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116330&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1166154</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1166154&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1205131</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,71 +694,71 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1198294</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1232243</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232243&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1244126</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1244887</t>
+          <t>1216801</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1216801&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1244887</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1272569</t>
+          <t>1245502</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,33 +827,33 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1272569&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1276721</t>
+          <t>1246966</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1281098</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -865,14 +865,14 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1281098&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1290730</t>
+          <t>1276721</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -884,14 +884,14 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1292751</t>
+          <t>1277784</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -903,14 +903,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1292751&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1307482</t>
+          <t>1278270</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -922,14 +922,14 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307482&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278270&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1310483</t>
+          <t>1290018</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -941,109 +941,109 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1311546</t>
+          <t>1290822</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1314037</t>
+          <t>1307229</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1314037&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1320832</t>
+          <t>1309827</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1329904</t>
+          <t>1311546</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329904&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1347117</t>
+          <t>1313730</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1373754</t>
+          <t>1327791</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,14 +1055,14 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1373754&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1327791&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1376722</t>
+          <t>1341081</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1074,14 +1074,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1376722&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341081&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1378157</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1093,33 +1093,33 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378157&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1383055</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1383055&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1389021</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1131,14 +1131,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1404418</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,14 +1150,14 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404418&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1415074</t>
+          <t>1354241</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1169,14 +1169,14 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415074&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354241&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1423447</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1188,33 +1188,33 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1434609</t>
+          <t>1365394</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434609&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1444447</t>
+          <t>1367807</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1226,33 +1226,33 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1444447&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367807&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1478663</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1485292</t>
+          <t>1381151</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1264,14 +1264,14 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1485292&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1495667</t>
+          <t>1385257</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1283,14 +1283,14 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1495667&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1497564</t>
+          <t>1393774</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,14 +1302,14 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497564&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1393774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1502050</t>
+          <t>1401375</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1321,14 +1321,14 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502050&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401375&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1508460</t>
+          <t>1413835</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1340,52 +1340,52 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413835&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1518947</t>
+          <t>1415417</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1518947&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>1423284</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1525331</t>
+          <t>1429169</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1397,14 +1397,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1525331&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1429169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1526964</t>
+          <t>1435726</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1416,14 +1416,14 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1526964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1532903</t>
+          <t>1435900</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1435,90 +1435,90 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1532903&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>177216</t>
+          <t>1443868</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=177216&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>223922</t>
+          <t>1456319</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=223922&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1456324</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>352545</t>
+          <t>1478663</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=352545&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>1480366</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1530,14 +1530,14 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1480366&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>416277</t>
+          <t>1491098</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1549,90 +1549,90 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=416277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491098&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>462337</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=462337&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1491892</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491892&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1496067</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496067&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1500484</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>641782</t>
+          <t>1501319</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1644,14 +1644,14 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=641782&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>689570</t>
+          <t>1502178</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1663,33 +1663,33 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=689570&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>771561</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=771561&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>1508460</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1701,71 +1701,71 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>804990</t>
+          <t>1509775</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>809163</t>
+          <t>1514221</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=809163&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514221&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>1524741</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1777,33 +1777,33 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1524741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>1536005</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1536005&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>898196</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1815,33 +1815,33 @@
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=898196&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>905169</t>
+          <t>350209</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>905347</t>
+          <t>421238</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1853,33 +1853,33 @@
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=905347&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>948800</t>
+          <t>494513</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -1891,14 +1891,14 @@
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=948800&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=494513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>972488</t>
+          <t>512405</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1910,14 +1910,14 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=972488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>998918</t>
+          <t>519183</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -1929,7 +1929,596 @@
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=998918&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=519183&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>520238</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>2</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=520238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>545355</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>2</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>610619</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>4</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>618130</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>3</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=618130&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>621809</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>2</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>643101</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>2</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>686802</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=686802&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>695670</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>701970</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=701970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>709696</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>2</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=709696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>734979</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=734979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>758994</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>2</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=758994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>764045</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>3</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>2</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>782815</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=782815&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>786481</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>787890</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>3</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=787890&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>801933</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>3</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>804990</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>6</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>809110</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=809110&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>835857</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="n">
+        <v>2</v>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=835857&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>835860</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="n">
+        <v>2</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=835860&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>856677</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>866983</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="n">
+        <v>3</v>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="n">
+        <v>5</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>894796</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="n">
+        <v>2</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=894796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>908949</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="n">
+        <v>2</v>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=908949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="n">
+        <v>3</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>972488</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="n">
+        <v>3</v>
+      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=972488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>972490</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>2</v>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=972490&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>2</v>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-09-29T01:22:57Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1001803</t>
+          <t>1033142</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,14 +485,14 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1001803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033142&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1032833</t>
+          <t>1076105</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -504,14 +504,14 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1032833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1093803</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,14 +523,14 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1055749</t>
+          <t>1149454</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -542,14 +542,14 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1055749&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1149454&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1158522</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -561,14 +561,14 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1064283</t>
+          <t>1160257</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1064283&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1160257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1067493</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,14 +599,14 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1067493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1103211</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -618,14 +618,14 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1103211&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1105882</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -637,14 +637,14 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1105882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1116330</t>
+          <t>1244126</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -656,14 +656,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1116330&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1166154</t>
+          <t>1244887</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1166154&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,52 +694,52 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1198294</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1198294&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1276718</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1276721</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,14 +751,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1279706</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1279706&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1216801</t>
+          <t>1286365</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1216801&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1286365&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1244887</t>
+          <t>1296744</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296744&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1245502</t>
+          <t>1307482</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,109 +827,109 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245502&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307482&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1246966</t>
+          <t>1311546</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1320773</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320773&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1276721</t>
+          <t>1320832</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1277784</t>
+          <t>1329488</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1278270</t>
+          <t>1332189</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278270&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1290018</t>
+          <t>1345551</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -941,14 +941,14 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290018&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345551&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1290822</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -960,71 +960,71 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1307229</t>
+          <t>1347156</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1309827</t>
+          <t>1347160</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347160&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1311546</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1313730</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1036,14 +1036,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1313730&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1327791</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,33 +1055,33 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1327791&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1341081</t>
+          <t>1364165</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1341081&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364165&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1344943</t>
+          <t>1372919</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1093,33 +1093,33 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372919&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1373167</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1131,14 +1131,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1373167&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1375261</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,14 +1150,14 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1354241</t>
+          <t>1395308</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1169,14 +1169,14 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1354241&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1400456</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1188,33 +1188,33 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1365394</t>
+          <t>1401261</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1367807</t>
+          <t>1404799</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1226,14 +1226,14 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1367807&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404799&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>1415417</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1245,14 +1245,14 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1381151</t>
+          <t>1419090</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1264,14 +1264,14 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1381151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419090&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1385257</t>
+          <t>1441033</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1283,14 +1283,14 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1385257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1441033&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1393774</t>
+          <t>1446472</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,90 +1302,90 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1393774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446472&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1401375</t>
+          <t>1456324</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401375&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1413835</t>
+          <t>1475693</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413835&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1415417</t>
+          <t>1476392</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476392&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1423284</t>
+          <t>1478663</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1429169</t>
+          <t>1486237</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1397,14 +1397,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1429169&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1435726</t>
+          <t>1491285</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1416,33 +1416,33 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435726&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1435900</t>
+          <t>1500484</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435900&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1443868</t>
+          <t>1503780</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,14 +1454,14 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503780&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1456319</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1473,14 +1473,14 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1456324</t>
+          <t>1510467</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1492,33 +1492,33 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1510467&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1478663</t>
+          <t>1512882</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1480366</t>
+          <t>1513141</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1530,14 +1530,14 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1480366&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1491098</t>
+          <t>1514221</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1549,90 +1549,90 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491098&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514221&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1491892</t>
+          <t>1532903</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491892&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1532903&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1496067</t>
+          <t>1539715</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1496067&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1539715&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1500484</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1501319</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1644,128 +1644,128 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1502178</t>
+          <t>524882</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=524882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1508457</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1508460</t>
+          <t>566001</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508460&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=566001&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1509775</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509775&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>1514221</t>
+          <t>612829</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514221&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=612829&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>1524741</t>
+          <t>761949</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1777,14 +1777,14 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1524741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=761949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>1536005</t>
+          <t>767168</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1796,14 +1796,14 @@
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1536005&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=767168&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>777295</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1815,33 +1815,33 @@
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=777295&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>350209</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=350209&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>421238</t>
+          <t>799432</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1853,52 +1853,52 @@
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=421238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=799432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>809110</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=809110&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>494513</t>
+          <t>813202</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=494513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=813202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>512405</t>
+          <t>821096</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1910,14 +1910,14 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=512405&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>519183</t>
+          <t>824517</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -1929,14 +1929,14 @@
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=519183&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>520238</t>
+          <t>824634</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -1948,14 +1948,14 @@
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=520238&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>828426</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -1967,52 +1967,52 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>833738</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=833738&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>618130</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=618130&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>857670</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2024,14 +2024,14 @@
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>643101</t>
+          <t>860988</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -2043,14 +2043,14 @@
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860988&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>686802</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2062,14 +2062,14 @@
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=686802&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>695670</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2081,14 +2081,14 @@
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>701970</t>
+          <t>889211</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2100,33 +2100,33 @@
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=701970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=889211&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>709696</t>
+          <t>915286</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=709696&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>734979</t>
+          <t>937471</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2138,14 +2138,14 @@
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=734979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>758994</t>
+          <t>961058</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2157,33 +2157,33 @@
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=758994&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=961058&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>764045</t>
+          <t>998010</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764045&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=998010&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>999592</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2195,329 +2195,6 @@
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>782815</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=782815&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>787890</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="n">
-        <v>3</v>
-      </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=787890&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>801933</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="n">
-        <v>3</v>
-      </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>804990</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="n">
-        <v>6</v>
-      </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=804990&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>809110</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=809110&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>835857</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="n">
-        <v>2</v>
-      </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=835857&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>835860</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="n">
-        <v>2</v>
-      </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=835860&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>856677</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="n">
-        <v>4</v>
-      </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>866983</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="n">
-        <v>3</v>
-      </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="n">
-        <v>5</v>
-      </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>894796</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="n">
-        <v>2</v>
-      </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=894796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>908949</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="n">
-        <v>2</v>
-      </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=908949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>937471</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="n">
-        <v>3</v>
-      </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>972488</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="n">
-        <v>3</v>
-      </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=972488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>972490</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="n">
-        <v>2</v>
-      </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=972490&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>999592</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="n">
-        <v>2</v>
-      </c>
-      <c r="F109" t="inlineStr"/>
-      <c r="G109" t="inlineStr">
-        <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-10-06T01:22:44Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1033142</t>
+          <t>1003851</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,14 +485,14 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033142&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1003851&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1076105</t>
+          <t>100458</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -504,14 +504,14 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1076105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=100458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1093803</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,14 +523,14 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1149454</t>
+          <t>1026153</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -542,14 +542,14 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1149454&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1026153&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1158522</t>
+          <t>1039106</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -561,14 +561,14 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1158522&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1160257</t>
+          <t>1045365</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1160257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1045365&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1180998</t>
+          <t>1047587</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,33 +599,33 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047587&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1073876</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -637,14 +637,14 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1073876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1244126</t>
+          <t>1078657</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -656,14 +656,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1078657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1244887</t>
+          <t>1093803</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1109493</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,33 +694,33 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1109493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1111064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1111064&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1276718</t>
+          <t>1112053</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -732,14 +732,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1112053&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1276721</t>
+          <t>1143046</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,14 +751,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276721&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1143046&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1279706</t>
+          <t>1154598</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1279706&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1286365</t>
+          <t>1193161</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1286365&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1193161&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1296744</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296744&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1307482</t>
+          <t>1212257</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,109 +827,109 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307482&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1212257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1311546</t>
+          <t>1228762</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1228762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1320773</t>
+          <t>1229228</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320773&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1320832</t>
+          <t>1232243</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1320832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232243&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1329488</t>
+          <t>1244887</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1329488&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1332189</t>
+          <t>1245064</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245064&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1345551</t>
+          <t>1245328</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -941,33 +941,33 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345551&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245328&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1347156</t>
+          <t>1261865</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -979,14 +979,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1261865&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1347160</t>
+          <t>1264565</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -998,14 +998,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347160&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264565&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1278598</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1017,33 +1017,33 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1296733</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1307229</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,52 +1055,52 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1364165</t>
+          <t>1332189</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364165&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1372919</t>
+          <t>1338923</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372919&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1338923&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1112,33 +1112,33 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1373167</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1373167&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1375261</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,52 +1150,52 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1375261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1395308</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1400456</t>
+          <t>1363107</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1400456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1401261</t>
+          <t>1364165</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1207,52 +1207,52 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364165&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1404799</t>
+          <t>1365394</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404799&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1415417</t>
+          <t>1379125</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1379125&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1419090</t>
+          <t>1387361</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1264,14 +1264,14 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1419090&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1441033</t>
+          <t>1390300</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1283,14 +1283,14 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1441033&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1390300&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1446472</t>
+          <t>1404418</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,52 +1302,52 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446472&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404418&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1456324</t>
+          <t>1410600</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410600&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1475693</t>
+          <t>1411805</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1476392</t>
+          <t>1413835</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1359,33 +1359,33 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1476392&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413835&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1478663</t>
+          <t>1415417</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478663&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1486237</t>
+          <t>1423619</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1397,14 +1397,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486237&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1491285</t>
+          <t>1430471</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1416,33 +1416,33 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1500484</t>
+          <t>1435766</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1503780</t>
+          <t>1438808</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,14 +1454,14 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1503780&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438808&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1508457</t>
+          <t>1446494</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1473,14 +1473,14 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446494&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1510467</t>
+          <t>1461369</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1492,33 +1492,33 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1510467&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1461369&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1512882</t>
+          <t>1478705</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478705&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1513141</t>
+          <t>1491285</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1530,128 +1530,128 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1513141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1514221</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1514221&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>1499071</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499071&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1532903</t>
+          <t>1500484</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1532903&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1539715</t>
+          <t>1501314</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1539715&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1502932</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1509363</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509363&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>524882</t>
+          <t>1512197</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1663,33 +1663,33 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=524882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1512882</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>566001</t>
+          <t>1519811</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1701,71 +1701,71 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=566001&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1519811&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>612829</t>
+          <t>1535929</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=612829&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535929&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1535932</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>761949</t>
+          <t>223922</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1777,14 +1777,14 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=761949&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=223922&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>767168</t>
+          <t>290733</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1796,52 +1796,52 @@
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=767168&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=290733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>777295</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=777295&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>470915</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=470915&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>799432</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1853,14 +1853,14 @@
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=799432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>809110</t>
+          <t>571200</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -1872,33 +1872,33 @@
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=809110&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=571200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>813202</t>
+          <t>601537</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=813202&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=601537&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>821096</t>
+          <t>607975</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -1910,147 +1910,147 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>824517</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>824634</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>828426</t>
+          <t>643101</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>833738</t>
+          <t>686023</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=833738&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=686023&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>857670</t>
+          <t>768387</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857670&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=768387&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>860988</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860988&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>866983</t>
+          <t>821096</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2062,14 +2062,14 @@
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>824679</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2081,33 +2081,33 @@
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824679&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>889211</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=889211&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>915286</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -2119,14 +2119,14 @@
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>937471</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2138,33 +2138,33 @@
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>961058</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=961058&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>998010</t>
+          <t>881907</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2176,14 +2176,14 @@
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=998010&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>893548</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2195,7 +2195,121 @@
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=893548&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>900265</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>2</v>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=900265&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>903830</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903830&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>983233</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>3</v>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=983233&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>986868</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=986868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>991741</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>992941</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>2</v>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=992941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-10-13T01:24:30Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1003851</t>
+          <t>1055749</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,33 +485,33 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1003851&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1055749&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>100458</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=100458&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1094785</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,33 +523,33 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1094785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1026153</t>
+          <t>1102757</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1026153&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1102757&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1039106</t>
+          <t>1119514</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -561,14 +561,14 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1039106&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1119514&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1045365</t>
+          <t>1142699</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1045365&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1142699&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1047587</t>
+          <t>1147927</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,52 +599,52 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1047587&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1147927&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1073876</t>
+          <t>1174183</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1073876&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1174183&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1078657</t>
+          <t>1211832</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -656,14 +656,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1078657&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1093803</t>
+          <t>1217729</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1217729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1109493</t>
+          <t>1227314</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,33 +694,33 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1109493&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1227314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1111064</t>
+          <t>1231889</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1111064&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1231889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1112053</t>
+          <t>1232284</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -732,14 +732,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1112053&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1143046</t>
+          <t>1244887</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,14 +751,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1143046&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1154598</t>
+          <t>1246450</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1193161</t>
+          <t>1246966</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1193161&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1246973</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1212257</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,14 +827,14 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1212257&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1228762</t>
+          <t>1271268</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -846,52 +846,52 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1228762&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1229228</t>
+          <t>1277156</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1232243</t>
+          <t>1292881</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232243&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1292881&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1244887</t>
+          <t>1307229</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -903,14 +903,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1245064</t>
+          <t>1326181</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -922,14 +922,14 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245064&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326181&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1245328</t>
+          <t>1345526</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -941,33 +941,33 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1245328&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1261865</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -979,14 +979,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1261865&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1264565</t>
+          <t>1401261</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -998,14 +998,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1264565&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1278598</t>
+          <t>1416383</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1017,14 +1017,14 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416383&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1296733</t>
+          <t>1418624</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1036,14 +1036,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418624&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1307229</t>
+          <t>1423774</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,33 +1055,33 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1332189</t>
+          <t>1424281</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1424281&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1338923</t>
+          <t>1431678</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1093,14 +1093,14 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1338923&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1344943</t>
+          <t>1443868</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1112,33 +1112,33 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1450889</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1451423</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,52 +1150,52 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1451423&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1456319</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1363107</t>
+          <t>1463308</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1363107&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1364165</t>
+          <t>1478705</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1207,52 +1207,52 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1364165&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478705&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1365394</t>
+          <t>148725</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365394&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=148725&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1379125</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1379125&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1387361</t>
+          <t>1497029</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1264,33 +1264,33 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1387361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497029&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1390300</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1390300&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1404418</t>
+          <t>1512197</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,14 +1302,14 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404418&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1410600</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1321,33 +1321,33 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1410600&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1411805</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1413835</t>
+          <t>265118</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1359,71 +1359,71 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413835&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=265118&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1415417</t>
+          <t>298443</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1423619</t>
+          <t>412675</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1430471</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1430471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1435766</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1435,14 +1435,14 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1435766&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1438808</t>
+          <t>561534</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,14 +1454,14 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438808&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=561534&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1446494</t>
+          <t>571200</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1473,14 +1473,14 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446494&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=571200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1461369</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1492,71 +1492,71 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1461369&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1478705</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478705&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1491285</t>
+          <t>801933</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491285&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>815322</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=815322&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1499071</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1568,14 +1568,14 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499071&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1500484</t>
+          <t>857942</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1587,14 +1587,14 @@
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500484&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1501314</t>
+          <t>866983</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1606,14 +1606,14 @@
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1501314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1502932</t>
+          <t>872049</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1625,71 +1625,71 @@
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872049&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1509363</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1509363&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1512197</t>
+          <t>880642</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1512882</t>
+          <t>920040</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512882&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1519811</t>
+          <t>941353</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1701,615 +1701,45 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1519811&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=941353&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>970842</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=970842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>1535929</t>
+          <t>989754</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535929&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>1535932</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>223922</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="n">
-        <v>2</v>
-      </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=223922&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>290733</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="n">
-        <v>2</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=290733&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>469358</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="n">
-        <v>6</v>
-      </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>470915</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="n">
-        <v>2</v>
-      </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=470915&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>545355</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="n">
-        <v>2</v>
-      </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>571200</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="n">
-        <v>2</v>
-      </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=571200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>601537</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="n">
-        <v>2</v>
-      </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=601537&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>607975</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="n">
-        <v>2</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=607975&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>610619</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="n">
-        <v>3</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>621809</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="n">
-        <v>7</v>
-      </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>643101</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="n">
-        <v>3</v>
-      </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=643101&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>686023</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="n">
-        <v>2</v>
-      </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=686023&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>764151</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="n">
-        <v>2</v>
-      </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>768387</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="n">
-        <v>3</v>
-      </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=768387&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>786481</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>821096</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="n">
-        <v>2</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=821096&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>824679</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="n">
-        <v>2</v>
-      </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824679&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>856677</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="n">
-        <v>6</v>
-      </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>857942</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="n">
-        <v>3</v>
-      </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>866983</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>876141</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
-        <v>4</v>
-      </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>881907</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="n">
-        <v>2</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=881907&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>893548</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="n">
-        <v>2</v>
-      </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=893548&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>900265</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=900265&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>903830</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=903830&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>983233</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="n">
-        <v>3</v>
-      </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=983233&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>986868</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="n">
-        <v>2</v>
-      </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=986868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>991741</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="n">
-        <v>2</v>
-      </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=991741&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>992941</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=992941&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=989754&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-10-20T01:28:18Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1055749</t>
+          <t>1019804</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,33 +485,33 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1055749&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1051541</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1051541&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1094785</t>
+          <t>1066700</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,33 +523,33 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1094785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066700&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1102757</t>
+          <t>1093803</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1102757&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1119514</t>
+          <t>1130219</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -561,14 +561,14 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1119514&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130219&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1142699</t>
+          <t>1130272</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1142699&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1147927</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,14 +599,14 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1147927&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1179336</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -618,33 +618,33 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1174183</t>
+          <t>1179976</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1174183&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1211832</t>
+          <t>1229228</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -656,14 +656,14 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1217729</t>
+          <t>1232243</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1217729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232243&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1227314</t>
+          <t>1244126</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,33 +694,33 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1227314&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1231889</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1231889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1232284</t>
+          <t>1259361</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -732,14 +732,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232284&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1259361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1244887</t>
+          <t>1275466</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,14 +751,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1275466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1246450</t>
+          <t>1276718</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246450&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1246966</t>
+          <t>1278598</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246966&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1246973</t>
+          <t>1290822</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1246973&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1305084</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,52 +827,52 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1271268</t>
+          <t>1309827</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1271268&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1277156</t>
+          <t>1311546</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1277156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1292881</t>
+          <t>1312519</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -884,14 +884,14 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1292881&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1312519&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1307229</t>
+          <t>1318034</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -903,14 +903,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1307229&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1318034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1326181</t>
+          <t>1322572</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -922,14 +922,14 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1326181&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1322572&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1345526</t>
+          <t>1332189</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -941,7 +941,7 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -955,7 +955,7 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
@@ -967,7 +967,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1347117</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -979,14 +979,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1401261</t>
+          <t>1350143</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -998,14 +998,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1401261&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1416383</t>
+          <t>1351207</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1017,14 +1017,14 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1416383&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1418624</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1036,14 +1036,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1418624&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1423774</t>
+          <t>1365729</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,14 +1055,14 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1423774&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1424281</t>
+          <t>1372943</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1074,52 +1074,52 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1424281&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>1377000</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1377000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1443868</t>
+          <t>1389021</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443868&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1450889</t>
+          <t>1395590</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1131,14 +1131,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450889&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395590&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1451423</t>
+          <t>1404418</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,14 +1150,14 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1451423&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404418&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1456319</t>
+          <t>1411805</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1169,14 +1169,14 @@
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456319&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1463308</t>
+          <t>1413323</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1188,14 +1188,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463308&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413323&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1478705</t>
+          <t>1414478</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1207,14 +1207,14 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1478705&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1414478&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>148725</t>
+          <t>1415417</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1226,71 +1226,71 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=148725&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1431678</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1497029</t>
+          <t>1438808</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497029&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438808&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1508457</t>
+          <t>1439485</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1439485&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1512197</t>
+          <t>1443796</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,14 +1302,14 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>1450704</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1321,14 +1321,14 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>260606</t>
+          <t>1475693</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1340,14 +1340,14 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>265118</t>
+          <t>1486879</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1359,71 +1359,71 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=265118&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486879&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>298443</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=298443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>412675</t>
+          <t>1497029</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=412675&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497029&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1498127</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498127&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1502622</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1435,14 +1435,14 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502622&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>561534</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,33 +1454,33 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=561534&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>571200</t>
+          <t>1512197</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=571200&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1520134</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1492,14 +1492,14 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1520134&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>1523616</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1511,33 +1511,33 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>801933</t>
+          <t>1526964</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=801933&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1526964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>815322</t>
+          <t>284031</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1549,14 +1549,14 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=815322&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=284031&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>380275</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1568,52 +1568,52 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>857942</t>
+          <t>469358</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=857942&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>866983</t>
+          <t>521155</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=866983&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=521155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>872049</t>
+          <t>545355</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1625,14 +1625,14 @@
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=872049&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>610619</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1644,33 +1644,33 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>880642</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>920040</t>
+          <t>695287</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1682,14 +1682,14 @@
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=920040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695287&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>941353</t>
+          <t>720141</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1701,14 +1701,14 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=941353&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=720141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>970842</t>
+          <t>734979</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1720,14 +1720,14 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=970842&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=734979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>989754</t>
+          <t>738289</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1739,7 +1739,406 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=989754&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>752970</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>2</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=752970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>764151</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>786481</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>4</v>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>822583</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>2</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=822583&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>824517</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>2</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>824634</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>828426</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>3</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>856677</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>5</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>860988</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860988&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>874156</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>2</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=874156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>876141</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>3</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>879692</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>2</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>880642</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>2</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>882843</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>2</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882843&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>895147</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>2</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=895147&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>910678</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>2</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=910678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>915286</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>937471</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="n">
+        <v>3</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=937471&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>968713</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>982044</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>2</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>3</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-10-27T01:30:38Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1019804</t>
+          <t>1033155</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,14 +485,14 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1019804&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1051541</t>
+          <t>1033513</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -504,14 +504,14 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1051541&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1066700</t>
+          <t>1042980</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,14 +523,14 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1066700&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1042980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1093803</t>
+          <t>1062124</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -542,33 +542,33 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1093803&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1130219</t>
+          <t>1062346</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130219&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1130272</t>
+          <t>1080170</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1130272&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1080170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1091007</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,33 +599,33 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1091007&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1179336</t>
+          <t>1154598</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179336&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1179976</t>
+          <t>1155959</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -637,33 +637,33 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1179976&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1155959&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1229228</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1229228&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1232243</t>
+          <t>1170247</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232243&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1170247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1244126</t>
+          <t>1172159</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,33 +694,33 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1244126&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172159&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1249874</t>
+          <t>1174958</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1174958&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1259361</t>
+          <t>1202855</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -732,14 +732,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1259361&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1275466</t>
+          <t>1205131</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,14 +751,14 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1275466&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1276718</t>
+          <t>1209526</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -770,14 +770,14 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1276718&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1278598</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1290822</t>
+          <t>1218784</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1218784&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1305084</t>
+          <t>1227443</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -827,14 +827,14 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1305084&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1227443&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1309827</t>
+          <t>1232432</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -846,33 +846,33 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1309827&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1311546</t>
+          <t>1232434</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1311546&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1232434&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1312519</t>
+          <t>1238399</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -884,14 +884,14 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1312519&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1238399&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1318034</t>
+          <t>1249874</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -903,14 +903,14 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1318034&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1249874&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1322572</t>
+          <t>1278851</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -922,33 +922,33 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1322572&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1278851&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1332189</t>
+          <t>1290822</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1332189&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1290822&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1345877</t>
+          <t>1296344</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -960,14 +960,14 @@
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1296344&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1347117</t>
+          <t>1310141</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -979,14 +979,14 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347117&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1310141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1350143</t>
+          <t>1324828</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -998,14 +998,14 @@
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1350143&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1324828&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1351207</t>
+          <t>1344943</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1017,14 +1017,14 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1351207&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1344943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1353406</t>
+          <t>1345877</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1036,14 +1036,14 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1345877&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1365729</t>
+          <t>1346146</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1055,14 +1055,14 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1365729&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1346146&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1372943</t>
+          <t>1347156</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1074,14 +1074,14 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1372943&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1347156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1377000</t>
+          <t>1349260</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1093,33 +1093,33 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1377000&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1349260&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1389021</t>
+          <t>1353406</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1389021&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1353406&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1395590</t>
+          <t>1378083</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1131,14 +1131,14 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1395590&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1378083&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1404418</t>
+          <t>1383055</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1150,33 +1150,33 @@
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1404418&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1383055&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1411805</t>
+          <t>1386556</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1411805&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1386556&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1413323</t>
+          <t>1394516</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1188,14 +1188,14 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413323&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1394516&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1414478</t>
+          <t>1397555</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1207,90 +1207,90 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1414478&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1397555&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1415417</t>
+          <t>1413835</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1415417&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1413835&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1431678</t>
+          <t>1421130</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1421130&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1438808</t>
+          <t>1428161</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1438808&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1428161&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1439485</t>
+          <t>1431678</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1439485&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1431678&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1443796</t>
+          <t>1434701</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1302,52 +1302,52 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1434701&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1450704</t>
+          <t>1437689</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450704&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1437689&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1475693</t>
+          <t>1443796</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1475693&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1443796&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1486879</t>
+          <t>1446472</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1359,33 +1359,33 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486879&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1446472&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1491886</t>
+          <t>1450197</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1450197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1497029</t>
+          <t>1456324</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1397,14 +1397,14 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1497029&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456324&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1498127</t>
+          <t>1456430</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1416,14 +1416,14 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1498127&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1456430&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1502622</t>
+          <t>1463310</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1435,14 +1435,14 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1502622&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1463310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1508457</t>
+          <t>1486562</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,52 +1454,52 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1486562&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1512197</t>
+          <t>1488236</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1512197&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1488236&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1520134</t>
+          <t>1491886</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1520134&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1491886&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1523616</t>
+          <t>1493887</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1511,14 +1511,14 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1523616&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1493887&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1526964</t>
+          <t>1494582</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1530,14 +1530,14 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1526964&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1494582&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>284031</t>
+          <t>1499129</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1549,90 +1549,90 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=284031&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1499129&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>380275</t>
+          <t>1500483</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=380275&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1500483&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>469358</t>
+          <t>1508457</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=469358&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1508457&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>521155</t>
+          <t>1519832</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=521155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1519832&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>545355</t>
+          <t>1524901</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=545355&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1524901&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>610619</t>
+          <t>1528845</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1644,14 +1644,14 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=610619&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1528845&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>621809</t>
+          <t>1533178</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1663,14 +1663,14 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1533178&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>695287</t>
+          <t>1535923</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1682,14 +1682,14 @@
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=695287&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535923&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>720141</t>
+          <t>1535932</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1701,14 +1701,14 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=720141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1535932&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>734979</t>
+          <t>260606</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1720,14 +1720,14 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=734979&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=260606&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>738289</t>
+          <t>384376</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1739,14 +1739,14 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=738289&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=384376&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>752970</t>
+          <t>566833</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -1758,52 +1758,52 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=752970&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=566833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>764151</t>
+          <t>606456</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=606456&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>786481</t>
+          <t>621809</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=621809&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>822583</t>
+          <t>631040</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1815,14 +1815,14 @@
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=822583&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=631040&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>824517</t>
+          <t>710563</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -1834,14 +1834,14 @@
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824517&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=710563&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>824634</t>
+          <t>744769</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -1853,14 +1853,14 @@
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=824634&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=744769&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>828426</t>
+          <t>764151</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -1872,52 +1872,52 @@
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=828426&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=764151&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>856677</t>
+          <t>786481</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=786481&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>860988</t>
+          <t>799432</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=860988&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=799432&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>874156</t>
+          <t>846092</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -1929,71 +1929,71 @@
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=874156&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=846092&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>876141</t>
+          <t>846759</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=846759&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>879692</t>
+          <t>856677</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=879692&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=856677&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>880642</t>
+          <t>876141</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=876141&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>882843</t>
+          <t>880642</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -2005,14 +2005,14 @@
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=882843&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=880642&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>895147</t>
+          <t>891274</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2024,7 +2024,7 @@
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=895147&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=891274&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>915286</t>
+          <t>935525</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2062,7 +2062,7 @@
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=915286&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=935525&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2088,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>968713</t>
+          <t>942338</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2100,43 +2100,62 @@
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=968713&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=942338&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>982044</t>
+          <t>960159</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=982044&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=960159&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>999592</t>
+          <t>983233</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
+        <is>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=983233&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>999592</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>2</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
         <is>
           <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=999592&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>

</xml_diff>

<commit_message>
Update Feefo and Review reports for 2025-11-03T01:30:59Z
</commit_message>
<xml_diff>
--- a/data/recent_reviews_web_ready.xlsx
+++ b/data/recent_reviews_web_ready.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1033155</t>
+          <t>1008277</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -485,14 +485,14 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033155&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1008277&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1033513</t>
+          <t>1032833</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -504,14 +504,14 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1033513&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1032833&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1042980</t>
+          <t>1055749</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -523,14 +523,14 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1042980&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1055749&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1062124</t>
+          <t>1056043</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -542,33 +542,33 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062124&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1056043&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1062346</t>
+          <t>1072216</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1062346&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1072216&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1080170</t>
+          <t>1090474</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -580,14 +580,14 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1080170&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1090474&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1091007</t>
+          <t>1094785</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -599,33 +599,33 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1091007&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1094785&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1154598</t>
+          <t>1150628</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1154598&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1150628&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1155959</t>
+          <t>1162105</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -637,33 +637,33 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1155959&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1162105</t>
+          <t>1172375</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1162105&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172375&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1170247</t>
+          <t>1180998</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -675,14 +675,14 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1170247&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1180998&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1172159</t>
+          <t>1183789</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -694,14 +694,14 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1172159&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1183789&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1174958</t>
+          <t>1193161</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -713,14 +713,14 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1174958&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1193161&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1202855</t>
+          <t>1205131</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -732,14 +732,14 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1202855&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1205131</t>
+          <t>1211012</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -751,33 +751,33 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1205131&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211012&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1209526</t>
+          <t>1211310</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1209526&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1211310</t>
+          <t>1217428</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -789,14 +789,14 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1211310&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
+          <t>https://www.feefo.com/en-US/reviews/notonthehighstreet-com/products/*?sku=1217428&amp;displayFeedbackType=PRODUCT&amp;timeFrame=ALL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1218784</t>
+          <t>1231071</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -808,14 +808,14 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-